<commit_message>
Added the new version of the activity locations template.
</commit_message>
<xml_diff>
--- a/ccafspr_ip/src/main/webapp/resources/locationTemplate/Activity_Location_Template.xlsx
+++ b/ccafspr_ip/src/main/webapp/resources/locationTemplate/Activity_Location_Template.xlsx
@@ -2212,17 +2212,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">4 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please be aware that if you selected CCAFS-Site or Climate Smart Village, and coordinates are 0.0, it's because they are not defined, we still updating this information.</t>
+      <t>NOTE: Please be aware that if you select a CCAFS-Site or a Climate Smart Village, and the coordinates are displayed (0.0), do not worry, we are going to update this information as soon as possible.</t>
     </r>
   </si>
 </sst>
@@ -2971,7 +2961,7 @@
   <dimension ref="A1:AV600"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="AY16" sqref="AY16"/>
+      <selection activeCell="B10" sqref="B10:AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38831,27 +38821,2308 @@
     </row>
   </sheetData>
   <mergeCells count="2355">
-    <mergeCell ref="AE596:AJ596"/>
-    <mergeCell ref="AK596:AP596"/>
-    <mergeCell ref="AE597:AJ597"/>
-    <mergeCell ref="AK597:AP597"/>
-    <mergeCell ref="AE598:AJ598"/>
-    <mergeCell ref="AK598:AP598"/>
-    <mergeCell ref="AE599:AJ599"/>
-    <mergeCell ref="AK599:AP599"/>
-    <mergeCell ref="AE600:AJ600"/>
-    <mergeCell ref="AK600:AP600"/>
-    <mergeCell ref="AK589:AP589"/>
-    <mergeCell ref="AE590:AJ590"/>
-    <mergeCell ref="AK590:AP590"/>
-    <mergeCell ref="AE591:AJ591"/>
-    <mergeCell ref="AK591:AP591"/>
-    <mergeCell ref="AE592:AJ592"/>
-    <mergeCell ref="AK592:AP592"/>
-    <mergeCell ref="AE593:AJ593"/>
-    <mergeCell ref="AK593:AP593"/>
-    <mergeCell ref="AE594:AJ594"/>
-    <mergeCell ref="AK594:AP594"/>
+    <mergeCell ref="N594:AD594"/>
+    <mergeCell ref="N595:AD595"/>
+    <mergeCell ref="A592:M592"/>
+    <mergeCell ref="A593:M593"/>
+    <mergeCell ref="N592:AD592"/>
+    <mergeCell ref="N593:AD593"/>
+    <mergeCell ref="A590:M590"/>
+    <mergeCell ref="A591:M591"/>
+    <mergeCell ref="N590:AD590"/>
+    <mergeCell ref="N591:AD591"/>
+    <mergeCell ref="N600:AD600"/>
+    <mergeCell ref="A600:M600"/>
+    <mergeCell ref="N14:AD14"/>
+    <mergeCell ref="N15:AD15"/>
+    <mergeCell ref="N16:AD16"/>
+    <mergeCell ref="N17:AD17"/>
+    <mergeCell ref="N18:AD18"/>
+    <mergeCell ref="N19:AD19"/>
+    <mergeCell ref="A598:M598"/>
+    <mergeCell ref="A599:M599"/>
+    <mergeCell ref="N598:AD598"/>
+    <mergeCell ref="N599:AD599"/>
+    <mergeCell ref="A596:M596"/>
+    <mergeCell ref="A597:M597"/>
+    <mergeCell ref="N596:AD596"/>
+    <mergeCell ref="N597:AD597"/>
+    <mergeCell ref="A594:M594"/>
+    <mergeCell ref="A595:M595"/>
+    <mergeCell ref="A576:M576"/>
+    <mergeCell ref="A577:M577"/>
+    <mergeCell ref="N576:AD576"/>
+    <mergeCell ref="N577:AD577"/>
+    <mergeCell ref="A588:M588"/>
+    <mergeCell ref="A589:M589"/>
+    <mergeCell ref="N588:AD588"/>
+    <mergeCell ref="N589:AD589"/>
+    <mergeCell ref="A586:M586"/>
+    <mergeCell ref="A587:M587"/>
+    <mergeCell ref="N586:AD586"/>
+    <mergeCell ref="N587:AD587"/>
+    <mergeCell ref="A584:M584"/>
+    <mergeCell ref="A585:M585"/>
+    <mergeCell ref="N584:AD584"/>
+    <mergeCell ref="N585:AD585"/>
+    <mergeCell ref="AE587:AJ587"/>
+    <mergeCell ref="AK587:AP587"/>
+    <mergeCell ref="AE588:AJ588"/>
+    <mergeCell ref="AK588:AP588"/>
+    <mergeCell ref="AE589:AJ589"/>
+    <mergeCell ref="A574:M574"/>
+    <mergeCell ref="A575:M575"/>
+    <mergeCell ref="N574:AD574"/>
+    <mergeCell ref="N575:AD575"/>
+    <mergeCell ref="A572:M572"/>
+    <mergeCell ref="A573:M573"/>
+    <mergeCell ref="N572:AD572"/>
+    <mergeCell ref="N573:AD573"/>
+    <mergeCell ref="A582:M582"/>
+    <mergeCell ref="A583:M583"/>
+    <mergeCell ref="N582:AD582"/>
+    <mergeCell ref="N583:AD583"/>
+    <mergeCell ref="A580:M580"/>
+    <mergeCell ref="A581:M581"/>
+    <mergeCell ref="N580:AD580"/>
+    <mergeCell ref="N581:AD581"/>
+    <mergeCell ref="A578:M578"/>
+    <mergeCell ref="A579:M579"/>
+    <mergeCell ref="N578:AD578"/>
+    <mergeCell ref="N579:AD579"/>
+    <mergeCell ref="A570:M570"/>
+    <mergeCell ref="A571:M571"/>
+    <mergeCell ref="N570:AD570"/>
+    <mergeCell ref="N571:AD571"/>
+    <mergeCell ref="A568:M568"/>
+    <mergeCell ref="A569:M569"/>
+    <mergeCell ref="N568:AD568"/>
+    <mergeCell ref="N569:AD569"/>
+    <mergeCell ref="A566:M566"/>
+    <mergeCell ref="A567:M567"/>
+    <mergeCell ref="N566:AD566"/>
+    <mergeCell ref="N567:AD567"/>
+    <mergeCell ref="AE569:AJ569"/>
+    <mergeCell ref="AK569:AP569"/>
+    <mergeCell ref="AE570:AJ570"/>
+    <mergeCell ref="AK570:AP570"/>
+    <mergeCell ref="AE571:AJ571"/>
+    <mergeCell ref="AE566:AJ566"/>
+    <mergeCell ref="AK566:AP566"/>
+    <mergeCell ref="AE567:AJ567"/>
+    <mergeCell ref="AK567:AP567"/>
+    <mergeCell ref="AE568:AJ568"/>
+    <mergeCell ref="AK568:AP568"/>
+    <mergeCell ref="AK571:AP571"/>
+    <mergeCell ref="A564:M564"/>
+    <mergeCell ref="A565:M565"/>
+    <mergeCell ref="N564:AD564"/>
+    <mergeCell ref="N565:AD565"/>
+    <mergeCell ref="A562:M562"/>
+    <mergeCell ref="A563:M563"/>
+    <mergeCell ref="N562:AD562"/>
+    <mergeCell ref="N563:AD563"/>
+    <mergeCell ref="A560:M560"/>
+    <mergeCell ref="A561:M561"/>
+    <mergeCell ref="N560:AD560"/>
+    <mergeCell ref="N561:AD561"/>
+    <mergeCell ref="AE560:AJ560"/>
+    <mergeCell ref="AK560:AP560"/>
+    <mergeCell ref="AE561:AJ561"/>
+    <mergeCell ref="AK561:AP561"/>
+    <mergeCell ref="AE562:AJ562"/>
+    <mergeCell ref="AE565:AJ565"/>
+    <mergeCell ref="AK565:AP565"/>
+    <mergeCell ref="AE547:AJ547"/>
+    <mergeCell ref="AK547:AP547"/>
+    <mergeCell ref="AE548:AJ548"/>
+    <mergeCell ref="AK548:AP548"/>
+    <mergeCell ref="AE549:AJ549"/>
+    <mergeCell ref="AK549:AP549"/>
+    <mergeCell ref="AE550:AJ550"/>
+    <mergeCell ref="AK550:AP550"/>
+    <mergeCell ref="AK553:AP553"/>
+    <mergeCell ref="A558:M558"/>
+    <mergeCell ref="A559:M559"/>
+    <mergeCell ref="N558:AD558"/>
+    <mergeCell ref="N559:AD559"/>
+    <mergeCell ref="A556:M556"/>
+    <mergeCell ref="A557:M557"/>
+    <mergeCell ref="N556:AD556"/>
+    <mergeCell ref="N557:AD557"/>
+    <mergeCell ref="A554:M554"/>
+    <mergeCell ref="A555:M555"/>
+    <mergeCell ref="N554:AD554"/>
+    <mergeCell ref="N555:AD555"/>
+    <mergeCell ref="A552:M552"/>
+    <mergeCell ref="A553:M553"/>
+    <mergeCell ref="N552:AD552"/>
+    <mergeCell ref="N553:AD553"/>
+    <mergeCell ref="A550:M550"/>
+    <mergeCell ref="A551:M551"/>
+    <mergeCell ref="N550:AD550"/>
+    <mergeCell ref="N551:AD551"/>
+    <mergeCell ref="A548:M548"/>
+    <mergeCell ref="A549:M549"/>
+    <mergeCell ref="N548:AD548"/>
+    <mergeCell ref="N549:AD549"/>
+    <mergeCell ref="AE551:AJ551"/>
+    <mergeCell ref="AK551:AP551"/>
+    <mergeCell ref="AE552:AJ552"/>
+    <mergeCell ref="AK552:AP552"/>
+    <mergeCell ref="AE553:AJ553"/>
+    <mergeCell ref="A540:M540"/>
+    <mergeCell ref="A541:M541"/>
+    <mergeCell ref="N540:AD540"/>
+    <mergeCell ref="N541:AD541"/>
+    <mergeCell ref="A538:M538"/>
+    <mergeCell ref="A539:M539"/>
+    <mergeCell ref="N538:AD538"/>
+    <mergeCell ref="N539:AD539"/>
+    <mergeCell ref="A536:M536"/>
+    <mergeCell ref="A537:M537"/>
+    <mergeCell ref="N536:AD536"/>
+    <mergeCell ref="N537:AD537"/>
+    <mergeCell ref="A546:M546"/>
+    <mergeCell ref="A547:M547"/>
+    <mergeCell ref="N546:AD546"/>
+    <mergeCell ref="N547:AD547"/>
+    <mergeCell ref="A544:M544"/>
+    <mergeCell ref="A545:M545"/>
+    <mergeCell ref="N544:AD544"/>
+    <mergeCell ref="N545:AD545"/>
+    <mergeCell ref="A542:M542"/>
+    <mergeCell ref="A543:M543"/>
+    <mergeCell ref="N542:AD542"/>
+    <mergeCell ref="N543:AD543"/>
+    <mergeCell ref="AE536:AJ536"/>
+    <mergeCell ref="AK536:AP536"/>
+    <mergeCell ref="A534:M534"/>
+    <mergeCell ref="A535:M535"/>
+    <mergeCell ref="N534:AD534"/>
+    <mergeCell ref="N535:AD535"/>
+    <mergeCell ref="A532:M532"/>
+    <mergeCell ref="A533:M533"/>
+    <mergeCell ref="N532:AD532"/>
+    <mergeCell ref="N533:AD533"/>
+    <mergeCell ref="A530:M530"/>
+    <mergeCell ref="A531:M531"/>
+    <mergeCell ref="N530:AD530"/>
+    <mergeCell ref="N531:AD531"/>
+    <mergeCell ref="AE533:AJ533"/>
+    <mergeCell ref="AK533:AP533"/>
+    <mergeCell ref="AE534:AJ534"/>
+    <mergeCell ref="AK534:AP534"/>
+    <mergeCell ref="AE535:AJ535"/>
+    <mergeCell ref="AE530:AJ530"/>
+    <mergeCell ref="AK530:AP530"/>
+    <mergeCell ref="AE531:AJ531"/>
+    <mergeCell ref="AK531:AP531"/>
+    <mergeCell ref="AE532:AJ532"/>
+    <mergeCell ref="AK532:AP532"/>
+    <mergeCell ref="AK535:AP535"/>
+    <mergeCell ref="A528:M528"/>
+    <mergeCell ref="A529:M529"/>
+    <mergeCell ref="N528:AD528"/>
+    <mergeCell ref="N529:AD529"/>
+    <mergeCell ref="A526:M526"/>
+    <mergeCell ref="A527:M527"/>
+    <mergeCell ref="N526:AD526"/>
+    <mergeCell ref="N527:AD527"/>
+    <mergeCell ref="A524:M524"/>
+    <mergeCell ref="A525:M525"/>
+    <mergeCell ref="N524:AD524"/>
+    <mergeCell ref="N525:AD525"/>
+    <mergeCell ref="AE524:AJ524"/>
+    <mergeCell ref="AK524:AP524"/>
+    <mergeCell ref="AE525:AJ525"/>
+    <mergeCell ref="AK525:AP525"/>
+    <mergeCell ref="AE526:AJ526"/>
+    <mergeCell ref="AE529:AJ529"/>
+    <mergeCell ref="AK529:AP529"/>
+    <mergeCell ref="AE511:AJ511"/>
+    <mergeCell ref="AK511:AP511"/>
+    <mergeCell ref="AE512:AJ512"/>
+    <mergeCell ref="AK512:AP512"/>
+    <mergeCell ref="AE513:AJ513"/>
+    <mergeCell ref="AK513:AP513"/>
+    <mergeCell ref="AE514:AJ514"/>
+    <mergeCell ref="AK514:AP514"/>
+    <mergeCell ref="AK517:AP517"/>
+    <mergeCell ref="A522:M522"/>
+    <mergeCell ref="A523:M523"/>
+    <mergeCell ref="N522:AD522"/>
+    <mergeCell ref="N523:AD523"/>
+    <mergeCell ref="A520:M520"/>
+    <mergeCell ref="A521:M521"/>
+    <mergeCell ref="N520:AD520"/>
+    <mergeCell ref="N521:AD521"/>
+    <mergeCell ref="A518:M518"/>
+    <mergeCell ref="A519:M519"/>
+    <mergeCell ref="N518:AD518"/>
+    <mergeCell ref="N519:AD519"/>
+    <mergeCell ref="A516:M516"/>
+    <mergeCell ref="A517:M517"/>
+    <mergeCell ref="N516:AD516"/>
+    <mergeCell ref="N517:AD517"/>
+    <mergeCell ref="A514:M514"/>
+    <mergeCell ref="A515:M515"/>
+    <mergeCell ref="N514:AD514"/>
+    <mergeCell ref="N515:AD515"/>
+    <mergeCell ref="A512:M512"/>
+    <mergeCell ref="A513:M513"/>
+    <mergeCell ref="N512:AD512"/>
+    <mergeCell ref="N513:AD513"/>
+    <mergeCell ref="AE515:AJ515"/>
+    <mergeCell ref="AK515:AP515"/>
+    <mergeCell ref="AE516:AJ516"/>
+    <mergeCell ref="AK516:AP516"/>
+    <mergeCell ref="AE517:AJ517"/>
+    <mergeCell ref="A504:M504"/>
+    <mergeCell ref="A505:M505"/>
+    <mergeCell ref="N504:AD504"/>
+    <mergeCell ref="N505:AD505"/>
+    <mergeCell ref="A502:M502"/>
+    <mergeCell ref="A503:M503"/>
+    <mergeCell ref="N502:AD502"/>
+    <mergeCell ref="N503:AD503"/>
+    <mergeCell ref="A500:M500"/>
+    <mergeCell ref="A501:M501"/>
+    <mergeCell ref="N500:AD500"/>
+    <mergeCell ref="N501:AD501"/>
+    <mergeCell ref="A510:M510"/>
+    <mergeCell ref="A511:M511"/>
+    <mergeCell ref="N510:AD510"/>
+    <mergeCell ref="N511:AD511"/>
+    <mergeCell ref="A508:M508"/>
+    <mergeCell ref="A509:M509"/>
+    <mergeCell ref="N508:AD508"/>
+    <mergeCell ref="N509:AD509"/>
+    <mergeCell ref="A506:M506"/>
+    <mergeCell ref="A507:M507"/>
+    <mergeCell ref="N506:AD506"/>
+    <mergeCell ref="N507:AD507"/>
+    <mergeCell ref="AE500:AJ500"/>
+    <mergeCell ref="AK500:AP500"/>
+    <mergeCell ref="A498:M498"/>
+    <mergeCell ref="A499:M499"/>
+    <mergeCell ref="N498:AD498"/>
+    <mergeCell ref="N499:AD499"/>
+    <mergeCell ref="A496:M496"/>
+    <mergeCell ref="A497:M497"/>
+    <mergeCell ref="N496:AD496"/>
+    <mergeCell ref="N497:AD497"/>
+    <mergeCell ref="A494:M494"/>
+    <mergeCell ref="A495:M495"/>
+    <mergeCell ref="N494:AD494"/>
+    <mergeCell ref="N495:AD495"/>
+    <mergeCell ref="AE497:AJ497"/>
+    <mergeCell ref="AK497:AP497"/>
+    <mergeCell ref="AE498:AJ498"/>
+    <mergeCell ref="AK498:AP498"/>
+    <mergeCell ref="AE499:AJ499"/>
+    <mergeCell ref="AE494:AJ494"/>
+    <mergeCell ref="AK494:AP494"/>
+    <mergeCell ref="AE495:AJ495"/>
+    <mergeCell ref="AK495:AP495"/>
+    <mergeCell ref="AE496:AJ496"/>
+    <mergeCell ref="AK496:AP496"/>
+    <mergeCell ref="AK499:AP499"/>
+    <mergeCell ref="A492:M492"/>
+    <mergeCell ref="A493:M493"/>
+    <mergeCell ref="N492:AD492"/>
+    <mergeCell ref="N493:AD493"/>
+    <mergeCell ref="A490:M490"/>
+    <mergeCell ref="A491:M491"/>
+    <mergeCell ref="N490:AD490"/>
+    <mergeCell ref="N491:AD491"/>
+    <mergeCell ref="A488:M488"/>
+    <mergeCell ref="A489:M489"/>
+    <mergeCell ref="N488:AD488"/>
+    <mergeCell ref="N489:AD489"/>
+    <mergeCell ref="AE488:AJ488"/>
+    <mergeCell ref="AK488:AP488"/>
+    <mergeCell ref="AE489:AJ489"/>
+    <mergeCell ref="AK489:AP489"/>
+    <mergeCell ref="AE490:AJ490"/>
+    <mergeCell ref="AE493:AJ493"/>
+    <mergeCell ref="AK493:AP493"/>
+    <mergeCell ref="AE475:AJ475"/>
+    <mergeCell ref="AK475:AP475"/>
+    <mergeCell ref="AE476:AJ476"/>
+    <mergeCell ref="AK476:AP476"/>
+    <mergeCell ref="AE477:AJ477"/>
+    <mergeCell ref="AK477:AP477"/>
+    <mergeCell ref="AE478:AJ478"/>
+    <mergeCell ref="AK478:AP478"/>
+    <mergeCell ref="AK481:AP481"/>
+    <mergeCell ref="A486:M486"/>
+    <mergeCell ref="A487:M487"/>
+    <mergeCell ref="N486:AD486"/>
+    <mergeCell ref="N487:AD487"/>
+    <mergeCell ref="A484:M484"/>
+    <mergeCell ref="A485:M485"/>
+    <mergeCell ref="N484:AD484"/>
+    <mergeCell ref="N485:AD485"/>
+    <mergeCell ref="A482:M482"/>
+    <mergeCell ref="A483:M483"/>
+    <mergeCell ref="N482:AD482"/>
+    <mergeCell ref="N483:AD483"/>
+    <mergeCell ref="A480:M480"/>
+    <mergeCell ref="A481:M481"/>
+    <mergeCell ref="N480:AD480"/>
+    <mergeCell ref="N481:AD481"/>
+    <mergeCell ref="A478:M478"/>
+    <mergeCell ref="A479:M479"/>
+    <mergeCell ref="N478:AD478"/>
+    <mergeCell ref="N479:AD479"/>
+    <mergeCell ref="A476:M476"/>
+    <mergeCell ref="A477:M477"/>
+    <mergeCell ref="N476:AD476"/>
+    <mergeCell ref="N477:AD477"/>
+    <mergeCell ref="AE479:AJ479"/>
+    <mergeCell ref="AK479:AP479"/>
+    <mergeCell ref="AE480:AJ480"/>
+    <mergeCell ref="AK480:AP480"/>
+    <mergeCell ref="AE481:AJ481"/>
+    <mergeCell ref="A468:M468"/>
+    <mergeCell ref="A469:M469"/>
+    <mergeCell ref="N468:AD468"/>
+    <mergeCell ref="N469:AD469"/>
+    <mergeCell ref="A466:M466"/>
+    <mergeCell ref="A467:M467"/>
+    <mergeCell ref="N466:AD466"/>
+    <mergeCell ref="N467:AD467"/>
+    <mergeCell ref="A464:M464"/>
+    <mergeCell ref="A465:M465"/>
+    <mergeCell ref="N464:AD464"/>
+    <mergeCell ref="N465:AD465"/>
+    <mergeCell ref="A474:M474"/>
+    <mergeCell ref="A475:M475"/>
+    <mergeCell ref="N474:AD474"/>
+    <mergeCell ref="N475:AD475"/>
+    <mergeCell ref="A472:M472"/>
+    <mergeCell ref="A473:M473"/>
+    <mergeCell ref="N472:AD472"/>
+    <mergeCell ref="N473:AD473"/>
+    <mergeCell ref="A470:M470"/>
+    <mergeCell ref="A471:M471"/>
+    <mergeCell ref="N470:AD470"/>
+    <mergeCell ref="N471:AD471"/>
+    <mergeCell ref="AE464:AJ464"/>
+    <mergeCell ref="AK464:AP464"/>
+    <mergeCell ref="A462:M462"/>
+    <mergeCell ref="A463:M463"/>
+    <mergeCell ref="N462:AD462"/>
+    <mergeCell ref="N463:AD463"/>
+    <mergeCell ref="A460:M460"/>
+    <mergeCell ref="A461:M461"/>
+    <mergeCell ref="N460:AD460"/>
+    <mergeCell ref="N461:AD461"/>
+    <mergeCell ref="A458:M458"/>
+    <mergeCell ref="A459:M459"/>
+    <mergeCell ref="N458:AD458"/>
+    <mergeCell ref="N459:AD459"/>
+    <mergeCell ref="AE461:AJ461"/>
+    <mergeCell ref="AK461:AP461"/>
+    <mergeCell ref="AE462:AJ462"/>
+    <mergeCell ref="AK462:AP462"/>
+    <mergeCell ref="AE463:AJ463"/>
+    <mergeCell ref="AE458:AJ458"/>
+    <mergeCell ref="AK458:AP458"/>
+    <mergeCell ref="AE459:AJ459"/>
+    <mergeCell ref="AK459:AP459"/>
+    <mergeCell ref="AE460:AJ460"/>
+    <mergeCell ref="AK460:AP460"/>
+    <mergeCell ref="AK463:AP463"/>
+    <mergeCell ref="A456:M456"/>
+    <mergeCell ref="A457:M457"/>
+    <mergeCell ref="N456:AD456"/>
+    <mergeCell ref="N457:AD457"/>
+    <mergeCell ref="A454:M454"/>
+    <mergeCell ref="A455:M455"/>
+    <mergeCell ref="N454:AD454"/>
+    <mergeCell ref="N455:AD455"/>
+    <mergeCell ref="A452:M452"/>
+    <mergeCell ref="A453:M453"/>
+    <mergeCell ref="N452:AD452"/>
+    <mergeCell ref="N453:AD453"/>
+    <mergeCell ref="AE452:AJ452"/>
+    <mergeCell ref="AK452:AP452"/>
+    <mergeCell ref="AE453:AJ453"/>
+    <mergeCell ref="AK453:AP453"/>
+    <mergeCell ref="AE454:AJ454"/>
+    <mergeCell ref="AE457:AJ457"/>
+    <mergeCell ref="AK457:AP457"/>
+    <mergeCell ref="AE439:AJ439"/>
+    <mergeCell ref="AK439:AP439"/>
+    <mergeCell ref="AE440:AJ440"/>
+    <mergeCell ref="AK440:AP440"/>
+    <mergeCell ref="AE441:AJ441"/>
+    <mergeCell ref="AK441:AP441"/>
+    <mergeCell ref="AE442:AJ442"/>
+    <mergeCell ref="AK442:AP442"/>
+    <mergeCell ref="AK445:AP445"/>
+    <mergeCell ref="A450:M450"/>
+    <mergeCell ref="A451:M451"/>
+    <mergeCell ref="N450:AD450"/>
+    <mergeCell ref="N451:AD451"/>
+    <mergeCell ref="A448:M448"/>
+    <mergeCell ref="A449:M449"/>
+    <mergeCell ref="N448:AD448"/>
+    <mergeCell ref="N449:AD449"/>
+    <mergeCell ref="A446:M446"/>
+    <mergeCell ref="A447:M447"/>
+    <mergeCell ref="N446:AD446"/>
+    <mergeCell ref="N447:AD447"/>
+    <mergeCell ref="A444:M444"/>
+    <mergeCell ref="A445:M445"/>
+    <mergeCell ref="N444:AD444"/>
+    <mergeCell ref="N445:AD445"/>
+    <mergeCell ref="A442:M442"/>
+    <mergeCell ref="A443:M443"/>
+    <mergeCell ref="N442:AD442"/>
+    <mergeCell ref="N443:AD443"/>
+    <mergeCell ref="A440:M440"/>
+    <mergeCell ref="A441:M441"/>
+    <mergeCell ref="N440:AD440"/>
+    <mergeCell ref="N441:AD441"/>
+    <mergeCell ref="AE443:AJ443"/>
+    <mergeCell ref="AK443:AP443"/>
+    <mergeCell ref="AE444:AJ444"/>
+    <mergeCell ref="AK444:AP444"/>
+    <mergeCell ref="AE445:AJ445"/>
+    <mergeCell ref="A432:M432"/>
+    <mergeCell ref="A433:M433"/>
+    <mergeCell ref="N432:AD432"/>
+    <mergeCell ref="N433:AD433"/>
+    <mergeCell ref="A430:M430"/>
+    <mergeCell ref="A431:M431"/>
+    <mergeCell ref="N430:AD430"/>
+    <mergeCell ref="N431:AD431"/>
+    <mergeCell ref="A428:M428"/>
+    <mergeCell ref="A429:M429"/>
+    <mergeCell ref="N428:AD428"/>
+    <mergeCell ref="N429:AD429"/>
+    <mergeCell ref="A438:M438"/>
+    <mergeCell ref="A439:M439"/>
+    <mergeCell ref="N438:AD438"/>
+    <mergeCell ref="N439:AD439"/>
+    <mergeCell ref="A436:M436"/>
+    <mergeCell ref="A437:M437"/>
+    <mergeCell ref="N436:AD436"/>
+    <mergeCell ref="N437:AD437"/>
+    <mergeCell ref="A434:M434"/>
+    <mergeCell ref="A435:M435"/>
+    <mergeCell ref="N434:AD434"/>
+    <mergeCell ref="N435:AD435"/>
+    <mergeCell ref="AE428:AJ428"/>
+    <mergeCell ref="AK428:AP428"/>
+    <mergeCell ref="A426:M426"/>
+    <mergeCell ref="A427:M427"/>
+    <mergeCell ref="N426:AD426"/>
+    <mergeCell ref="N427:AD427"/>
+    <mergeCell ref="A424:M424"/>
+    <mergeCell ref="A425:M425"/>
+    <mergeCell ref="N424:AD424"/>
+    <mergeCell ref="N425:AD425"/>
+    <mergeCell ref="A422:M422"/>
+    <mergeCell ref="A423:M423"/>
+    <mergeCell ref="N422:AD422"/>
+    <mergeCell ref="N423:AD423"/>
+    <mergeCell ref="AE425:AJ425"/>
+    <mergeCell ref="AK425:AP425"/>
+    <mergeCell ref="AE426:AJ426"/>
+    <mergeCell ref="AK426:AP426"/>
+    <mergeCell ref="AE427:AJ427"/>
+    <mergeCell ref="AE422:AJ422"/>
+    <mergeCell ref="AK422:AP422"/>
+    <mergeCell ref="AE423:AJ423"/>
+    <mergeCell ref="AK423:AP423"/>
+    <mergeCell ref="AE424:AJ424"/>
+    <mergeCell ref="AK424:AP424"/>
+    <mergeCell ref="AK427:AP427"/>
+    <mergeCell ref="A420:M420"/>
+    <mergeCell ref="A421:M421"/>
+    <mergeCell ref="N420:AD420"/>
+    <mergeCell ref="N421:AD421"/>
+    <mergeCell ref="A418:M418"/>
+    <mergeCell ref="A419:M419"/>
+    <mergeCell ref="N418:AD418"/>
+    <mergeCell ref="N419:AD419"/>
+    <mergeCell ref="A416:M416"/>
+    <mergeCell ref="A417:M417"/>
+    <mergeCell ref="N416:AD416"/>
+    <mergeCell ref="N417:AD417"/>
+    <mergeCell ref="AE416:AJ416"/>
+    <mergeCell ref="AK416:AP416"/>
+    <mergeCell ref="AE417:AJ417"/>
+    <mergeCell ref="AK417:AP417"/>
+    <mergeCell ref="AE418:AJ418"/>
+    <mergeCell ref="AE421:AJ421"/>
+    <mergeCell ref="AK421:AP421"/>
+    <mergeCell ref="AE403:AJ403"/>
+    <mergeCell ref="AK403:AP403"/>
+    <mergeCell ref="AE404:AJ404"/>
+    <mergeCell ref="AK404:AP404"/>
+    <mergeCell ref="AE405:AJ405"/>
+    <mergeCell ref="AK405:AP405"/>
+    <mergeCell ref="AE406:AJ406"/>
+    <mergeCell ref="AK406:AP406"/>
+    <mergeCell ref="AK409:AP409"/>
+    <mergeCell ref="A414:M414"/>
+    <mergeCell ref="A415:M415"/>
+    <mergeCell ref="N414:AD414"/>
+    <mergeCell ref="N415:AD415"/>
+    <mergeCell ref="A412:M412"/>
+    <mergeCell ref="A413:M413"/>
+    <mergeCell ref="N412:AD412"/>
+    <mergeCell ref="N413:AD413"/>
+    <mergeCell ref="A410:M410"/>
+    <mergeCell ref="A411:M411"/>
+    <mergeCell ref="N410:AD410"/>
+    <mergeCell ref="N411:AD411"/>
+    <mergeCell ref="A408:M408"/>
+    <mergeCell ref="A409:M409"/>
+    <mergeCell ref="N408:AD408"/>
+    <mergeCell ref="N409:AD409"/>
+    <mergeCell ref="A406:M406"/>
+    <mergeCell ref="A407:M407"/>
+    <mergeCell ref="N406:AD406"/>
+    <mergeCell ref="N407:AD407"/>
+    <mergeCell ref="A404:M404"/>
+    <mergeCell ref="A405:M405"/>
+    <mergeCell ref="N404:AD404"/>
+    <mergeCell ref="N405:AD405"/>
+    <mergeCell ref="AE407:AJ407"/>
+    <mergeCell ref="AK407:AP407"/>
+    <mergeCell ref="AE408:AJ408"/>
+    <mergeCell ref="AK408:AP408"/>
+    <mergeCell ref="AE409:AJ409"/>
+    <mergeCell ref="A396:M396"/>
+    <mergeCell ref="A397:M397"/>
+    <mergeCell ref="N396:AD396"/>
+    <mergeCell ref="N397:AD397"/>
+    <mergeCell ref="A394:M394"/>
+    <mergeCell ref="A395:M395"/>
+    <mergeCell ref="N394:AD394"/>
+    <mergeCell ref="N395:AD395"/>
+    <mergeCell ref="A392:M392"/>
+    <mergeCell ref="A393:M393"/>
+    <mergeCell ref="N392:AD392"/>
+    <mergeCell ref="N393:AD393"/>
+    <mergeCell ref="A402:M402"/>
+    <mergeCell ref="A403:M403"/>
+    <mergeCell ref="N402:AD402"/>
+    <mergeCell ref="N403:AD403"/>
+    <mergeCell ref="A400:M400"/>
+    <mergeCell ref="A401:M401"/>
+    <mergeCell ref="N400:AD400"/>
+    <mergeCell ref="N401:AD401"/>
+    <mergeCell ref="A398:M398"/>
+    <mergeCell ref="A399:M399"/>
+    <mergeCell ref="N398:AD398"/>
+    <mergeCell ref="N399:AD399"/>
+    <mergeCell ref="AE392:AJ392"/>
+    <mergeCell ref="AK392:AP392"/>
+    <mergeCell ref="A390:M390"/>
+    <mergeCell ref="A391:M391"/>
+    <mergeCell ref="N390:AD390"/>
+    <mergeCell ref="N391:AD391"/>
+    <mergeCell ref="A388:M388"/>
+    <mergeCell ref="A389:M389"/>
+    <mergeCell ref="N388:AD388"/>
+    <mergeCell ref="N389:AD389"/>
+    <mergeCell ref="A386:M386"/>
+    <mergeCell ref="A387:M387"/>
+    <mergeCell ref="N386:AD386"/>
+    <mergeCell ref="N387:AD387"/>
+    <mergeCell ref="AE389:AJ389"/>
+    <mergeCell ref="AK389:AP389"/>
+    <mergeCell ref="AE390:AJ390"/>
+    <mergeCell ref="AK390:AP390"/>
+    <mergeCell ref="AE391:AJ391"/>
+    <mergeCell ref="AE386:AJ386"/>
+    <mergeCell ref="AK386:AP386"/>
+    <mergeCell ref="AE387:AJ387"/>
+    <mergeCell ref="AK387:AP387"/>
+    <mergeCell ref="AE388:AJ388"/>
+    <mergeCell ref="AK388:AP388"/>
+    <mergeCell ref="AK391:AP391"/>
+    <mergeCell ref="A384:M384"/>
+    <mergeCell ref="A385:M385"/>
+    <mergeCell ref="N384:AD384"/>
+    <mergeCell ref="N385:AD385"/>
+    <mergeCell ref="A382:M382"/>
+    <mergeCell ref="A383:M383"/>
+    <mergeCell ref="N382:AD382"/>
+    <mergeCell ref="N383:AD383"/>
+    <mergeCell ref="A380:M380"/>
+    <mergeCell ref="A381:M381"/>
+    <mergeCell ref="N380:AD380"/>
+    <mergeCell ref="N381:AD381"/>
+    <mergeCell ref="AE380:AJ380"/>
+    <mergeCell ref="AK380:AP380"/>
+    <mergeCell ref="AE381:AJ381"/>
+    <mergeCell ref="AK381:AP381"/>
+    <mergeCell ref="AE382:AJ382"/>
+    <mergeCell ref="AE385:AJ385"/>
+    <mergeCell ref="AK385:AP385"/>
+    <mergeCell ref="AE367:AJ367"/>
+    <mergeCell ref="AK367:AP367"/>
+    <mergeCell ref="AE368:AJ368"/>
+    <mergeCell ref="AK368:AP368"/>
+    <mergeCell ref="AE369:AJ369"/>
+    <mergeCell ref="AK369:AP369"/>
+    <mergeCell ref="AE370:AJ370"/>
+    <mergeCell ref="AK370:AP370"/>
+    <mergeCell ref="AK373:AP373"/>
+    <mergeCell ref="A378:M378"/>
+    <mergeCell ref="A379:M379"/>
+    <mergeCell ref="N378:AD378"/>
+    <mergeCell ref="N379:AD379"/>
+    <mergeCell ref="A376:M376"/>
+    <mergeCell ref="A377:M377"/>
+    <mergeCell ref="N376:AD376"/>
+    <mergeCell ref="N377:AD377"/>
+    <mergeCell ref="A374:M374"/>
+    <mergeCell ref="A375:M375"/>
+    <mergeCell ref="N374:AD374"/>
+    <mergeCell ref="N375:AD375"/>
+    <mergeCell ref="A372:M372"/>
+    <mergeCell ref="A373:M373"/>
+    <mergeCell ref="N372:AD372"/>
+    <mergeCell ref="N373:AD373"/>
+    <mergeCell ref="A370:M370"/>
+    <mergeCell ref="A371:M371"/>
+    <mergeCell ref="N370:AD370"/>
+    <mergeCell ref="N371:AD371"/>
+    <mergeCell ref="A368:M368"/>
+    <mergeCell ref="A369:M369"/>
+    <mergeCell ref="N368:AD368"/>
+    <mergeCell ref="N369:AD369"/>
+    <mergeCell ref="AE371:AJ371"/>
+    <mergeCell ref="AK371:AP371"/>
+    <mergeCell ref="AE372:AJ372"/>
+    <mergeCell ref="AK372:AP372"/>
+    <mergeCell ref="AE373:AJ373"/>
+    <mergeCell ref="A360:M360"/>
+    <mergeCell ref="A361:M361"/>
+    <mergeCell ref="N360:AD360"/>
+    <mergeCell ref="N361:AD361"/>
+    <mergeCell ref="A358:M358"/>
+    <mergeCell ref="A359:M359"/>
+    <mergeCell ref="N358:AD358"/>
+    <mergeCell ref="N359:AD359"/>
+    <mergeCell ref="A356:M356"/>
+    <mergeCell ref="A357:M357"/>
+    <mergeCell ref="N356:AD356"/>
+    <mergeCell ref="N357:AD357"/>
+    <mergeCell ref="A366:M366"/>
+    <mergeCell ref="A367:M367"/>
+    <mergeCell ref="N366:AD366"/>
+    <mergeCell ref="N367:AD367"/>
+    <mergeCell ref="A364:M364"/>
+    <mergeCell ref="A365:M365"/>
+    <mergeCell ref="N364:AD364"/>
+    <mergeCell ref="N365:AD365"/>
+    <mergeCell ref="A362:M362"/>
+    <mergeCell ref="A363:M363"/>
+    <mergeCell ref="N362:AD362"/>
+    <mergeCell ref="N363:AD363"/>
+    <mergeCell ref="AE356:AJ356"/>
+    <mergeCell ref="AK356:AP356"/>
+    <mergeCell ref="A354:M354"/>
+    <mergeCell ref="A355:M355"/>
+    <mergeCell ref="N354:AD354"/>
+    <mergeCell ref="N355:AD355"/>
+    <mergeCell ref="A352:M352"/>
+    <mergeCell ref="A353:M353"/>
+    <mergeCell ref="N352:AD352"/>
+    <mergeCell ref="N353:AD353"/>
+    <mergeCell ref="A350:M350"/>
+    <mergeCell ref="A351:M351"/>
+    <mergeCell ref="N350:AD350"/>
+    <mergeCell ref="N351:AD351"/>
+    <mergeCell ref="AE353:AJ353"/>
+    <mergeCell ref="AK353:AP353"/>
+    <mergeCell ref="AE354:AJ354"/>
+    <mergeCell ref="AK354:AP354"/>
+    <mergeCell ref="AE355:AJ355"/>
+    <mergeCell ref="AE350:AJ350"/>
+    <mergeCell ref="AK350:AP350"/>
+    <mergeCell ref="AE351:AJ351"/>
+    <mergeCell ref="AK351:AP351"/>
+    <mergeCell ref="AE352:AJ352"/>
+    <mergeCell ref="AK352:AP352"/>
+    <mergeCell ref="AK355:AP355"/>
+    <mergeCell ref="A348:M348"/>
+    <mergeCell ref="A349:M349"/>
+    <mergeCell ref="N348:AD348"/>
+    <mergeCell ref="N349:AD349"/>
+    <mergeCell ref="A346:M346"/>
+    <mergeCell ref="A347:M347"/>
+    <mergeCell ref="N346:AD346"/>
+    <mergeCell ref="N347:AD347"/>
+    <mergeCell ref="A344:M344"/>
+    <mergeCell ref="A345:M345"/>
+    <mergeCell ref="N344:AD344"/>
+    <mergeCell ref="N345:AD345"/>
+    <mergeCell ref="AE344:AJ344"/>
+    <mergeCell ref="AK344:AP344"/>
+    <mergeCell ref="AE345:AJ345"/>
+    <mergeCell ref="AK345:AP345"/>
+    <mergeCell ref="AE346:AJ346"/>
+    <mergeCell ref="AE349:AJ349"/>
+    <mergeCell ref="AK349:AP349"/>
+    <mergeCell ref="AE331:AJ331"/>
+    <mergeCell ref="AK331:AP331"/>
+    <mergeCell ref="AE332:AJ332"/>
+    <mergeCell ref="AK332:AP332"/>
+    <mergeCell ref="AE333:AJ333"/>
+    <mergeCell ref="AK333:AP333"/>
+    <mergeCell ref="AE334:AJ334"/>
+    <mergeCell ref="AK334:AP334"/>
+    <mergeCell ref="AK337:AP337"/>
+    <mergeCell ref="A342:M342"/>
+    <mergeCell ref="A343:M343"/>
+    <mergeCell ref="N342:AD342"/>
+    <mergeCell ref="N343:AD343"/>
+    <mergeCell ref="A340:M340"/>
+    <mergeCell ref="A341:M341"/>
+    <mergeCell ref="N340:AD340"/>
+    <mergeCell ref="N341:AD341"/>
+    <mergeCell ref="A338:M338"/>
+    <mergeCell ref="A339:M339"/>
+    <mergeCell ref="N338:AD338"/>
+    <mergeCell ref="N339:AD339"/>
+    <mergeCell ref="A336:M336"/>
+    <mergeCell ref="A337:M337"/>
+    <mergeCell ref="N336:AD336"/>
+    <mergeCell ref="N337:AD337"/>
+    <mergeCell ref="A334:M334"/>
+    <mergeCell ref="A335:M335"/>
+    <mergeCell ref="N334:AD334"/>
+    <mergeCell ref="N335:AD335"/>
+    <mergeCell ref="A332:M332"/>
+    <mergeCell ref="A333:M333"/>
+    <mergeCell ref="N332:AD332"/>
+    <mergeCell ref="N333:AD333"/>
+    <mergeCell ref="AE335:AJ335"/>
+    <mergeCell ref="AK335:AP335"/>
+    <mergeCell ref="AE336:AJ336"/>
+    <mergeCell ref="AK336:AP336"/>
+    <mergeCell ref="AE337:AJ337"/>
+    <mergeCell ref="A324:M324"/>
+    <mergeCell ref="A325:M325"/>
+    <mergeCell ref="N324:AD324"/>
+    <mergeCell ref="N325:AD325"/>
+    <mergeCell ref="A322:M322"/>
+    <mergeCell ref="A323:M323"/>
+    <mergeCell ref="N322:AD322"/>
+    <mergeCell ref="N323:AD323"/>
+    <mergeCell ref="A320:M320"/>
+    <mergeCell ref="A321:M321"/>
+    <mergeCell ref="N320:AD320"/>
+    <mergeCell ref="N321:AD321"/>
+    <mergeCell ref="A330:M330"/>
+    <mergeCell ref="A331:M331"/>
+    <mergeCell ref="N330:AD330"/>
+    <mergeCell ref="N331:AD331"/>
+    <mergeCell ref="A328:M328"/>
+    <mergeCell ref="A329:M329"/>
+    <mergeCell ref="N328:AD328"/>
+    <mergeCell ref="N329:AD329"/>
+    <mergeCell ref="A326:M326"/>
+    <mergeCell ref="A327:M327"/>
+    <mergeCell ref="N326:AD326"/>
+    <mergeCell ref="N327:AD327"/>
+    <mergeCell ref="AE320:AJ320"/>
+    <mergeCell ref="AK320:AP320"/>
+    <mergeCell ref="A318:M318"/>
+    <mergeCell ref="A319:M319"/>
+    <mergeCell ref="N318:AD318"/>
+    <mergeCell ref="N319:AD319"/>
+    <mergeCell ref="A316:M316"/>
+    <mergeCell ref="A317:M317"/>
+    <mergeCell ref="N316:AD316"/>
+    <mergeCell ref="N317:AD317"/>
+    <mergeCell ref="A314:M314"/>
+    <mergeCell ref="A315:M315"/>
+    <mergeCell ref="N314:AD314"/>
+    <mergeCell ref="N315:AD315"/>
+    <mergeCell ref="AE317:AJ317"/>
+    <mergeCell ref="AK317:AP317"/>
+    <mergeCell ref="AE318:AJ318"/>
+    <mergeCell ref="AK318:AP318"/>
+    <mergeCell ref="AE319:AJ319"/>
+    <mergeCell ref="AE314:AJ314"/>
+    <mergeCell ref="AK314:AP314"/>
+    <mergeCell ref="AE315:AJ315"/>
+    <mergeCell ref="AK315:AP315"/>
+    <mergeCell ref="AE316:AJ316"/>
+    <mergeCell ref="AK316:AP316"/>
+    <mergeCell ref="AK319:AP319"/>
+    <mergeCell ref="A312:M312"/>
+    <mergeCell ref="A313:M313"/>
+    <mergeCell ref="N312:AD312"/>
+    <mergeCell ref="N313:AD313"/>
+    <mergeCell ref="A310:M310"/>
+    <mergeCell ref="A311:M311"/>
+    <mergeCell ref="N310:AD310"/>
+    <mergeCell ref="N311:AD311"/>
+    <mergeCell ref="A308:M308"/>
+    <mergeCell ref="A309:M309"/>
+    <mergeCell ref="N308:AD308"/>
+    <mergeCell ref="N309:AD309"/>
+    <mergeCell ref="AE308:AJ308"/>
+    <mergeCell ref="AK308:AP308"/>
+    <mergeCell ref="AE309:AJ309"/>
+    <mergeCell ref="AK309:AP309"/>
+    <mergeCell ref="AE310:AJ310"/>
+    <mergeCell ref="AE313:AJ313"/>
+    <mergeCell ref="AK313:AP313"/>
+    <mergeCell ref="AE295:AJ295"/>
+    <mergeCell ref="AK295:AP295"/>
+    <mergeCell ref="AE296:AJ296"/>
+    <mergeCell ref="AK296:AP296"/>
+    <mergeCell ref="AE297:AJ297"/>
+    <mergeCell ref="AK297:AP297"/>
+    <mergeCell ref="AE298:AJ298"/>
+    <mergeCell ref="AK298:AP298"/>
+    <mergeCell ref="AK301:AP301"/>
+    <mergeCell ref="A306:M306"/>
+    <mergeCell ref="A307:M307"/>
+    <mergeCell ref="N306:AD306"/>
+    <mergeCell ref="N307:AD307"/>
+    <mergeCell ref="A304:M304"/>
+    <mergeCell ref="A305:M305"/>
+    <mergeCell ref="N304:AD304"/>
+    <mergeCell ref="N305:AD305"/>
+    <mergeCell ref="A302:M302"/>
+    <mergeCell ref="A303:M303"/>
+    <mergeCell ref="N302:AD302"/>
+    <mergeCell ref="N303:AD303"/>
+    <mergeCell ref="A300:M300"/>
+    <mergeCell ref="A301:M301"/>
+    <mergeCell ref="N300:AD300"/>
+    <mergeCell ref="N301:AD301"/>
+    <mergeCell ref="A298:M298"/>
+    <mergeCell ref="A299:M299"/>
+    <mergeCell ref="N298:AD298"/>
+    <mergeCell ref="N299:AD299"/>
+    <mergeCell ref="A296:M296"/>
+    <mergeCell ref="A297:M297"/>
+    <mergeCell ref="N296:AD296"/>
+    <mergeCell ref="N297:AD297"/>
+    <mergeCell ref="AE299:AJ299"/>
+    <mergeCell ref="AK299:AP299"/>
+    <mergeCell ref="AE300:AJ300"/>
+    <mergeCell ref="AK300:AP300"/>
+    <mergeCell ref="AE301:AJ301"/>
+    <mergeCell ref="A288:M288"/>
+    <mergeCell ref="A289:M289"/>
+    <mergeCell ref="N288:AD288"/>
+    <mergeCell ref="N289:AD289"/>
+    <mergeCell ref="A286:M286"/>
+    <mergeCell ref="A287:M287"/>
+    <mergeCell ref="N286:AD286"/>
+    <mergeCell ref="N287:AD287"/>
+    <mergeCell ref="A284:M284"/>
+    <mergeCell ref="A285:M285"/>
+    <mergeCell ref="N284:AD284"/>
+    <mergeCell ref="N285:AD285"/>
+    <mergeCell ref="A294:M294"/>
+    <mergeCell ref="A295:M295"/>
+    <mergeCell ref="N294:AD294"/>
+    <mergeCell ref="N295:AD295"/>
+    <mergeCell ref="A292:M292"/>
+    <mergeCell ref="A293:M293"/>
+    <mergeCell ref="N292:AD292"/>
+    <mergeCell ref="N293:AD293"/>
+    <mergeCell ref="A290:M290"/>
+    <mergeCell ref="A291:M291"/>
+    <mergeCell ref="N290:AD290"/>
+    <mergeCell ref="N291:AD291"/>
+    <mergeCell ref="AE284:AJ284"/>
+    <mergeCell ref="AK284:AP284"/>
+    <mergeCell ref="A282:M282"/>
+    <mergeCell ref="A283:M283"/>
+    <mergeCell ref="N282:AD282"/>
+    <mergeCell ref="N283:AD283"/>
+    <mergeCell ref="A280:M280"/>
+    <mergeCell ref="A281:M281"/>
+    <mergeCell ref="N280:AD280"/>
+    <mergeCell ref="N281:AD281"/>
+    <mergeCell ref="A278:M278"/>
+    <mergeCell ref="A279:M279"/>
+    <mergeCell ref="N278:AD278"/>
+    <mergeCell ref="N279:AD279"/>
+    <mergeCell ref="AE281:AJ281"/>
+    <mergeCell ref="AK281:AP281"/>
+    <mergeCell ref="AE282:AJ282"/>
+    <mergeCell ref="AK282:AP282"/>
+    <mergeCell ref="AE283:AJ283"/>
+    <mergeCell ref="AE278:AJ278"/>
+    <mergeCell ref="AK278:AP278"/>
+    <mergeCell ref="AE279:AJ279"/>
+    <mergeCell ref="AK279:AP279"/>
+    <mergeCell ref="AE280:AJ280"/>
+    <mergeCell ref="AK280:AP280"/>
+    <mergeCell ref="AK283:AP283"/>
+    <mergeCell ref="A276:M276"/>
+    <mergeCell ref="A277:M277"/>
+    <mergeCell ref="N276:AD276"/>
+    <mergeCell ref="N277:AD277"/>
+    <mergeCell ref="A274:M274"/>
+    <mergeCell ref="A275:M275"/>
+    <mergeCell ref="N274:AD274"/>
+    <mergeCell ref="N275:AD275"/>
+    <mergeCell ref="A272:M272"/>
+    <mergeCell ref="A273:M273"/>
+    <mergeCell ref="N272:AD272"/>
+    <mergeCell ref="N273:AD273"/>
+    <mergeCell ref="AE272:AJ272"/>
+    <mergeCell ref="AK272:AP272"/>
+    <mergeCell ref="AE273:AJ273"/>
+    <mergeCell ref="AK273:AP273"/>
+    <mergeCell ref="AE274:AJ274"/>
+    <mergeCell ref="AE277:AJ277"/>
+    <mergeCell ref="AK277:AP277"/>
+    <mergeCell ref="AE259:AJ259"/>
+    <mergeCell ref="AK259:AP259"/>
+    <mergeCell ref="AE260:AJ260"/>
+    <mergeCell ref="AK260:AP260"/>
+    <mergeCell ref="AE261:AJ261"/>
+    <mergeCell ref="AK261:AP261"/>
+    <mergeCell ref="AE262:AJ262"/>
+    <mergeCell ref="AK262:AP262"/>
+    <mergeCell ref="AK265:AP265"/>
+    <mergeCell ref="A270:M270"/>
+    <mergeCell ref="A271:M271"/>
+    <mergeCell ref="N270:AD270"/>
+    <mergeCell ref="N271:AD271"/>
+    <mergeCell ref="A268:M268"/>
+    <mergeCell ref="A269:M269"/>
+    <mergeCell ref="N268:AD268"/>
+    <mergeCell ref="N269:AD269"/>
+    <mergeCell ref="A266:M266"/>
+    <mergeCell ref="A267:M267"/>
+    <mergeCell ref="N266:AD266"/>
+    <mergeCell ref="N267:AD267"/>
+    <mergeCell ref="A264:M264"/>
+    <mergeCell ref="A265:M265"/>
+    <mergeCell ref="N264:AD264"/>
+    <mergeCell ref="N265:AD265"/>
+    <mergeCell ref="A262:M262"/>
+    <mergeCell ref="A263:M263"/>
+    <mergeCell ref="N262:AD262"/>
+    <mergeCell ref="N263:AD263"/>
+    <mergeCell ref="A260:M260"/>
+    <mergeCell ref="A261:M261"/>
+    <mergeCell ref="N260:AD260"/>
+    <mergeCell ref="N261:AD261"/>
+    <mergeCell ref="AE263:AJ263"/>
+    <mergeCell ref="AK263:AP263"/>
+    <mergeCell ref="AE264:AJ264"/>
+    <mergeCell ref="AK264:AP264"/>
+    <mergeCell ref="AE265:AJ265"/>
+    <mergeCell ref="A252:M252"/>
+    <mergeCell ref="A253:M253"/>
+    <mergeCell ref="N252:AD252"/>
+    <mergeCell ref="N253:AD253"/>
+    <mergeCell ref="A250:M250"/>
+    <mergeCell ref="A251:M251"/>
+    <mergeCell ref="N250:AD250"/>
+    <mergeCell ref="N251:AD251"/>
+    <mergeCell ref="A248:M248"/>
+    <mergeCell ref="A249:M249"/>
+    <mergeCell ref="N248:AD248"/>
+    <mergeCell ref="N249:AD249"/>
+    <mergeCell ref="A258:M258"/>
+    <mergeCell ref="A259:M259"/>
+    <mergeCell ref="N258:AD258"/>
+    <mergeCell ref="N259:AD259"/>
+    <mergeCell ref="A256:M256"/>
+    <mergeCell ref="A257:M257"/>
+    <mergeCell ref="N256:AD256"/>
+    <mergeCell ref="N257:AD257"/>
+    <mergeCell ref="A254:M254"/>
+    <mergeCell ref="A255:M255"/>
+    <mergeCell ref="N254:AD254"/>
+    <mergeCell ref="N255:AD255"/>
+    <mergeCell ref="AE248:AJ248"/>
+    <mergeCell ref="AK248:AP248"/>
+    <mergeCell ref="A246:M246"/>
+    <mergeCell ref="A247:M247"/>
+    <mergeCell ref="N246:AD246"/>
+    <mergeCell ref="N247:AD247"/>
+    <mergeCell ref="A244:M244"/>
+    <mergeCell ref="A245:M245"/>
+    <mergeCell ref="N244:AD244"/>
+    <mergeCell ref="N245:AD245"/>
+    <mergeCell ref="A242:M242"/>
+    <mergeCell ref="A243:M243"/>
+    <mergeCell ref="N242:AD242"/>
+    <mergeCell ref="N243:AD243"/>
+    <mergeCell ref="AE245:AJ245"/>
+    <mergeCell ref="AK245:AP245"/>
+    <mergeCell ref="AE246:AJ246"/>
+    <mergeCell ref="AK246:AP246"/>
+    <mergeCell ref="AE247:AJ247"/>
+    <mergeCell ref="AE242:AJ242"/>
+    <mergeCell ref="AK242:AP242"/>
+    <mergeCell ref="AE243:AJ243"/>
+    <mergeCell ref="AK243:AP243"/>
+    <mergeCell ref="AE244:AJ244"/>
+    <mergeCell ref="AK244:AP244"/>
+    <mergeCell ref="AK247:AP247"/>
+    <mergeCell ref="A240:M240"/>
+    <mergeCell ref="A241:M241"/>
+    <mergeCell ref="N240:AD240"/>
+    <mergeCell ref="N241:AD241"/>
+    <mergeCell ref="A238:M238"/>
+    <mergeCell ref="A239:M239"/>
+    <mergeCell ref="N238:AD238"/>
+    <mergeCell ref="N239:AD239"/>
+    <mergeCell ref="A236:M236"/>
+    <mergeCell ref="A237:M237"/>
+    <mergeCell ref="N236:AD236"/>
+    <mergeCell ref="N237:AD237"/>
+    <mergeCell ref="AE236:AJ236"/>
+    <mergeCell ref="AK236:AP236"/>
+    <mergeCell ref="AE237:AJ237"/>
+    <mergeCell ref="AK237:AP237"/>
+    <mergeCell ref="AE238:AJ238"/>
+    <mergeCell ref="AE241:AJ241"/>
+    <mergeCell ref="AK241:AP241"/>
+    <mergeCell ref="AE223:AJ223"/>
+    <mergeCell ref="AK223:AP223"/>
+    <mergeCell ref="AE224:AJ224"/>
+    <mergeCell ref="AK224:AP224"/>
+    <mergeCell ref="AE225:AJ225"/>
+    <mergeCell ref="AK225:AP225"/>
+    <mergeCell ref="AE226:AJ226"/>
+    <mergeCell ref="AK226:AP226"/>
+    <mergeCell ref="AK229:AP229"/>
+    <mergeCell ref="A234:M234"/>
+    <mergeCell ref="A235:M235"/>
+    <mergeCell ref="N234:AD234"/>
+    <mergeCell ref="N235:AD235"/>
+    <mergeCell ref="A232:M232"/>
+    <mergeCell ref="A233:M233"/>
+    <mergeCell ref="N232:AD232"/>
+    <mergeCell ref="N233:AD233"/>
+    <mergeCell ref="A230:M230"/>
+    <mergeCell ref="A231:M231"/>
+    <mergeCell ref="N230:AD230"/>
+    <mergeCell ref="N231:AD231"/>
+    <mergeCell ref="A228:M228"/>
+    <mergeCell ref="A229:M229"/>
+    <mergeCell ref="N228:AD228"/>
+    <mergeCell ref="N229:AD229"/>
+    <mergeCell ref="A226:M226"/>
+    <mergeCell ref="A227:M227"/>
+    <mergeCell ref="N226:AD226"/>
+    <mergeCell ref="N227:AD227"/>
+    <mergeCell ref="A224:M224"/>
+    <mergeCell ref="A225:M225"/>
+    <mergeCell ref="N224:AD224"/>
+    <mergeCell ref="N225:AD225"/>
+    <mergeCell ref="AE227:AJ227"/>
+    <mergeCell ref="AK227:AP227"/>
+    <mergeCell ref="AE228:AJ228"/>
+    <mergeCell ref="AK228:AP228"/>
+    <mergeCell ref="AE229:AJ229"/>
+    <mergeCell ref="A216:M216"/>
+    <mergeCell ref="A217:M217"/>
+    <mergeCell ref="N216:AD216"/>
+    <mergeCell ref="N217:AD217"/>
+    <mergeCell ref="A214:M214"/>
+    <mergeCell ref="A215:M215"/>
+    <mergeCell ref="N214:AD214"/>
+    <mergeCell ref="N215:AD215"/>
+    <mergeCell ref="A212:M212"/>
+    <mergeCell ref="A213:M213"/>
+    <mergeCell ref="N212:AD212"/>
+    <mergeCell ref="N213:AD213"/>
+    <mergeCell ref="A222:M222"/>
+    <mergeCell ref="A223:M223"/>
+    <mergeCell ref="N222:AD222"/>
+    <mergeCell ref="N223:AD223"/>
+    <mergeCell ref="A220:M220"/>
+    <mergeCell ref="A221:M221"/>
+    <mergeCell ref="N220:AD220"/>
+    <mergeCell ref="N221:AD221"/>
+    <mergeCell ref="A218:M218"/>
+    <mergeCell ref="A219:M219"/>
+    <mergeCell ref="N218:AD218"/>
+    <mergeCell ref="N219:AD219"/>
+    <mergeCell ref="AE212:AJ212"/>
+    <mergeCell ref="AK212:AP212"/>
+    <mergeCell ref="A210:M210"/>
+    <mergeCell ref="A211:M211"/>
+    <mergeCell ref="N210:AD210"/>
+    <mergeCell ref="N211:AD211"/>
+    <mergeCell ref="A208:M208"/>
+    <mergeCell ref="A209:M209"/>
+    <mergeCell ref="N208:AD208"/>
+    <mergeCell ref="N209:AD209"/>
+    <mergeCell ref="A206:M206"/>
+    <mergeCell ref="A207:M207"/>
+    <mergeCell ref="N206:AD206"/>
+    <mergeCell ref="N207:AD207"/>
+    <mergeCell ref="AE209:AJ209"/>
+    <mergeCell ref="AK209:AP209"/>
+    <mergeCell ref="AE210:AJ210"/>
+    <mergeCell ref="AK210:AP210"/>
+    <mergeCell ref="AE211:AJ211"/>
+    <mergeCell ref="AE206:AJ206"/>
+    <mergeCell ref="AK206:AP206"/>
+    <mergeCell ref="AE207:AJ207"/>
+    <mergeCell ref="AK207:AP207"/>
+    <mergeCell ref="AE208:AJ208"/>
+    <mergeCell ref="AK208:AP208"/>
+    <mergeCell ref="AK211:AP211"/>
+    <mergeCell ref="A204:M204"/>
+    <mergeCell ref="A205:M205"/>
+    <mergeCell ref="N204:AD204"/>
+    <mergeCell ref="N205:AD205"/>
+    <mergeCell ref="A202:M202"/>
+    <mergeCell ref="A203:M203"/>
+    <mergeCell ref="N202:AD202"/>
+    <mergeCell ref="N203:AD203"/>
+    <mergeCell ref="A200:M200"/>
+    <mergeCell ref="A201:M201"/>
+    <mergeCell ref="N200:AD200"/>
+    <mergeCell ref="N201:AD201"/>
+    <mergeCell ref="AE200:AJ200"/>
+    <mergeCell ref="AK200:AP200"/>
+    <mergeCell ref="AE201:AJ201"/>
+    <mergeCell ref="AK201:AP201"/>
+    <mergeCell ref="AE202:AJ202"/>
+    <mergeCell ref="AE205:AJ205"/>
+    <mergeCell ref="AK205:AP205"/>
+    <mergeCell ref="AE187:AJ187"/>
+    <mergeCell ref="AK187:AP187"/>
+    <mergeCell ref="AE188:AJ188"/>
+    <mergeCell ref="AK188:AP188"/>
+    <mergeCell ref="AE189:AJ189"/>
+    <mergeCell ref="AK189:AP189"/>
+    <mergeCell ref="AE190:AJ190"/>
+    <mergeCell ref="AK190:AP190"/>
+    <mergeCell ref="AK193:AP193"/>
+    <mergeCell ref="A198:M198"/>
+    <mergeCell ref="A199:M199"/>
+    <mergeCell ref="N198:AD198"/>
+    <mergeCell ref="N199:AD199"/>
+    <mergeCell ref="A196:M196"/>
+    <mergeCell ref="A197:M197"/>
+    <mergeCell ref="N196:AD196"/>
+    <mergeCell ref="N197:AD197"/>
+    <mergeCell ref="A194:M194"/>
+    <mergeCell ref="A195:M195"/>
+    <mergeCell ref="N194:AD194"/>
+    <mergeCell ref="N195:AD195"/>
+    <mergeCell ref="A192:M192"/>
+    <mergeCell ref="A193:M193"/>
+    <mergeCell ref="N192:AD192"/>
+    <mergeCell ref="N193:AD193"/>
+    <mergeCell ref="A190:M190"/>
+    <mergeCell ref="A191:M191"/>
+    <mergeCell ref="N190:AD190"/>
+    <mergeCell ref="N191:AD191"/>
+    <mergeCell ref="A188:M188"/>
+    <mergeCell ref="A189:M189"/>
+    <mergeCell ref="N188:AD188"/>
+    <mergeCell ref="N189:AD189"/>
+    <mergeCell ref="AE191:AJ191"/>
+    <mergeCell ref="AK191:AP191"/>
+    <mergeCell ref="AE192:AJ192"/>
+    <mergeCell ref="AK192:AP192"/>
+    <mergeCell ref="AE193:AJ193"/>
+    <mergeCell ref="A180:M180"/>
+    <mergeCell ref="A181:M181"/>
+    <mergeCell ref="N180:AD180"/>
+    <mergeCell ref="N181:AD181"/>
+    <mergeCell ref="A178:M178"/>
+    <mergeCell ref="A179:M179"/>
+    <mergeCell ref="N178:AD178"/>
+    <mergeCell ref="N179:AD179"/>
+    <mergeCell ref="A176:M176"/>
+    <mergeCell ref="A177:M177"/>
+    <mergeCell ref="N176:AD176"/>
+    <mergeCell ref="N177:AD177"/>
+    <mergeCell ref="A186:M186"/>
+    <mergeCell ref="A187:M187"/>
+    <mergeCell ref="N186:AD186"/>
+    <mergeCell ref="N187:AD187"/>
+    <mergeCell ref="A184:M184"/>
+    <mergeCell ref="A185:M185"/>
+    <mergeCell ref="N184:AD184"/>
+    <mergeCell ref="N185:AD185"/>
+    <mergeCell ref="A182:M182"/>
+    <mergeCell ref="A183:M183"/>
+    <mergeCell ref="N182:AD182"/>
+    <mergeCell ref="N183:AD183"/>
+    <mergeCell ref="AE176:AJ176"/>
+    <mergeCell ref="AK176:AP176"/>
+    <mergeCell ref="A174:M174"/>
+    <mergeCell ref="A175:M175"/>
+    <mergeCell ref="N174:AD174"/>
+    <mergeCell ref="N175:AD175"/>
+    <mergeCell ref="A172:M172"/>
+    <mergeCell ref="A173:M173"/>
+    <mergeCell ref="N172:AD172"/>
+    <mergeCell ref="N173:AD173"/>
+    <mergeCell ref="A170:M170"/>
+    <mergeCell ref="A171:M171"/>
+    <mergeCell ref="N170:AD170"/>
+    <mergeCell ref="N171:AD171"/>
+    <mergeCell ref="AE173:AJ173"/>
+    <mergeCell ref="AK173:AP173"/>
+    <mergeCell ref="AE174:AJ174"/>
+    <mergeCell ref="AK174:AP174"/>
+    <mergeCell ref="AE175:AJ175"/>
+    <mergeCell ref="AE170:AJ170"/>
+    <mergeCell ref="AK170:AP170"/>
+    <mergeCell ref="AE171:AJ171"/>
+    <mergeCell ref="AK171:AP171"/>
+    <mergeCell ref="AE172:AJ172"/>
+    <mergeCell ref="AK172:AP172"/>
+    <mergeCell ref="AK175:AP175"/>
+    <mergeCell ref="A168:M168"/>
+    <mergeCell ref="A169:M169"/>
+    <mergeCell ref="N168:AD168"/>
+    <mergeCell ref="N169:AD169"/>
+    <mergeCell ref="A166:M166"/>
+    <mergeCell ref="A167:M167"/>
+    <mergeCell ref="N166:AD166"/>
+    <mergeCell ref="N167:AD167"/>
+    <mergeCell ref="A164:M164"/>
+    <mergeCell ref="A165:M165"/>
+    <mergeCell ref="N164:AD164"/>
+    <mergeCell ref="N165:AD165"/>
+    <mergeCell ref="AE164:AJ164"/>
+    <mergeCell ref="AK164:AP164"/>
+    <mergeCell ref="AE165:AJ165"/>
+    <mergeCell ref="AK165:AP165"/>
+    <mergeCell ref="AE166:AJ166"/>
+    <mergeCell ref="AE169:AJ169"/>
+    <mergeCell ref="AK169:AP169"/>
+    <mergeCell ref="AE151:AJ151"/>
+    <mergeCell ref="AK151:AP151"/>
+    <mergeCell ref="AE152:AJ152"/>
+    <mergeCell ref="AK152:AP152"/>
+    <mergeCell ref="AE153:AJ153"/>
+    <mergeCell ref="AK153:AP153"/>
+    <mergeCell ref="AE154:AJ154"/>
+    <mergeCell ref="AK154:AP154"/>
+    <mergeCell ref="AK157:AP157"/>
+    <mergeCell ref="A162:M162"/>
+    <mergeCell ref="A163:M163"/>
+    <mergeCell ref="N162:AD162"/>
+    <mergeCell ref="N163:AD163"/>
+    <mergeCell ref="A160:M160"/>
+    <mergeCell ref="A161:M161"/>
+    <mergeCell ref="N160:AD160"/>
+    <mergeCell ref="N161:AD161"/>
+    <mergeCell ref="A158:M158"/>
+    <mergeCell ref="A159:M159"/>
+    <mergeCell ref="N158:AD158"/>
+    <mergeCell ref="N159:AD159"/>
+    <mergeCell ref="A156:M156"/>
+    <mergeCell ref="A157:M157"/>
+    <mergeCell ref="N156:AD156"/>
+    <mergeCell ref="N157:AD157"/>
+    <mergeCell ref="A154:M154"/>
+    <mergeCell ref="A155:M155"/>
+    <mergeCell ref="N154:AD154"/>
+    <mergeCell ref="N155:AD155"/>
+    <mergeCell ref="A152:M152"/>
+    <mergeCell ref="A153:M153"/>
+    <mergeCell ref="N152:AD152"/>
+    <mergeCell ref="N153:AD153"/>
+    <mergeCell ref="AE155:AJ155"/>
+    <mergeCell ref="AK155:AP155"/>
+    <mergeCell ref="AE156:AJ156"/>
+    <mergeCell ref="AK156:AP156"/>
+    <mergeCell ref="AE157:AJ157"/>
+    <mergeCell ref="A144:M144"/>
+    <mergeCell ref="A145:M145"/>
+    <mergeCell ref="N144:AD144"/>
+    <mergeCell ref="N145:AD145"/>
+    <mergeCell ref="A142:M142"/>
+    <mergeCell ref="A143:M143"/>
+    <mergeCell ref="N142:AD142"/>
+    <mergeCell ref="N143:AD143"/>
+    <mergeCell ref="A140:M140"/>
+    <mergeCell ref="A141:M141"/>
+    <mergeCell ref="N140:AD140"/>
+    <mergeCell ref="N141:AD141"/>
+    <mergeCell ref="A150:M150"/>
+    <mergeCell ref="A151:M151"/>
+    <mergeCell ref="N150:AD150"/>
+    <mergeCell ref="N151:AD151"/>
+    <mergeCell ref="A148:M148"/>
+    <mergeCell ref="A149:M149"/>
+    <mergeCell ref="N148:AD148"/>
+    <mergeCell ref="N149:AD149"/>
+    <mergeCell ref="A146:M146"/>
+    <mergeCell ref="A147:M147"/>
+    <mergeCell ref="N146:AD146"/>
+    <mergeCell ref="N147:AD147"/>
+    <mergeCell ref="AE140:AJ140"/>
+    <mergeCell ref="AK140:AP140"/>
+    <mergeCell ref="A138:M138"/>
+    <mergeCell ref="A139:M139"/>
+    <mergeCell ref="N138:AD138"/>
+    <mergeCell ref="N139:AD139"/>
+    <mergeCell ref="A136:M136"/>
+    <mergeCell ref="A137:M137"/>
+    <mergeCell ref="N136:AD136"/>
+    <mergeCell ref="N137:AD137"/>
+    <mergeCell ref="A134:M134"/>
+    <mergeCell ref="A135:M135"/>
+    <mergeCell ref="N134:AD134"/>
+    <mergeCell ref="N135:AD135"/>
+    <mergeCell ref="AE137:AJ137"/>
+    <mergeCell ref="AK137:AP137"/>
+    <mergeCell ref="AE138:AJ138"/>
+    <mergeCell ref="AK138:AP138"/>
+    <mergeCell ref="AE139:AJ139"/>
+    <mergeCell ref="AE134:AJ134"/>
+    <mergeCell ref="AK134:AP134"/>
+    <mergeCell ref="AE135:AJ135"/>
+    <mergeCell ref="AK135:AP135"/>
+    <mergeCell ref="AE136:AJ136"/>
+    <mergeCell ref="AK136:AP136"/>
+    <mergeCell ref="AK139:AP139"/>
+    <mergeCell ref="A132:M132"/>
+    <mergeCell ref="A133:M133"/>
+    <mergeCell ref="N132:AD132"/>
+    <mergeCell ref="N133:AD133"/>
+    <mergeCell ref="A130:M130"/>
+    <mergeCell ref="A131:M131"/>
+    <mergeCell ref="N130:AD130"/>
+    <mergeCell ref="N131:AD131"/>
+    <mergeCell ref="A128:M128"/>
+    <mergeCell ref="A129:M129"/>
+    <mergeCell ref="N128:AD128"/>
+    <mergeCell ref="N129:AD129"/>
+    <mergeCell ref="AE128:AJ128"/>
+    <mergeCell ref="AK128:AP128"/>
+    <mergeCell ref="AE129:AJ129"/>
+    <mergeCell ref="AK129:AP129"/>
+    <mergeCell ref="AE130:AJ130"/>
+    <mergeCell ref="AE133:AJ133"/>
+    <mergeCell ref="AK133:AP133"/>
+    <mergeCell ref="AE115:AJ115"/>
+    <mergeCell ref="AK115:AP115"/>
+    <mergeCell ref="AE116:AJ116"/>
+    <mergeCell ref="AK116:AP116"/>
+    <mergeCell ref="AE117:AJ117"/>
+    <mergeCell ref="AK117:AP117"/>
+    <mergeCell ref="AE118:AJ118"/>
+    <mergeCell ref="AK118:AP118"/>
+    <mergeCell ref="AK121:AP121"/>
+    <mergeCell ref="A126:M126"/>
+    <mergeCell ref="A127:M127"/>
+    <mergeCell ref="N126:AD126"/>
+    <mergeCell ref="N127:AD127"/>
+    <mergeCell ref="A124:M124"/>
+    <mergeCell ref="A125:M125"/>
+    <mergeCell ref="N124:AD124"/>
+    <mergeCell ref="N125:AD125"/>
+    <mergeCell ref="A122:M122"/>
+    <mergeCell ref="A123:M123"/>
+    <mergeCell ref="N122:AD122"/>
+    <mergeCell ref="N123:AD123"/>
+    <mergeCell ref="A120:M120"/>
+    <mergeCell ref="A121:M121"/>
+    <mergeCell ref="N120:AD120"/>
+    <mergeCell ref="N121:AD121"/>
+    <mergeCell ref="A118:M118"/>
+    <mergeCell ref="A119:M119"/>
+    <mergeCell ref="N118:AD118"/>
+    <mergeCell ref="N119:AD119"/>
+    <mergeCell ref="A116:M116"/>
+    <mergeCell ref="A117:M117"/>
+    <mergeCell ref="N116:AD116"/>
+    <mergeCell ref="N117:AD117"/>
+    <mergeCell ref="AE119:AJ119"/>
+    <mergeCell ref="AK119:AP119"/>
+    <mergeCell ref="AE120:AJ120"/>
+    <mergeCell ref="AK120:AP120"/>
+    <mergeCell ref="AE121:AJ121"/>
+    <mergeCell ref="A108:M108"/>
+    <mergeCell ref="A109:M109"/>
+    <mergeCell ref="N108:AD108"/>
+    <mergeCell ref="N109:AD109"/>
+    <mergeCell ref="A106:M106"/>
+    <mergeCell ref="A107:M107"/>
+    <mergeCell ref="N106:AD106"/>
+    <mergeCell ref="N107:AD107"/>
+    <mergeCell ref="A104:M104"/>
+    <mergeCell ref="A105:M105"/>
+    <mergeCell ref="N104:AD104"/>
+    <mergeCell ref="N105:AD105"/>
+    <mergeCell ref="A114:M114"/>
+    <mergeCell ref="A115:M115"/>
+    <mergeCell ref="N114:AD114"/>
+    <mergeCell ref="N115:AD115"/>
+    <mergeCell ref="A112:M112"/>
+    <mergeCell ref="A113:M113"/>
+    <mergeCell ref="N112:AD112"/>
+    <mergeCell ref="N113:AD113"/>
+    <mergeCell ref="A110:M110"/>
+    <mergeCell ref="A111:M111"/>
+    <mergeCell ref="N110:AD110"/>
+    <mergeCell ref="N111:AD111"/>
+    <mergeCell ref="AE104:AJ104"/>
+    <mergeCell ref="AK104:AP104"/>
+    <mergeCell ref="A102:M102"/>
+    <mergeCell ref="A103:M103"/>
+    <mergeCell ref="N102:AD102"/>
+    <mergeCell ref="N103:AD103"/>
+    <mergeCell ref="A100:M100"/>
+    <mergeCell ref="A101:M101"/>
+    <mergeCell ref="N100:AD100"/>
+    <mergeCell ref="N101:AD101"/>
+    <mergeCell ref="A98:M98"/>
+    <mergeCell ref="A99:M99"/>
+    <mergeCell ref="N98:AD98"/>
+    <mergeCell ref="N99:AD99"/>
+    <mergeCell ref="AE101:AJ101"/>
+    <mergeCell ref="AK101:AP101"/>
+    <mergeCell ref="AE102:AJ102"/>
+    <mergeCell ref="AK102:AP102"/>
+    <mergeCell ref="AE103:AJ103"/>
+    <mergeCell ref="AE98:AJ98"/>
+    <mergeCell ref="AK98:AP98"/>
+    <mergeCell ref="AE99:AJ99"/>
+    <mergeCell ref="AK99:AP99"/>
+    <mergeCell ref="AE100:AJ100"/>
+    <mergeCell ref="AK100:AP100"/>
+    <mergeCell ref="AK103:AP103"/>
+    <mergeCell ref="A96:M96"/>
+    <mergeCell ref="A97:M97"/>
+    <mergeCell ref="N96:AD96"/>
+    <mergeCell ref="N97:AD97"/>
+    <mergeCell ref="A94:M94"/>
+    <mergeCell ref="A95:M95"/>
+    <mergeCell ref="N94:AD94"/>
+    <mergeCell ref="N95:AD95"/>
+    <mergeCell ref="A92:M92"/>
+    <mergeCell ref="A93:M93"/>
+    <mergeCell ref="N92:AD92"/>
+    <mergeCell ref="N93:AD93"/>
+    <mergeCell ref="AE92:AJ92"/>
+    <mergeCell ref="AK92:AP92"/>
+    <mergeCell ref="AE93:AJ93"/>
+    <mergeCell ref="AK93:AP93"/>
+    <mergeCell ref="AE94:AJ94"/>
+    <mergeCell ref="AE97:AJ97"/>
+    <mergeCell ref="AK97:AP97"/>
+    <mergeCell ref="AE79:AJ79"/>
+    <mergeCell ref="AK79:AP79"/>
+    <mergeCell ref="AE80:AJ80"/>
+    <mergeCell ref="AK80:AP80"/>
+    <mergeCell ref="AE81:AJ81"/>
+    <mergeCell ref="AK81:AP81"/>
+    <mergeCell ref="AE82:AJ82"/>
+    <mergeCell ref="AK82:AP82"/>
+    <mergeCell ref="AK85:AP85"/>
+    <mergeCell ref="A90:M90"/>
+    <mergeCell ref="A91:M91"/>
+    <mergeCell ref="N90:AD90"/>
+    <mergeCell ref="N91:AD91"/>
+    <mergeCell ref="A88:M88"/>
+    <mergeCell ref="A89:M89"/>
+    <mergeCell ref="N88:AD88"/>
+    <mergeCell ref="N89:AD89"/>
+    <mergeCell ref="A86:M86"/>
+    <mergeCell ref="A87:M87"/>
+    <mergeCell ref="N86:AD86"/>
+    <mergeCell ref="N87:AD87"/>
+    <mergeCell ref="A84:M84"/>
+    <mergeCell ref="A85:M85"/>
+    <mergeCell ref="N84:AD84"/>
+    <mergeCell ref="N85:AD85"/>
+    <mergeCell ref="A82:M82"/>
+    <mergeCell ref="A83:M83"/>
+    <mergeCell ref="N82:AD82"/>
+    <mergeCell ref="N83:AD83"/>
+    <mergeCell ref="A80:M80"/>
+    <mergeCell ref="A81:M81"/>
+    <mergeCell ref="N80:AD80"/>
+    <mergeCell ref="N81:AD81"/>
+    <mergeCell ref="AE83:AJ83"/>
+    <mergeCell ref="AK83:AP83"/>
+    <mergeCell ref="AE84:AJ84"/>
+    <mergeCell ref="AK84:AP84"/>
+    <mergeCell ref="AE85:AJ85"/>
+    <mergeCell ref="A72:M72"/>
+    <mergeCell ref="A73:M73"/>
+    <mergeCell ref="N72:AD72"/>
+    <mergeCell ref="N73:AD73"/>
+    <mergeCell ref="A70:M70"/>
+    <mergeCell ref="A71:M71"/>
+    <mergeCell ref="N70:AD70"/>
+    <mergeCell ref="N71:AD71"/>
+    <mergeCell ref="A68:M68"/>
+    <mergeCell ref="A69:M69"/>
+    <mergeCell ref="N68:AD68"/>
+    <mergeCell ref="N69:AD69"/>
+    <mergeCell ref="A78:M78"/>
+    <mergeCell ref="A79:M79"/>
+    <mergeCell ref="N78:AD78"/>
+    <mergeCell ref="N79:AD79"/>
+    <mergeCell ref="A76:M76"/>
+    <mergeCell ref="A77:M77"/>
+    <mergeCell ref="N76:AD76"/>
+    <mergeCell ref="N77:AD77"/>
+    <mergeCell ref="A74:M74"/>
+    <mergeCell ref="A75:M75"/>
+    <mergeCell ref="N74:AD74"/>
+    <mergeCell ref="N75:AD75"/>
+    <mergeCell ref="AE68:AJ68"/>
+    <mergeCell ref="AK68:AP68"/>
+    <mergeCell ref="A66:M66"/>
+    <mergeCell ref="A67:M67"/>
+    <mergeCell ref="N66:AD66"/>
+    <mergeCell ref="N67:AD67"/>
+    <mergeCell ref="A64:M64"/>
+    <mergeCell ref="A65:M65"/>
+    <mergeCell ref="N64:AD64"/>
+    <mergeCell ref="N65:AD65"/>
+    <mergeCell ref="A62:M62"/>
+    <mergeCell ref="A63:M63"/>
+    <mergeCell ref="N62:AD62"/>
+    <mergeCell ref="N63:AD63"/>
+    <mergeCell ref="AE65:AJ65"/>
+    <mergeCell ref="AK65:AP65"/>
+    <mergeCell ref="AE66:AJ66"/>
+    <mergeCell ref="AK66:AP66"/>
+    <mergeCell ref="AE67:AJ67"/>
+    <mergeCell ref="AE62:AJ62"/>
+    <mergeCell ref="AK62:AP62"/>
+    <mergeCell ref="AE63:AJ63"/>
+    <mergeCell ref="AK63:AP63"/>
+    <mergeCell ref="AE64:AJ64"/>
+    <mergeCell ref="AK64:AP64"/>
+    <mergeCell ref="AK67:AP67"/>
+    <mergeCell ref="A60:M60"/>
+    <mergeCell ref="A61:M61"/>
+    <mergeCell ref="N60:AD60"/>
+    <mergeCell ref="N61:AD61"/>
+    <mergeCell ref="A58:M58"/>
+    <mergeCell ref="A59:M59"/>
+    <mergeCell ref="N58:AD58"/>
+    <mergeCell ref="N59:AD59"/>
+    <mergeCell ref="A56:M56"/>
+    <mergeCell ref="A57:M57"/>
+    <mergeCell ref="N56:AD56"/>
+    <mergeCell ref="N57:AD57"/>
+    <mergeCell ref="AE56:AJ56"/>
+    <mergeCell ref="AK56:AP56"/>
+    <mergeCell ref="AE57:AJ57"/>
+    <mergeCell ref="AK57:AP57"/>
+    <mergeCell ref="AE58:AJ58"/>
+    <mergeCell ref="AE61:AJ61"/>
+    <mergeCell ref="AK61:AP61"/>
+    <mergeCell ref="AE43:AJ43"/>
+    <mergeCell ref="AK43:AP43"/>
+    <mergeCell ref="AE44:AJ44"/>
+    <mergeCell ref="AK44:AP44"/>
+    <mergeCell ref="AE45:AJ45"/>
+    <mergeCell ref="AK45:AP45"/>
+    <mergeCell ref="AE46:AJ46"/>
+    <mergeCell ref="AK46:AP46"/>
+    <mergeCell ref="AK49:AP49"/>
+    <mergeCell ref="A54:M54"/>
+    <mergeCell ref="A55:M55"/>
+    <mergeCell ref="N54:AD54"/>
+    <mergeCell ref="N55:AD55"/>
+    <mergeCell ref="A52:M52"/>
+    <mergeCell ref="A53:M53"/>
+    <mergeCell ref="N52:AD52"/>
+    <mergeCell ref="N53:AD53"/>
+    <mergeCell ref="A50:M50"/>
+    <mergeCell ref="A51:M51"/>
+    <mergeCell ref="N50:AD50"/>
+    <mergeCell ref="N51:AD51"/>
+    <mergeCell ref="A48:M48"/>
+    <mergeCell ref="A49:M49"/>
+    <mergeCell ref="N48:AD48"/>
+    <mergeCell ref="N49:AD49"/>
+    <mergeCell ref="A46:M46"/>
+    <mergeCell ref="A47:M47"/>
+    <mergeCell ref="N46:AD46"/>
+    <mergeCell ref="N47:AD47"/>
+    <mergeCell ref="A44:M44"/>
+    <mergeCell ref="A45:M45"/>
+    <mergeCell ref="N44:AD44"/>
+    <mergeCell ref="N45:AD45"/>
+    <mergeCell ref="AE47:AJ47"/>
+    <mergeCell ref="AK47:AP47"/>
+    <mergeCell ref="AE48:AJ48"/>
+    <mergeCell ref="AK48:AP48"/>
+    <mergeCell ref="AE49:AJ49"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="A37:M37"/>
+    <mergeCell ref="N36:AD36"/>
+    <mergeCell ref="N37:AD37"/>
+    <mergeCell ref="A34:M34"/>
+    <mergeCell ref="A35:M35"/>
+    <mergeCell ref="N34:AD34"/>
+    <mergeCell ref="N35:AD35"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="N32:AD32"/>
+    <mergeCell ref="N33:AD33"/>
+    <mergeCell ref="A42:M42"/>
+    <mergeCell ref="A43:M43"/>
+    <mergeCell ref="N42:AD42"/>
+    <mergeCell ref="N43:AD43"/>
+    <mergeCell ref="A40:M40"/>
+    <mergeCell ref="A41:M41"/>
+    <mergeCell ref="N40:AD40"/>
+    <mergeCell ref="N41:AD41"/>
+    <mergeCell ref="A38:M38"/>
+    <mergeCell ref="A39:M39"/>
+    <mergeCell ref="N38:AD38"/>
+    <mergeCell ref="N39:AD39"/>
+    <mergeCell ref="AE32:AJ32"/>
+    <mergeCell ref="AK32:AP32"/>
+    <mergeCell ref="A30:M30"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="N30:AD30"/>
+    <mergeCell ref="N31:AD31"/>
+    <mergeCell ref="A28:M28"/>
+    <mergeCell ref="A29:M29"/>
+    <mergeCell ref="N28:AD28"/>
+    <mergeCell ref="N29:AD29"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="N26:AD26"/>
+    <mergeCell ref="N27:AD27"/>
+    <mergeCell ref="AE29:AJ29"/>
+    <mergeCell ref="AK29:AP29"/>
+    <mergeCell ref="AE30:AJ30"/>
+    <mergeCell ref="AK30:AP30"/>
+    <mergeCell ref="AE31:AJ31"/>
+    <mergeCell ref="AE26:AJ26"/>
+    <mergeCell ref="AK26:AP26"/>
+    <mergeCell ref="AE27:AJ27"/>
+    <mergeCell ref="AK27:AP27"/>
+    <mergeCell ref="AE28:AJ28"/>
+    <mergeCell ref="AK28:AP28"/>
+    <mergeCell ref="AK31:AP31"/>
+    <mergeCell ref="A1:AP8"/>
+    <mergeCell ref="A9:AO9"/>
+    <mergeCell ref="B10:AN12"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="N24:AD24"/>
+    <mergeCell ref="N25:AD25"/>
+    <mergeCell ref="A22:M22"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="N22:AD22"/>
+    <mergeCell ref="N23:AD23"/>
+    <mergeCell ref="A20:M20"/>
+    <mergeCell ref="A21:M21"/>
+    <mergeCell ref="N20:AD20"/>
+    <mergeCell ref="N21:AD21"/>
+    <mergeCell ref="AE20:AJ20"/>
+    <mergeCell ref="AK20:AP20"/>
+    <mergeCell ref="AE21:AJ21"/>
+    <mergeCell ref="AK21:AP21"/>
+    <mergeCell ref="AE22:AJ22"/>
+    <mergeCell ref="AK22:AP22"/>
+    <mergeCell ref="AE23:AJ23"/>
+    <mergeCell ref="AK23:AP23"/>
+    <mergeCell ref="AE24:AJ24"/>
+    <mergeCell ref="AK24:AP24"/>
+    <mergeCell ref="AE25:AJ25"/>
+    <mergeCell ref="AK25:AP25"/>
+    <mergeCell ref="N13:AD13"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="AE13:AJ13"/>
+    <mergeCell ref="AK13:AP13"/>
+    <mergeCell ref="AE14:AJ14"/>
+    <mergeCell ref="AK14:AP14"/>
+    <mergeCell ref="AE15:AJ15"/>
+    <mergeCell ref="AK15:AP15"/>
+    <mergeCell ref="AE16:AJ16"/>
+    <mergeCell ref="AK16:AP16"/>
+    <mergeCell ref="A18:M18"/>
+    <mergeCell ref="A19:M19"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="A17:M17"/>
+    <mergeCell ref="A14:M14"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="AE17:AJ17"/>
+    <mergeCell ref="AK17:AP17"/>
+    <mergeCell ref="AE18:AJ18"/>
+    <mergeCell ref="AK18:AP18"/>
+    <mergeCell ref="AE19:AJ19"/>
+    <mergeCell ref="AK19:AP19"/>
+    <mergeCell ref="AE33:AJ33"/>
+    <mergeCell ref="AK33:AP33"/>
+    <mergeCell ref="AE34:AJ34"/>
+    <mergeCell ref="AK34:AP34"/>
+    <mergeCell ref="AE35:AJ35"/>
+    <mergeCell ref="AK35:AP35"/>
+    <mergeCell ref="AE36:AJ36"/>
+    <mergeCell ref="AK36:AP36"/>
+    <mergeCell ref="AE37:AJ37"/>
+    <mergeCell ref="AK37:AP37"/>
+    <mergeCell ref="AK40:AP40"/>
+    <mergeCell ref="AE41:AJ41"/>
+    <mergeCell ref="AK41:AP41"/>
+    <mergeCell ref="AE42:AJ42"/>
+    <mergeCell ref="AK42:AP42"/>
+    <mergeCell ref="AE38:AJ38"/>
+    <mergeCell ref="AK38:AP38"/>
+    <mergeCell ref="AE39:AJ39"/>
+    <mergeCell ref="AK39:AP39"/>
+    <mergeCell ref="AE40:AJ40"/>
+    <mergeCell ref="AE50:AJ50"/>
+    <mergeCell ref="AK50:AP50"/>
+    <mergeCell ref="AE51:AJ51"/>
+    <mergeCell ref="AK51:AP51"/>
+    <mergeCell ref="AE52:AJ52"/>
+    <mergeCell ref="AK52:AP52"/>
+    <mergeCell ref="AE53:AJ53"/>
+    <mergeCell ref="AK53:AP53"/>
+    <mergeCell ref="AE54:AJ54"/>
+    <mergeCell ref="AK54:AP54"/>
+    <mergeCell ref="AE55:AJ55"/>
+    <mergeCell ref="AK55:AP55"/>
+    <mergeCell ref="AK58:AP58"/>
+    <mergeCell ref="AE59:AJ59"/>
+    <mergeCell ref="AK59:AP59"/>
+    <mergeCell ref="AE60:AJ60"/>
+    <mergeCell ref="AK60:AP60"/>
+    <mergeCell ref="AE69:AJ69"/>
+    <mergeCell ref="AK69:AP69"/>
+    <mergeCell ref="AE70:AJ70"/>
+    <mergeCell ref="AK70:AP70"/>
+    <mergeCell ref="AE71:AJ71"/>
+    <mergeCell ref="AK71:AP71"/>
+    <mergeCell ref="AE72:AJ72"/>
+    <mergeCell ref="AK72:AP72"/>
+    <mergeCell ref="AE73:AJ73"/>
+    <mergeCell ref="AK73:AP73"/>
+    <mergeCell ref="AK76:AP76"/>
+    <mergeCell ref="AE77:AJ77"/>
+    <mergeCell ref="AK77:AP77"/>
+    <mergeCell ref="AE78:AJ78"/>
+    <mergeCell ref="AK78:AP78"/>
+    <mergeCell ref="AE74:AJ74"/>
+    <mergeCell ref="AK74:AP74"/>
+    <mergeCell ref="AE75:AJ75"/>
+    <mergeCell ref="AK75:AP75"/>
+    <mergeCell ref="AE76:AJ76"/>
+    <mergeCell ref="AE86:AJ86"/>
+    <mergeCell ref="AK86:AP86"/>
+    <mergeCell ref="AE87:AJ87"/>
+    <mergeCell ref="AK87:AP87"/>
+    <mergeCell ref="AE88:AJ88"/>
+    <mergeCell ref="AK88:AP88"/>
+    <mergeCell ref="AE89:AJ89"/>
+    <mergeCell ref="AK89:AP89"/>
+    <mergeCell ref="AE90:AJ90"/>
+    <mergeCell ref="AK90:AP90"/>
+    <mergeCell ref="AE91:AJ91"/>
+    <mergeCell ref="AK91:AP91"/>
+    <mergeCell ref="AK94:AP94"/>
+    <mergeCell ref="AE95:AJ95"/>
+    <mergeCell ref="AK95:AP95"/>
+    <mergeCell ref="AE96:AJ96"/>
+    <mergeCell ref="AK96:AP96"/>
+    <mergeCell ref="AE105:AJ105"/>
+    <mergeCell ref="AK105:AP105"/>
+    <mergeCell ref="AE106:AJ106"/>
+    <mergeCell ref="AK106:AP106"/>
+    <mergeCell ref="AE107:AJ107"/>
+    <mergeCell ref="AK107:AP107"/>
+    <mergeCell ref="AE108:AJ108"/>
+    <mergeCell ref="AK108:AP108"/>
+    <mergeCell ref="AE109:AJ109"/>
+    <mergeCell ref="AK109:AP109"/>
+    <mergeCell ref="AK112:AP112"/>
+    <mergeCell ref="AE113:AJ113"/>
+    <mergeCell ref="AK113:AP113"/>
+    <mergeCell ref="AE114:AJ114"/>
+    <mergeCell ref="AK114:AP114"/>
+    <mergeCell ref="AE110:AJ110"/>
+    <mergeCell ref="AK110:AP110"/>
+    <mergeCell ref="AE111:AJ111"/>
+    <mergeCell ref="AK111:AP111"/>
+    <mergeCell ref="AE112:AJ112"/>
+    <mergeCell ref="AE122:AJ122"/>
+    <mergeCell ref="AK122:AP122"/>
+    <mergeCell ref="AE123:AJ123"/>
+    <mergeCell ref="AK123:AP123"/>
+    <mergeCell ref="AE124:AJ124"/>
+    <mergeCell ref="AK124:AP124"/>
+    <mergeCell ref="AE125:AJ125"/>
+    <mergeCell ref="AK125:AP125"/>
+    <mergeCell ref="AE126:AJ126"/>
+    <mergeCell ref="AK126:AP126"/>
+    <mergeCell ref="AE127:AJ127"/>
+    <mergeCell ref="AK127:AP127"/>
+    <mergeCell ref="AK130:AP130"/>
+    <mergeCell ref="AE131:AJ131"/>
+    <mergeCell ref="AK131:AP131"/>
+    <mergeCell ref="AE132:AJ132"/>
+    <mergeCell ref="AK132:AP132"/>
+    <mergeCell ref="AE141:AJ141"/>
+    <mergeCell ref="AK141:AP141"/>
+    <mergeCell ref="AE142:AJ142"/>
+    <mergeCell ref="AK142:AP142"/>
+    <mergeCell ref="AE143:AJ143"/>
+    <mergeCell ref="AK143:AP143"/>
+    <mergeCell ref="AE144:AJ144"/>
+    <mergeCell ref="AK144:AP144"/>
+    <mergeCell ref="AE145:AJ145"/>
+    <mergeCell ref="AK145:AP145"/>
+    <mergeCell ref="AK148:AP148"/>
+    <mergeCell ref="AE149:AJ149"/>
+    <mergeCell ref="AK149:AP149"/>
+    <mergeCell ref="AE150:AJ150"/>
+    <mergeCell ref="AK150:AP150"/>
+    <mergeCell ref="AE146:AJ146"/>
+    <mergeCell ref="AK146:AP146"/>
+    <mergeCell ref="AE147:AJ147"/>
+    <mergeCell ref="AK147:AP147"/>
+    <mergeCell ref="AE148:AJ148"/>
+    <mergeCell ref="AE158:AJ158"/>
+    <mergeCell ref="AK158:AP158"/>
+    <mergeCell ref="AE159:AJ159"/>
+    <mergeCell ref="AK159:AP159"/>
+    <mergeCell ref="AE160:AJ160"/>
+    <mergeCell ref="AK160:AP160"/>
+    <mergeCell ref="AE161:AJ161"/>
+    <mergeCell ref="AK161:AP161"/>
+    <mergeCell ref="AE162:AJ162"/>
+    <mergeCell ref="AK162:AP162"/>
+    <mergeCell ref="AE163:AJ163"/>
+    <mergeCell ref="AK163:AP163"/>
+    <mergeCell ref="AK166:AP166"/>
+    <mergeCell ref="AE167:AJ167"/>
+    <mergeCell ref="AK167:AP167"/>
+    <mergeCell ref="AE168:AJ168"/>
+    <mergeCell ref="AK168:AP168"/>
+    <mergeCell ref="AE177:AJ177"/>
+    <mergeCell ref="AK177:AP177"/>
+    <mergeCell ref="AE178:AJ178"/>
+    <mergeCell ref="AK178:AP178"/>
+    <mergeCell ref="AE179:AJ179"/>
+    <mergeCell ref="AK179:AP179"/>
+    <mergeCell ref="AE180:AJ180"/>
+    <mergeCell ref="AK180:AP180"/>
+    <mergeCell ref="AE181:AJ181"/>
+    <mergeCell ref="AK181:AP181"/>
+    <mergeCell ref="AK184:AP184"/>
+    <mergeCell ref="AE185:AJ185"/>
+    <mergeCell ref="AK185:AP185"/>
+    <mergeCell ref="AE186:AJ186"/>
+    <mergeCell ref="AK186:AP186"/>
+    <mergeCell ref="AE182:AJ182"/>
+    <mergeCell ref="AK182:AP182"/>
+    <mergeCell ref="AE183:AJ183"/>
+    <mergeCell ref="AK183:AP183"/>
+    <mergeCell ref="AE184:AJ184"/>
+    <mergeCell ref="AE194:AJ194"/>
+    <mergeCell ref="AK194:AP194"/>
+    <mergeCell ref="AE195:AJ195"/>
+    <mergeCell ref="AK195:AP195"/>
+    <mergeCell ref="AE196:AJ196"/>
+    <mergeCell ref="AK196:AP196"/>
+    <mergeCell ref="AE197:AJ197"/>
+    <mergeCell ref="AK197:AP197"/>
+    <mergeCell ref="AE198:AJ198"/>
+    <mergeCell ref="AK198:AP198"/>
+    <mergeCell ref="AE199:AJ199"/>
+    <mergeCell ref="AK199:AP199"/>
+    <mergeCell ref="AK202:AP202"/>
+    <mergeCell ref="AE203:AJ203"/>
+    <mergeCell ref="AK203:AP203"/>
+    <mergeCell ref="AE204:AJ204"/>
+    <mergeCell ref="AK204:AP204"/>
+    <mergeCell ref="AE213:AJ213"/>
+    <mergeCell ref="AK213:AP213"/>
+    <mergeCell ref="AE214:AJ214"/>
+    <mergeCell ref="AK214:AP214"/>
+    <mergeCell ref="AE215:AJ215"/>
+    <mergeCell ref="AK215:AP215"/>
+    <mergeCell ref="AE216:AJ216"/>
+    <mergeCell ref="AK216:AP216"/>
+    <mergeCell ref="AE217:AJ217"/>
+    <mergeCell ref="AK217:AP217"/>
+    <mergeCell ref="AK220:AP220"/>
+    <mergeCell ref="AE221:AJ221"/>
+    <mergeCell ref="AK221:AP221"/>
+    <mergeCell ref="AE222:AJ222"/>
+    <mergeCell ref="AK222:AP222"/>
+    <mergeCell ref="AE218:AJ218"/>
+    <mergeCell ref="AK218:AP218"/>
+    <mergeCell ref="AE219:AJ219"/>
+    <mergeCell ref="AK219:AP219"/>
+    <mergeCell ref="AE220:AJ220"/>
+    <mergeCell ref="AE230:AJ230"/>
+    <mergeCell ref="AK230:AP230"/>
+    <mergeCell ref="AE231:AJ231"/>
+    <mergeCell ref="AK231:AP231"/>
+    <mergeCell ref="AE232:AJ232"/>
+    <mergeCell ref="AK232:AP232"/>
+    <mergeCell ref="AE233:AJ233"/>
+    <mergeCell ref="AK233:AP233"/>
+    <mergeCell ref="AE234:AJ234"/>
+    <mergeCell ref="AK234:AP234"/>
+    <mergeCell ref="AE235:AJ235"/>
+    <mergeCell ref="AK235:AP235"/>
+    <mergeCell ref="AK238:AP238"/>
+    <mergeCell ref="AE239:AJ239"/>
+    <mergeCell ref="AK239:AP239"/>
+    <mergeCell ref="AE240:AJ240"/>
+    <mergeCell ref="AK240:AP240"/>
+    <mergeCell ref="AE249:AJ249"/>
+    <mergeCell ref="AK249:AP249"/>
+    <mergeCell ref="AE250:AJ250"/>
+    <mergeCell ref="AK250:AP250"/>
+    <mergeCell ref="AE251:AJ251"/>
+    <mergeCell ref="AK251:AP251"/>
+    <mergeCell ref="AE252:AJ252"/>
+    <mergeCell ref="AK252:AP252"/>
+    <mergeCell ref="AE253:AJ253"/>
+    <mergeCell ref="AK253:AP253"/>
+    <mergeCell ref="AK256:AP256"/>
+    <mergeCell ref="AE257:AJ257"/>
+    <mergeCell ref="AK257:AP257"/>
+    <mergeCell ref="AE258:AJ258"/>
+    <mergeCell ref="AK258:AP258"/>
+    <mergeCell ref="AE254:AJ254"/>
+    <mergeCell ref="AK254:AP254"/>
+    <mergeCell ref="AE255:AJ255"/>
+    <mergeCell ref="AK255:AP255"/>
+    <mergeCell ref="AE256:AJ256"/>
+    <mergeCell ref="AE266:AJ266"/>
+    <mergeCell ref="AK266:AP266"/>
+    <mergeCell ref="AE267:AJ267"/>
+    <mergeCell ref="AK267:AP267"/>
+    <mergeCell ref="AE268:AJ268"/>
+    <mergeCell ref="AK268:AP268"/>
+    <mergeCell ref="AE269:AJ269"/>
+    <mergeCell ref="AK269:AP269"/>
+    <mergeCell ref="AE270:AJ270"/>
+    <mergeCell ref="AK270:AP270"/>
+    <mergeCell ref="AE271:AJ271"/>
+    <mergeCell ref="AK271:AP271"/>
+    <mergeCell ref="AK274:AP274"/>
+    <mergeCell ref="AE275:AJ275"/>
+    <mergeCell ref="AK275:AP275"/>
+    <mergeCell ref="AE276:AJ276"/>
+    <mergeCell ref="AK276:AP276"/>
+    <mergeCell ref="AE285:AJ285"/>
+    <mergeCell ref="AK285:AP285"/>
+    <mergeCell ref="AE286:AJ286"/>
+    <mergeCell ref="AK286:AP286"/>
+    <mergeCell ref="AE287:AJ287"/>
+    <mergeCell ref="AK287:AP287"/>
+    <mergeCell ref="AE288:AJ288"/>
+    <mergeCell ref="AK288:AP288"/>
+    <mergeCell ref="AE289:AJ289"/>
+    <mergeCell ref="AK289:AP289"/>
+    <mergeCell ref="AK292:AP292"/>
+    <mergeCell ref="AE293:AJ293"/>
+    <mergeCell ref="AK293:AP293"/>
+    <mergeCell ref="AE294:AJ294"/>
+    <mergeCell ref="AK294:AP294"/>
+    <mergeCell ref="AE290:AJ290"/>
+    <mergeCell ref="AK290:AP290"/>
+    <mergeCell ref="AE291:AJ291"/>
+    <mergeCell ref="AK291:AP291"/>
+    <mergeCell ref="AE292:AJ292"/>
+    <mergeCell ref="AE302:AJ302"/>
+    <mergeCell ref="AK302:AP302"/>
+    <mergeCell ref="AE303:AJ303"/>
+    <mergeCell ref="AK303:AP303"/>
+    <mergeCell ref="AE304:AJ304"/>
+    <mergeCell ref="AK304:AP304"/>
+    <mergeCell ref="AE305:AJ305"/>
+    <mergeCell ref="AK305:AP305"/>
+    <mergeCell ref="AE306:AJ306"/>
+    <mergeCell ref="AK306:AP306"/>
+    <mergeCell ref="AE307:AJ307"/>
+    <mergeCell ref="AK307:AP307"/>
+    <mergeCell ref="AK310:AP310"/>
+    <mergeCell ref="AE311:AJ311"/>
+    <mergeCell ref="AK311:AP311"/>
+    <mergeCell ref="AE312:AJ312"/>
+    <mergeCell ref="AK312:AP312"/>
+    <mergeCell ref="AE321:AJ321"/>
+    <mergeCell ref="AK321:AP321"/>
+    <mergeCell ref="AE322:AJ322"/>
+    <mergeCell ref="AK322:AP322"/>
+    <mergeCell ref="AE323:AJ323"/>
+    <mergeCell ref="AK323:AP323"/>
+    <mergeCell ref="AE324:AJ324"/>
+    <mergeCell ref="AK324:AP324"/>
+    <mergeCell ref="AE325:AJ325"/>
+    <mergeCell ref="AK325:AP325"/>
+    <mergeCell ref="AK328:AP328"/>
+    <mergeCell ref="AE329:AJ329"/>
+    <mergeCell ref="AK329:AP329"/>
+    <mergeCell ref="AE330:AJ330"/>
+    <mergeCell ref="AK330:AP330"/>
+    <mergeCell ref="AE326:AJ326"/>
+    <mergeCell ref="AK326:AP326"/>
+    <mergeCell ref="AE327:AJ327"/>
+    <mergeCell ref="AK327:AP327"/>
+    <mergeCell ref="AE328:AJ328"/>
+    <mergeCell ref="AE338:AJ338"/>
+    <mergeCell ref="AK338:AP338"/>
+    <mergeCell ref="AE339:AJ339"/>
+    <mergeCell ref="AK339:AP339"/>
+    <mergeCell ref="AE340:AJ340"/>
+    <mergeCell ref="AK340:AP340"/>
+    <mergeCell ref="AE341:AJ341"/>
+    <mergeCell ref="AK341:AP341"/>
+    <mergeCell ref="AE342:AJ342"/>
+    <mergeCell ref="AK342:AP342"/>
+    <mergeCell ref="AE343:AJ343"/>
+    <mergeCell ref="AK343:AP343"/>
+    <mergeCell ref="AK346:AP346"/>
+    <mergeCell ref="AE347:AJ347"/>
+    <mergeCell ref="AK347:AP347"/>
+    <mergeCell ref="AE348:AJ348"/>
+    <mergeCell ref="AK348:AP348"/>
+    <mergeCell ref="AE357:AJ357"/>
+    <mergeCell ref="AK357:AP357"/>
+    <mergeCell ref="AE358:AJ358"/>
+    <mergeCell ref="AK358:AP358"/>
+    <mergeCell ref="AE359:AJ359"/>
+    <mergeCell ref="AK359:AP359"/>
+    <mergeCell ref="AE360:AJ360"/>
+    <mergeCell ref="AK360:AP360"/>
+    <mergeCell ref="AE361:AJ361"/>
+    <mergeCell ref="AK361:AP361"/>
+    <mergeCell ref="AK364:AP364"/>
+    <mergeCell ref="AE365:AJ365"/>
+    <mergeCell ref="AK365:AP365"/>
+    <mergeCell ref="AE366:AJ366"/>
+    <mergeCell ref="AK366:AP366"/>
+    <mergeCell ref="AE362:AJ362"/>
+    <mergeCell ref="AK362:AP362"/>
+    <mergeCell ref="AE363:AJ363"/>
+    <mergeCell ref="AK363:AP363"/>
+    <mergeCell ref="AE364:AJ364"/>
+    <mergeCell ref="AE374:AJ374"/>
+    <mergeCell ref="AK374:AP374"/>
+    <mergeCell ref="AE375:AJ375"/>
+    <mergeCell ref="AK375:AP375"/>
+    <mergeCell ref="AE376:AJ376"/>
+    <mergeCell ref="AK376:AP376"/>
+    <mergeCell ref="AE377:AJ377"/>
+    <mergeCell ref="AK377:AP377"/>
+    <mergeCell ref="AE378:AJ378"/>
+    <mergeCell ref="AK378:AP378"/>
+    <mergeCell ref="AE379:AJ379"/>
+    <mergeCell ref="AK379:AP379"/>
+    <mergeCell ref="AK382:AP382"/>
+    <mergeCell ref="AE383:AJ383"/>
+    <mergeCell ref="AK383:AP383"/>
+    <mergeCell ref="AE384:AJ384"/>
+    <mergeCell ref="AK384:AP384"/>
+    <mergeCell ref="AE393:AJ393"/>
+    <mergeCell ref="AK393:AP393"/>
+    <mergeCell ref="AE394:AJ394"/>
+    <mergeCell ref="AK394:AP394"/>
+    <mergeCell ref="AE395:AJ395"/>
+    <mergeCell ref="AK395:AP395"/>
+    <mergeCell ref="AE396:AJ396"/>
+    <mergeCell ref="AK396:AP396"/>
+    <mergeCell ref="AE397:AJ397"/>
+    <mergeCell ref="AK397:AP397"/>
+    <mergeCell ref="AK400:AP400"/>
+    <mergeCell ref="AE401:AJ401"/>
+    <mergeCell ref="AK401:AP401"/>
+    <mergeCell ref="AE402:AJ402"/>
+    <mergeCell ref="AK402:AP402"/>
+    <mergeCell ref="AE398:AJ398"/>
+    <mergeCell ref="AK398:AP398"/>
+    <mergeCell ref="AE399:AJ399"/>
+    <mergeCell ref="AK399:AP399"/>
+    <mergeCell ref="AE400:AJ400"/>
+    <mergeCell ref="AE410:AJ410"/>
+    <mergeCell ref="AK410:AP410"/>
+    <mergeCell ref="AE411:AJ411"/>
+    <mergeCell ref="AK411:AP411"/>
+    <mergeCell ref="AE412:AJ412"/>
+    <mergeCell ref="AK412:AP412"/>
+    <mergeCell ref="AE413:AJ413"/>
+    <mergeCell ref="AK413:AP413"/>
+    <mergeCell ref="AE414:AJ414"/>
+    <mergeCell ref="AK414:AP414"/>
+    <mergeCell ref="AE415:AJ415"/>
+    <mergeCell ref="AK415:AP415"/>
+    <mergeCell ref="AK418:AP418"/>
+    <mergeCell ref="AE419:AJ419"/>
+    <mergeCell ref="AK419:AP419"/>
+    <mergeCell ref="AE420:AJ420"/>
+    <mergeCell ref="AK420:AP420"/>
+    <mergeCell ref="AE429:AJ429"/>
+    <mergeCell ref="AK429:AP429"/>
+    <mergeCell ref="AE430:AJ430"/>
+    <mergeCell ref="AK430:AP430"/>
+    <mergeCell ref="AE431:AJ431"/>
+    <mergeCell ref="AK431:AP431"/>
+    <mergeCell ref="AE432:AJ432"/>
+    <mergeCell ref="AK432:AP432"/>
+    <mergeCell ref="AE433:AJ433"/>
+    <mergeCell ref="AK433:AP433"/>
+    <mergeCell ref="AK436:AP436"/>
+    <mergeCell ref="AE437:AJ437"/>
+    <mergeCell ref="AK437:AP437"/>
+    <mergeCell ref="AE438:AJ438"/>
+    <mergeCell ref="AK438:AP438"/>
+    <mergeCell ref="AE434:AJ434"/>
+    <mergeCell ref="AK434:AP434"/>
+    <mergeCell ref="AE435:AJ435"/>
+    <mergeCell ref="AK435:AP435"/>
+    <mergeCell ref="AE436:AJ436"/>
+    <mergeCell ref="AE446:AJ446"/>
+    <mergeCell ref="AK446:AP446"/>
+    <mergeCell ref="AE447:AJ447"/>
+    <mergeCell ref="AK447:AP447"/>
+    <mergeCell ref="AE448:AJ448"/>
+    <mergeCell ref="AK448:AP448"/>
+    <mergeCell ref="AE449:AJ449"/>
+    <mergeCell ref="AK449:AP449"/>
+    <mergeCell ref="AE450:AJ450"/>
+    <mergeCell ref="AK450:AP450"/>
+    <mergeCell ref="AE451:AJ451"/>
+    <mergeCell ref="AK451:AP451"/>
+    <mergeCell ref="AK454:AP454"/>
+    <mergeCell ref="AE455:AJ455"/>
+    <mergeCell ref="AK455:AP455"/>
+    <mergeCell ref="AE456:AJ456"/>
+    <mergeCell ref="AK456:AP456"/>
+    <mergeCell ref="AE465:AJ465"/>
+    <mergeCell ref="AK465:AP465"/>
+    <mergeCell ref="AE466:AJ466"/>
+    <mergeCell ref="AK466:AP466"/>
+    <mergeCell ref="AE467:AJ467"/>
+    <mergeCell ref="AK467:AP467"/>
+    <mergeCell ref="AE468:AJ468"/>
+    <mergeCell ref="AK468:AP468"/>
+    <mergeCell ref="AE469:AJ469"/>
+    <mergeCell ref="AK469:AP469"/>
+    <mergeCell ref="AK472:AP472"/>
+    <mergeCell ref="AE473:AJ473"/>
+    <mergeCell ref="AK473:AP473"/>
+    <mergeCell ref="AE474:AJ474"/>
+    <mergeCell ref="AK474:AP474"/>
+    <mergeCell ref="AE470:AJ470"/>
+    <mergeCell ref="AK470:AP470"/>
+    <mergeCell ref="AE471:AJ471"/>
+    <mergeCell ref="AK471:AP471"/>
+    <mergeCell ref="AE472:AJ472"/>
+    <mergeCell ref="AE482:AJ482"/>
+    <mergeCell ref="AK482:AP482"/>
+    <mergeCell ref="AE483:AJ483"/>
+    <mergeCell ref="AK483:AP483"/>
+    <mergeCell ref="AE484:AJ484"/>
+    <mergeCell ref="AK484:AP484"/>
+    <mergeCell ref="AE485:AJ485"/>
+    <mergeCell ref="AK485:AP485"/>
+    <mergeCell ref="AE486:AJ486"/>
+    <mergeCell ref="AK486:AP486"/>
+    <mergeCell ref="AE487:AJ487"/>
+    <mergeCell ref="AK487:AP487"/>
+    <mergeCell ref="AK490:AP490"/>
+    <mergeCell ref="AE491:AJ491"/>
+    <mergeCell ref="AK491:AP491"/>
+    <mergeCell ref="AE492:AJ492"/>
+    <mergeCell ref="AK492:AP492"/>
+    <mergeCell ref="AE501:AJ501"/>
+    <mergeCell ref="AK501:AP501"/>
+    <mergeCell ref="AE502:AJ502"/>
+    <mergeCell ref="AK502:AP502"/>
+    <mergeCell ref="AE503:AJ503"/>
+    <mergeCell ref="AK503:AP503"/>
+    <mergeCell ref="AE504:AJ504"/>
+    <mergeCell ref="AK504:AP504"/>
+    <mergeCell ref="AE505:AJ505"/>
+    <mergeCell ref="AK505:AP505"/>
+    <mergeCell ref="AK508:AP508"/>
+    <mergeCell ref="AE509:AJ509"/>
+    <mergeCell ref="AK509:AP509"/>
+    <mergeCell ref="AE510:AJ510"/>
+    <mergeCell ref="AK510:AP510"/>
+    <mergeCell ref="AE506:AJ506"/>
+    <mergeCell ref="AK506:AP506"/>
+    <mergeCell ref="AE507:AJ507"/>
+    <mergeCell ref="AK507:AP507"/>
+    <mergeCell ref="AE508:AJ508"/>
+    <mergeCell ref="AE518:AJ518"/>
+    <mergeCell ref="AK518:AP518"/>
+    <mergeCell ref="AE519:AJ519"/>
+    <mergeCell ref="AK519:AP519"/>
+    <mergeCell ref="AE520:AJ520"/>
+    <mergeCell ref="AK520:AP520"/>
+    <mergeCell ref="AE521:AJ521"/>
+    <mergeCell ref="AK521:AP521"/>
+    <mergeCell ref="AE522:AJ522"/>
+    <mergeCell ref="AK522:AP522"/>
+    <mergeCell ref="AE523:AJ523"/>
+    <mergeCell ref="AK523:AP523"/>
+    <mergeCell ref="AK526:AP526"/>
+    <mergeCell ref="AE527:AJ527"/>
+    <mergeCell ref="AK527:AP527"/>
+    <mergeCell ref="AE528:AJ528"/>
+    <mergeCell ref="AK528:AP528"/>
+    <mergeCell ref="AE537:AJ537"/>
+    <mergeCell ref="AK537:AP537"/>
+    <mergeCell ref="AE538:AJ538"/>
+    <mergeCell ref="AK538:AP538"/>
+    <mergeCell ref="AE539:AJ539"/>
+    <mergeCell ref="AK539:AP539"/>
+    <mergeCell ref="AE540:AJ540"/>
+    <mergeCell ref="AK540:AP540"/>
+    <mergeCell ref="AE541:AJ541"/>
+    <mergeCell ref="AK541:AP541"/>
+    <mergeCell ref="AK544:AP544"/>
+    <mergeCell ref="AE545:AJ545"/>
+    <mergeCell ref="AK545:AP545"/>
+    <mergeCell ref="AE546:AJ546"/>
+    <mergeCell ref="AK546:AP546"/>
+    <mergeCell ref="AE542:AJ542"/>
+    <mergeCell ref="AK542:AP542"/>
+    <mergeCell ref="AE543:AJ543"/>
+    <mergeCell ref="AK543:AP543"/>
+    <mergeCell ref="AE544:AJ544"/>
+    <mergeCell ref="AE554:AJ554"/>
+    <mergeCell ref="AK554:AP554"/>
+    <mergeCell ref="AE555:AJ555"/>
+    <mergeCell ref="AK555:AP555"/>
+    <mergeCell ref="AE556:AJ556"/>
+    <mergeCell ref="AK556:AP556"/>
+    <mergeCell ref="AE557:AJ557"/>
+    <mergeCell ref="AK557:AP557"/>
+    <mergeCell ref="AE558:AJ558"/>
+    <mergeCell ref="AK558:AP558"/>
+    <mergeCell ref="AE559:AJ559"/>
+    <mergeCell ref="AK559:AP559"/>
+    <mergeCell ref="AK562:AP562"/>
+    <mergeCell ref="AE563:AJ563"/>
+    <mergeCell ref="AK563:AP563"/>
+    <mergeCell ref="AE564:AJ564"/>
+    <mergeCell ref="AK564:AP564"/>
     <mergeCell ref="AE572:AJ572"/>
     <mergeCell ref="AK572:AP572"/>
     <mergeCell ref="AE573:AJ573"/>
@@ -38884,2308 +41155,27 @@
     <mergeCell ref="AE579:AJ579"/>
     <mergeCell ref="AK579:AP579"/>
     <mergeCell ref="AE580:AJ580"/>
-    <mergeCell ref="AE554:AJ554"/>
-    <mergeCell ref="AK554:AP554"/>
-    <mergeCell ref="AE555:AJ555"/>
-    <mergeCell ref="AK555:AP555"/>
-    <mergeCell ref="AE556:AJ556"/>
-    <mergeCell ref="AK556:AP556"/>
-    <mergeCell ref="AE557:AJ557"/>
-    <mergeCell ref="AK557:AP557"/>
-    <mergeCell ref="AE558:AJ558"/>
-    <mergeCell ref="AK558:AP558"/>
-    <mergeCell ref="AE559:AJ559"/>
-    <mergeCell ref="AK559:AP559"/>
-    <mergeCell ref="AK562:AP562"/>
-    <mergeCell ref="AE563:AJ563"/>
-    <mergeCell ref="AK563:AP563"/>
-    <mergeCell ref="AE564:AJ564"/>
-    <mergeCell ref="AK564:AP564"/>
-    <mergeCell ref="AE537:AJ537"/>
-    <mergeCell ref="AK537:AP537"/>
-    <mergeCell ref="AE538:AJ538"/>
-    <mergeCell ref="AK538:AP538"/>
-    <mergeCell ref="AE539:AJ539"/>
-    <mergeCell ref="AK539:AP539"/>
-    <mergeCell ref="AE540:AJ540"/>
-    <mergeCell ref="AK540:AP540"/>
-    <mergeCell ref="AE541:AJ541"/>
-    <mergeCell ref="AK541:AP541"/>
-    <mergeCell ref="AK544:AP544"/>
-    <mergeCell ref="AE545:AJ545"/>
-    <mergeCell ref="AK545:AP545"/>
-    <mergeCell ref="AE546:AJ546"/>
-    <mergeCell ref="AK546:AP546"/>
-    <mergeCell ref="AE542:AJ542"/>
-    <mergeCell ref="AK542:AP542"/>
-    <mergeCell ref="AE543:AJ543"/>
-    <mergeCell ref="AK543:AP543"/>
-    <mergeCell ref="AE544:AJ544"/>
-    <mergeCell ref="AE518:AJ518"/>
-    <mergeCell ref="AK518:AP518"/>
-    <mergeCell ref="AE519:AJ519"/>
-    <mergeCell ref="AK519:AP519"/>
-    <mergeCell ref="AE520:AJ520"/>
-    <mergeCell ref="AK520:AP520"/>
-    <mergeCell ref="AE521:AJ521"/>
-    <mergeCell ref="AK521:AP521"/>
-    <mergeCell ref="AE522:AJ522"/>
-    <mergeCell ref="AK522:AP522"/>
-    <mergeCell ref="AE523:AJ523"/>
-    <mergeCell ref="AK523:AP523"/>
-    <mergeCell ref="AK526:AP526"/>
-    <mergeCell ref="AE527:AJ527"/>
-    <mergeCell ref="AK527:AP527"/>
-    <mergeCell ref="AE528:AJ528"/>
-    <mergeCell ref="AK528:AP528"/>
-    <mergeCell ref="AE501:AJ501"/>
-    <mergeCell ref="AK501:AP501"/>
-    <mergeCell ref="AE502:AJ502"/>
-    <mergeCell ref="AK502:AP502"/>
-    <mergeCell ref="AE503:AJ503"/>
-    <mergeCell ref="AK503:AP503"/>
-    <mergeCell ref="AE504:AJ504"/>
-    <mergeCell ref="AK504:AP504"/>
-    <mergeCell ref="AE505:AJ505"/>
-    <mergeCell ref="AK505:AP505"/>
-    <mergeCell ref="AK508:AP508"/>
-    <mergeCell ref="AE509:AJ509"/>
-    <mergeCell ref="AK509:AP509"/>
-    <mergeCell ref="AE510:AJ510"/>
-    <mergeCell ref="AK510:AP510"/>
-    <mergeCell ref="AE506:AJ506"/>
-    <mergeCell ref="AK506:AP506"/>
-    <mergeCell ref="AE507:AJ507"/>
-    <mergeCell ref="AK507:AP507"/>
-    <mergeCell ref="AE508:AJ508"/>
-    <mergeCell ref="AE482:AJ482"/>
-    <mergeCell ref="AK482:AP482"/>
-    <mergeCell ref="AE483:AJ483"/>
-    <mergeCell ref="AK483:AP483"/>
-    <mergeCell ref="AE484:AJ484"/>
-    <mergeCell ref="AK484:AP484"/>
-    <mergeCell ref="AE485:AJ485"/>
-    <mergeCell ref="AK485:AP485"/>
-    <mergeCell ref="AE486:AJ486"/>
-    <mergeCell ref="AK486:AP486"/>
-    <mergeCell ref="AE487:AJ487"/>
-    <mergeCell ref="AK487:AP487"/>
-    <mergeCell ref="AK490:AP490"/>
-    <mergeCell ref="AE491:AJ491"/>
-    <mergeCell ref="AK491:AP491"/>
-    <mergeCell ref="AE492:AJ492"/>
-    <mergeCell ref="AK492:AP492"/>
-    <mergeCell ref="AE465:AJ465"/>
-    <mergeCell ref="AK465:AP465"/>
-    <mergeCell ref="AE466:AJ466"/>
-    <mergeCell ref="AK466:AP466"/>
-    <mergeCell ref="AE467:AJ467"/>
-    <mergeCell ref="AK467:AP467"/>
-    <mergeCell ref="AE468:AJ468"/>
-    <mergeCell ref="AK468:AP468"/>
-    <mergeCell ref="AE469:AJ469"/>
-    <mergeCell ref="AK469:AP469"/>
-    <mergeCell ref="AK472:AP472"/>
-    <mergeCell ref="AE473:AJ473"/>
-    <mergeCell ref="AK473:AP473"/>
-    <mergeCell ref="AE474:AJ474"/>
-    <mergeCell ref="AK474:AP474"/>
-    <mergeCell ref="AE470:AJ470"/>
-    <mergeCell ref="AK470:AP470"/>
-    <mergeCell ref="AE471:AJ471"/>
-    <mergeCell ref="AK471:AP471"/>
-    <mergeCell ref="AE472:AJ472"/>
-    <mergeCell ref="AE446:AJ446"/>
-    <mergeCell ref="AK446:AP446"/>
-    <mergeCell ref="AE447:AJ447"/>
-    <mergeCell ref="AK447:AP447"/>
-    <mergeCell ref="AE448:AJ448"/>
-    <mergeCell ref="AK448:AP448"/>
-    <mergeCell ref="AE449:AJ449"/>
-    <mergeCell ref="AK449:AP449"/>
-    <mergeCell ref="AE450:AJ450"/>
-    <mergeCell ref="AK450:AP450"/>
-    <mergeCell ref="AE451:AJ451"/>
-    <mergeCell ref="AK451:AP451"/>
-    <mergeCell ref="AK454:AP454"/>
-    <mergeCell ref="AE455:AJ455"/>
-    <mergeCell ref="AK455:AP455"/>
-    <mergeCell ref="AE456:AJ456"/>
-    <mergeCell ref="AK456:AP456"/>
-    <mergeCell ref="AE429:AJ429"/>
-    <mergeCell ref="AK429:AP429"/>
-    <mergeCell ref="AE430:AJ430"/>
-    <mergeCell ref="AK430:AP430"/>
-    <mergeCell ref="AE431:AJ431"/>
-    <mergeCell ref="AK431:AP431"/>
-    <mergeCell ref="AE432:AJ432"/>
-    <mergeCell ref="AK432:AP432"/>
-    <mergeCell ref="AE433:AJ433"/>
-    <mergeCell ref="AK433:AP433"/>
-    <mergeCell ref="AK436:AP436"/>
-    <mergeCell ref="AE437:AJ437"/>
-    <mergeCell ref="AK437:AP437"/>
-    <mergeCell ref="AE438:AJ438"/>
-    <mergeCell ref="AK438:AP438"/>
-    <mergeCell ref="AE434:AJ434"/>
-    <mergeCell ref="AK434:AP434"/>
-    <mergeCell ref="AE435:AJ435"/>
-    <mergeCell ref="AK435:AP435"/>
-    <mergeCell ref="AE436:AJ436"/>
-    <mergeCell ref="AE410:AJ410"/>
-    <mergeCell ref="AK410:AP410"/>
-    <mergeCell ref="AE411:AJ411"/>
-    <mergeCell ref="AK411:AP411"/>
-    <mergeCell ref="AE412:AJ412"/>
-    <mergeCell ref="AK412:AP412"/>
-    <mergeCell ref="AE413:AJ413"/>
-    <mergeCell ref="AK413:AP413"/>
-    <mergeCell ref="AE414:AJ414"/>
-    <mergeCell ref="AK414:AP414"/>
-    <mergeCell ref="AE415:AJ415"/>
-    <mergeCell ref="AK415:AP415"/>
-    <mergeCell ref="AK418:AP418"/>
-    <mergeCell ref="AE419:AJ419"/>
-    <mergeCell ref="AK419:AP419"/>
-    <mergeCell ref="AE420:AJ420"/>
-    <mergeCell ref="AK420:AP420"/>
-    <mergeCell ref="AE393:AJ393"/>
-    <mergeCell ref="AK393:AP393"/>
-    <mergeCell ref="AE394:AJ394"/>
-    <mergeCell ref="AK394:AP394"/>
-    <mergeCell ref="AE395:AJ395"/>
-    <mergeCell ref="AK395:AP395"/>
-    <mergeCell ref="AE396:AJ396"/>
-    <mergeCell ref="AK396:AP396"/>
-    <mergeCell ref="AE397:AJ397"/>
-    <mergeCell ref="AK397:AP397"/>
-    <mergeCell ref="AK400:AP400"/>
-    <mergeCell ref="AE401:AJ401"/>
-    <mergeCell ref="AK401:AP401"/>
-    <mergeCell ref="AE402:AJ402"/>
-    <mergeCell ref="AK402:AP402"/>
-    <mergeCell ref="AE398:AJ398"/>
-    <mergeCell ref="AK398:AP398"/>
-    <mergeCell ref="AE399:AJ399"/>
-    <mergeCell ref="AK399:AP399"/>
-    <mergeCell ref="AE400:AJ400"/>
-    <mergeCell ref="AE374:AJ374"/>
-    <mergeCell ref="AK374:AP374"/>
-    <mergeCell ref="AE375:AJ375"/>
-    <mergeCell ref="AK375:AP375"/>
-    <mergeCell ref="AE376:AJ376"/>
-    <mergeCell ref="AK376:AP376"/>
-    <mergeCell ref="AE377:AJ377"/>
-    <mergeCell ref="AK377:AP377"/>
-    <mergeCell ref="AE378:AJ378"/>
-    <mergeCell ref="AK378:AP378"/>
-    <mergeCell ref="AE379:AJ379"/>
-    <mergeCell ref="AK379:AP379"/>
-    <mergeCell ref="AK382:AP382"/>
-    <mergeCell ref="AE383:AJ383"/>
-    <mergeCell ref="AK383:AP383"/>
-    <mergeCell ref="AE384:AJ384"/>
-    <mergeCell ref="AK384:AP384"/>
-    <mergeCell ref="AE357:AJ357"/>
-    <mergeCell ref="AK357:AP357"/>
-    <mergeCell ref="AE358:AJ358"/>
-    <mergeCell ref="AK358:AP358"/>
-    <mergeCell ref="AE359:AJ359"/>
-    <mergeCell ref="AK359:AP359"/>
-    <mergeCell ref="AE360:AJ360"/>
-    <mergeCell ref="AK360:AP360"/>
-    <mergeCell ref="AE361:AJ361"/>
-    <mergeCell ref="AK361:AP361"/>
-    <mergeCell ref="AK364:AP364"/>
-    <mergeCell ref="AE365:AJ365"/>
-    <mergeCell ref="AK365:AP365"/>
-    <mergeCell ref="AE366:AJ366"/>
-    <mergeCell ref="AK366:AP366"/>
-    <mergeCell ref="AE362:AJ362"/>
-    <mergeCell ref="AK362:AP362"/>
-    <mergeCell ref="AE363:AJ363"/>
-    <mergeCell ref="AK363:AP363"/>
-    <mergeCell ref="AE364:AJ364"/>
-    <mergeCell ref="AE338:AJ338"/>
-    <mergeCell ref="AK338:AP338"/>
-    <mergeCell ref="AE339:AJ339"/>
-    <mergeCell ref="AK339:AP339"/>
-    <mergeCell ref="AE340:AJ340"/>
-    <mergeCell ref="AK340:AP340"/>
-    <mergeCell ref="AE341:AJ341"/>
-    <mergeCell ref="AK341:AP341"/>
-    <mergeCell ref="AE342:AJ342"/>
-    <mergeCell ref="AK342:AP342"/>
-    <mergeCell ref="AE343:AJ343"/>
-    <mergeCell ref="AK343:AP343"/>
-    <mergeCell ref="AK346:AP346"/>
-    <mergeCell ref="AE347:AJ347"/>
-    <mergeCell ref="AK347:AP347"/>
-    <mergeCell ref="AE348:AJ348"/>
-    <mergeCell ref="AK348:AP348"/>
-    <mergeCell ref="AE321:AJ321"/>
-    <mergeCell ref="AK321:AP321"/>
-    <mergeCell ref="AE322:AJ322"/>
-    <mergeCell ref="AK322:AP322"/>
-    <mergeCell ref="AE323:AJ323"/>
-    <mergeCell ref="AK323:AP323"/>
-    <mergeCell ref="AE324:AJ324"/>
-    <mergeCell ref="AK324:AP324"/>
-    <mergeCell ref="AE325:AJ325"/>
-    <mergeCell ref="AK325:AP325"/>
-    <mergeCell ref="AK328:AP328"/>
-    <mergeCell ref="AE329:AJ329"/>
-    <mergeCell ref="AK329:AP329"/>
-    <mergeCell ref="AE330:AJ330"/>
-    <mergeCell ref="AK330:AP330"/>
-    <mergeCell ref="AE326:AJ326"/>
-    <mergeCell ref="AK326:AP326"/>
-    <mergeCell ref="AE327:AJ327"/>
-    <mergeCell ref="AK327:AP327"/>
-    <mergeCell ref="AE328:AJ328"/>
-    <mergeCell ref="AE302:AJ302"/>
-    <mergeCell ref="AK302:AP302"/>
-    <mergeCell ref="AE303:AJ303"/>
-    <mergeCell ref="AK303:AP303"/>
-    <mergeCell ref="AE304:AJ304"/>
-    <mergeCell ref="AK304:AP304"/>
-    <mergeCell ref="AE305:AJ305"/>
-    <mergeCell ref="AK305:AP305"/>
-    <mergeCell ref="AE306:AJ306"/>
-    <mergeCell ref="AK306:AP306"/>
-    <mergeCell ref="AE307:AJ307"/>
-    <mergeCell ref="AK307:AP307"/>
-    <mergeCell ref="AK310:AP310"/>
-    <mergeCell ref="AE311:AJ311"/>
-    <mergeCell ref="AK311:AP311"/>
-    <mergeCell ref="AE312:AJ312"/>
-    <mergeCell ref="AK312:AP312"/>
-    <mergeCell ref="AE285:AJ285"/>
-    <mergeCell ref="AK285:AP285"/>
-    <mergeCell ref="AE286:AJ286"/>
-    <mergeCell ref="AK286:AP286"/>
-    <mergeCell ref="AE287:AJ287"/>
-    <mergeCell ref="AK287:AP287"/>
-    <mergeCell ref="AE288:AJ288"/>
-    <mergeCell ref="AK288:AP288"/>
-    <mergeCell ref="AE289:AJ289"/>
-    <mergeCell ref="AK289:AP289"/>
-    <mergeCell ref="AK292:AP292"/>
-    <mergeCell ref="AE293:AJ293"/>
-    <mergeCell ref="AK293:AP293"/>
-    <mergeCell ref="AE294:AJ294"/>
-    <mergeCell ref="AK294:AP294"/>
-    <mergeCell ref="AE290:AJ290"/>
-    <mergeCell ref="AK290:AP290"/>
-    <mergeCell ref="AE291:AJ291"/>
-    <mergeCell ref="AK291:AP291"/>
-    <mergeCell ref="AE292:AJ292"/>
-    <mergeCell ref="AE266:AJ266"/>
-    <mergeCell ref="AK266:AP266"/>
-    <mergeCell ref="AE267:AJ267"/>
-    <mergeCell ref="AK267:AP267"/>
-    <mergeCell ref="AE268:AJ268"/>
-    <mergeCell ref="AK268:AP268"/>
-    <mergeCell ref="AE269:AJ269"/>
-    <mergeCell ref="AK269:AP269"/>
-    <mergeCell ref="AE270:AJ270"/>
-    <mergeCell ref="AK270:AP270"/>
-    <mergeCell ref="AE271:AJ271"/>
-    <mergeCell ref="AK271:AP271"/>
-    <mergeCell ref="AK274:AP274"/>
-    <mergeCell ref="AE275:AJ275"/>
-    <mergeCell ref="AK275:AP275"/>
-    <mergeCell ref="AE276:AJ276"/>
-    <mergeCell ref="AK276:AP276"/>
-    <mergeCell ref="AE249:AJ249"/>
-    <mergeCell ref="AK249:AP249"/>
-    <mergeCell ref="AE250:AJ250"/>
-    <mergeCell ref="AK250:AP250"/>
-    <mergeCell ref="AE251:AJ251"/>
-    <mergeCell ref="AK251:AP251"/>
-    <mergeCell ref="AE252:AJ252"/>
-    <mergeCell ref="AK252:AP252"/>
-    <mergeCell ref="AE253:AJ253"/>
-    <mergeCell ref="AK253:AP253"/>
-    <mergeCell ref="AK256:AP256"/>
-    <mergeCell ref="AE257:AJ257"/>
-    <mergeCell ref="AK257:AP257"/>
-    <mergeCell ref="AE258:AJ258"/>
-    <mergeCell ref="AK258:AP258"/>
-    <mergeCell ref="AE254:AJ254"/>
-    <mergeCell ref="AK254:AP254"/>
-    <mergeCell ref="AE255:AJ255"/>
-    <mergeCell ref="AK255:AP255"/>
-    <mergeCell ref="AE256:AJ256"/>
-    <mergeCell ref="AE230:AJ230"/>
-    <mergeCell ref="AK230:AP230"/>
-    <mergeCell ref="AE231:AJ231"/>
-    <mergeCell ref="AK231:AP231"/>
-    <mergeCell ref="AE232:AJ232"/>
-    <mergeCell ref="AK232:AP232"/>
-    <mergeCell ref="AE233:AJ233"/>
-    <mergeCell ref="AK233:AP233"/>
-    <mergeCell ref="AE234:AJ234"/>
-    <mergeCell ref="AK234:AP234"/>
-    <mergeCell ref="AE235:AJ235"/>
-    <mergeCell ref="AK235:AP235"/>
-    <mergeCell ref="AK238:AP238"/>
-    <mergeCell ref="AE239:AJ239"/>
-    <mergeCell ref="AK239:AP239"/>
-    <mergeCell ref="AE240:AJ240"/>
-    <mergeCell ref="AK240:AP240"/>
-    <mergeCell ref="AE213:AJ213"/>
-    <mergeCell ref="AK213:AP213"/>
-    <mergeCell ref="AE214:AJ214"/>
-    <mergeCell ref="AK214:AP214"/>
-    <mergeCell ref="AE215:AJ215"/>
-    <mergeCell ref="AK215:AP215"/>
-    <mergeCell ref="AE216:AJ216"/>
-    <mergeCell ref="AK216:AP216"/>
-    <mergeCell ref="AE217:AJ217"/>
-    <mergeCell ref="AK217:AP217"/>
-    <mergeCell ref="AK220:AP220"/>
-    <mergeCell ref="AE221:AJ221"/>
-    <mergeCell ref="AK221:AP221"/>
-    <mergeCell ref="AE222:AJ222"/>
-    <mergeCell ref="AK222:AP222"/>
-    <mergeCell ref="AE218:AJ218"/>
-    <mergeCell ref="AK218:AP218"/>
-    <mergeCell ref="AE219:AJ219"/>
-    <mergeCell ref="AK219:AP219"/>
-    <mergeCell ref="AE220:AJ220"/>
-    <mergeCell ref="AE194:AJ194"/>
-    <mergeCell ref="AK194:AP194"/>
-    <mergeCell ref="AE195:AJ195"/>
-    <mergeCell ref="AK195:AP195"/>
-    <mergeCell ref="AE196:AJ196"/>
-    <mergeCell ref="AK196:AP196"/>
-    <mergeCell ref="AE197:AJ197"/>
-    <mergeCell ref="AK197:AP197"/>
-    <mergeCell ref="AE198:AJ198"/>
-    <mergeCell ref="AK198:AP198"/>
-    <mergeCell ref="AE199:AJ199"/>
-    <mergeCell ref="AK199:AP199"/>
-    <mergeCell ref="AK202:AP202"/>
-    <mergeCell ref="AE203:AJ203"/>
-    <mergeCell ref="AK203:AP203"/>
-    <mergeCell ref="AE204:AJ204"/>
-    <mergeCell ref="AK204:AP204"/>
-    <mergeCell ref="AE177:AJ177"/>
-    <mergeCell ref="AK177:AP177"/>
-    <mergeCell ref="AE178:AJ178"/>
-    <mergeCell ref="AK178:AP178"/>
-    <mergeCell ref="AE179:AJ179"/>
-    <mergeCell ref="AK179:AP179"/>
-    <mergeCell ref="AE180:AJ180"/>
-    <mergeCell ref="AK180:AP180"/>
-    <mergeCell ref="AE181:AJ181"/>
-    <mergeCell ref="AK181:AP181"/>
-    <mergeCell ref="AK184:AP184"/>
-    <mergeCell ref="AE185:AJ185"/>
-    <mergeCell ref="AK185:AP185"/>
-    <mergeCell ref="AE186:AJ186"/>
-    <mergeCell ref="AK186:AP186"/>
-    <mergeCell ref="AE182:AJ182"/>
-    <mergeCell ref="AK182:AP182"/>
-    <mergeCell ref="AE183:AJ183"/>
-    <mergeCell ref="AK183:AP183"/>
-    <mergeCell ref="AE184:AJ184"/>
-    <mergeCell ref="AE158:AJ158"/>
-    <mergeCell ref="AK158:AP158"/>
-    <mergeCell ref="AE159:AJ159"/>
-    <mergeCell ref="AK159:AP159"/>
-    <mergeCell ref="AE160:AJ160"/>
-    <mergeCell ref="AK160:AP160"/>
-    <mergeCell ref="AE161:AJ161"/>
-    <mergeCell ref="AK161:AP161"/>
-    <mergeCell ref="AE162:AJ162"/>
-    <mergeCell ref="AK162:AP162"/>
-    <mergeCell ref="AE163:AJ163"/>
-    <mergeCell ref="AK163:AP163"/>
-    <mergeCell ref="AK166:AP166"/>
-    <mergeCell ref="AE167:AJ167"/>
-    <mergeCell ref="AK167:AP167"/>
-    <mergeCell ref="AE168:AJ168"/>
-    <mergeCell ref="AK168:AP168"/>
-    <mergeCell ref="AE141:AJ141"/>
-    <mergeCell ref="AK141:AP141"/>
-    <mergeCell ref="AE142:AJ142"/>
-    <mergeCell ref="AK142:AP142"/>
-    <mergeCell ref="AE143:AJ143"/>
-    <mergeCell ref="AK143:AP143"/>
-    <mergeCell ref="AE144:AJ144"/>
-    <mergeCell ref="AK144:AP144"/>
-    <mergeCell ref="AE145:AJ145"/>
-    <mergeCell ref="AK145:AP145"/>
-    <mergeCell ref="AK148:AP148"/>
-    <mergeCell ref="AE149:AJ149"/>
-    <mergeCell ref="AK149:AP149"/>
-    <mergeCell ref="AE150:AJ150"/>
-    <mergeCell ref="AK150:AP150"/>
-    <mergeCell ref="AE146:AJ146"/>
-    <mergeCell ref="AK146:AP146"/>
-    <mergeCell ref="AE147:AJ147"/>
-    <mergeCell ref="AK147:AP147"/>
-    <mergeCell ref="AE148:AJ148"/>
-    <mergeCell ref="AE122:AJ122"/>
-    <mergeCell ref="AK122:AP122"/>
-    <mergeCell ref="AE123:AJ123"/>
-    <mergeCell ref="AK123:AP123"/>
-    <mergeCell ref="AE124:AJ124"/>
-    <mergeCell ref="AK124:AP124"/>
-    <mergeCell ref="AE125:AJ125"/>
-    <mergeCell ref="AK125:AP125"/>
-    <mergeCell ref="AE126:AJ126"/>
-    <mergeCell ref="AK126:AP126"/>
-    <mergeCell ref="AE127:AJ127"/>
-    <mergeCell ref="AK127:AP127"/>
-    <mergeCell ref="AK130:AP130"/>
-    <mergeCell ref="AE131:AJ131"/>
-    <mergeCell ref="AK131:AP131"/>
-    <mergeCell ref="AE132:AJ132"/>
-    <mergeCell ref="AK132:AP132"/>
-    <mergeCell ref="AE105:AJ105"/>
-    <mergeCell ref="AK105:AP105"/>
-    <mergeCell ref="AE106:AJ106"/>
-    <mergeCell ref="AK106:AP106"/>
-    <mergeCell ref="AE107:AJ107"/>
-    <mergeCell ref="AK107:AP107"/>
-    <mergeCell ref="AE108:AJ108"/>
-    <mergeCell ref="AK108:AP108"/>
-    <mergeCell ref="AE109:AJ109"/>
-    <mergeCell ref="AK109:AP109"/>
-    <mergeCell ref="AK112:AP112"/>
-    <mergeCell ref="AE113:AJ113"/>
-    <mergeCell ref="AK113:AP113"/>
-    <mergeCell ref="AE114:AJ114"/>
-    <mergeCell ref="AK114:AP114"/>
-    <mergeCell ref="AE110:AJ110"/>
-    <mergeCell ref="AK110:AP110"/>
-    <mergeCell ref="AE111:AJ111"/>
-    <mergeCell ref="AK111:AP111"/>
-    <mergeCell ref="AE112:AJ112"/>
-    <mergeCell ref="AE86:AJ86"/>
-    <mergeCell ref="AK86:AP86"/>
-    <mergeCell ref="AE87:AJ87"/>
-    <mergeCell ref="AK87:AP87"/>
-    <mergeCell ref="AE88:AJ88"/>
-    <mergeCell ref="AK88:AP88"/>
-    <mergeCell ref="AE89:AJ89"/>
-    <mergeCell ref="AK89:AP89"/>
-    <mergeCell ref="AE90:AJ90"/>
-    <mergeCell ref="AK90:AP90"/>
-    <mergeCell ref="AE91:AJ91"/>
-    <mergeCell ref="AK91:AP91"/>
-    <mergeCell ref="AK94:AP94"/>
-    <mergeCell ref="AE95:AJ95"/>
-    <mergeCell ref="AK95:AP95"/>
-    <mergeCell ref="AE96:AJ96"/>
-    <mergeCell ref="AK96:AP96"/>
-    <mergeCell ref="AE69:AJ69"/>
-    <mergeCell ref="AK69:AP69"/>
-    <mergeCell ref="AE70:AJ70"/>
-    <mergeCell ref="AK70:AP70"/>
-    <mergeCell ref="AE71:AJ71"/>
-    <mergeCell ref="AK71:AP71"/>
-    <mergeCell ref="AE72:AJ72"/>
-    <mergeCell ref="AK72:AP72"/>
-    <mergeCell ref="AE73:AJ73"/>
-    <mergeCell ref="AK73:AP73"/>
-    <mergeCell ref="AK76:AP76"/>
-    <mergeCell ref="AE77:AJ77"/>
-    <mergeCell ref="AK77:AP77"/>
-    <mergeCell ref="AE78:AJ78"/>
-    <mergeCell ref="AK78:AP78"/>
-    <mergeCell ref="AE74:AJ74"/>
-    <mergeCell ref="AK74:AP74"/>
-    <mergeCell ref="AE75:AJ75"/>
-    <mergeCell ref="AK75:AP75"/>
-    <mergeCell ref="AE76:AJ76"/>
-    <mergeCell ref="AE50:AJ50"/>
-    <mergeCell ref="AK50:AP50"/>
-    <mergeCell ref="AE51:AJ51"/>
-    <mergeCell ref="AK51:AP51"/>
-    <mergeCell ref="AE52:AJ52"/>
-    <mergeCell ref="AK52:AP52"/>
-    <mergeCell ref="AE53:AJ53"/>
-    <mergeCell ref="AK53:AP53"/>
-    <mergeCell ref="AE54:AJ54"/>
-    <mergeCell ref="AK54:AP54"/>
-    <mergeCell ref="AE55:AJ55"/>
-    <mergeCell ref="AK55:AP55"/>
-    <mergeCell ref="AK58:AP58"/>
-    <mergeCell ref="AE59:AJ59"/>
-    <mergeCell ref="AK59:AP59"/>
-    <mergeCell ref="AE60:AJ60"/>
-    <mergeCell ref="AK60:AP60"/>
-    <mergeCell ref="AE33:AJ33"/>
-    <mergeCell ref="AK33:AP33"/>
-    <mergeCell ref="AE34:AJ34"/>
-    <mergeCell ref="AK34:AP34"/>
-    <mergeCell ref="AE35:AJ35"/>
-    <mergeCell ref="AK35:AP35"/>
-    <mergeCell ref="AE36:AJ36"/>
-    <mergeCell ref="AK36:AP36"/>
-    <mergeCell ref="AE37:AJ37"/>
-    <mergeCell ref="AK37:AP37"/>
-    <mergeCell ref="AK40:AP40"/>
-    <mergeCell ref="AE41:AJ41"/>
-    <mergeCell ref="AK41:AP41"/>
-    <mergeCell ref="AE42:AJ42"/>
-    <mergeCell ref="AK42:AP42"/>
-    <mergeCell ref="AE38:AJ38"/>
-    <mergeCell ref="AK38:AP38"/>
-    <mergeCell ref="AE39:AJ39"/>
-    <mergeCell ref="AK39:AP39"/>
-    <mergeCell ref="AE40:AJ40"/>
-    <mergeCell ref="AK14:AP14"/>
-    <mergeCell ref="AE15:AJ15"/>
-    <mergeCell ref="AK15:AP15"/>
-    <mergeCell ref="AE16:AJ16"/>
-    <mergeCell ref="AK16:AP16"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="A19:M19"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="A17:M17"/>
-    <mergeCell ref="A14:M14"/>
-    <mergeCell ref="A15:M15"/>
-    <mergeCell ref="AE17:AJ17"/>
-    <mergeCell ref="AK17:AP17"/>
-    <mergeCell ref="AE18:AJ18"/>
-    <mergeCell ref="AK18:AP18"/>
-    <mergeCell ref="AE19:AJ19"/>
-    <mergeCell ref="AK19:AP19"/>
-    <mergeCell ref="A1:AP8"/>
-    <mergeCell ref="A9:AO9"/>
-    <mergeCell ref="B10:AN12"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="N24:AD24"/>
-    <mergeCell ref="N25:AD25"/>
-    <mergeCell ref="A22:M22"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="N22:AD22"/>
-    <mergeCell ref="N23:AD23"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="A21:M21"/>
-    <mergeCell ref="N20:AD20"/>
-    <mergeCell ref="N21:AD21"/>
-    <mergeCell ref="AE20:AJ20"/>
-    <mergeCell ref="AK20:AP20"/>
-    <mergeCell ref="AE21:AJ21"/>
-    <mergeCell ref="AK21:AP21"/>
-    <mergeCell ref="AE22:AJ22"/>
-    <mergeCell ref="AK22:AP22"/>
-    <mergeCell ref="AE23:AJ23"/>
-    <mergeCell ref="AK23:AP23"/>
-    <mergeCell ref="AE24:AJ24"/>
-    <mergeCell ref="AK24:AP24"/>
-    <mergeCell ref="AE25:AJ25"/>
-    <mergeCell ref="AK25:AP25"/>
-    <mergeCell ref="N13:AD13"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="AE13:AJ13"/>
-    <mergeCell ref="AK13:AP13"/>
-    <mergeCell ref="AE14:AJ14"/>
-    <mergeCell ref="A30:M30"/>
-    <mergeCell ref="A31:M31"/>
-    <mergeCell ref="N30:AD30"/>
-    <mergeCell ref="N31:AD31"/>
-    <mergeCell ref="A28:M28"/>
-    <mergeCell ref="A29:M29"/>
-    <mergeCell ref="N28:AD28"/>
-    <mergeCell ref="N29:AD29"/>
-    <mergeCell ref="A26:M26"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="N26:AD26"/>
-    <mergeCell ref="N27:AD27"/>
-    <mergeCell ref="AE29:AJ29"/>
-    <mergeCell ref="AK29:AP29"/>
-    <mergeCell ref="AE30:AJ30"/>
-    <mergeCell ref="AK30:AP30"/>
-    <mergeCell ref="AE31:AJ31"/>
-    <mergeCell ref="AE26:AJ26"/>
-    <mergeCell ref="AK26:AP26"/>
-    <mergeCell ref="AE27:AJ27"/>
-    <mergeCell ref="AK27:AP27"/>
-    <mergeCell ref="AE28:AJ28"/>
-    <mergeCell ref="AK28:AP28"/>
-    <mergeCell ref="AK31:AP31"/>
-    <mergeCell ref="N45:AD45"/>
-    <mergeCell ref="AE47:AJ47"/>
-    <mergeCell ref="AK47:AP47"/>
-    <mergeCell ref="AE48:AJ48"/>
-    <mergeCell ref="AK48:AP48"/>
-    <mergeCell ref="AE49:AJ49"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="A37:M37"/>
-    <mergeCell ref="N36:AD36"/>
-    <mergeCell ref="N37:AD37"/>
-    <mergeCell ref="A34:M34"/>
-    <mergeCell ref="A35:M35"/>
-    <mergeCell ref="N34:AD34"/>
-    <mergeCell ref="N35:AD35"/>
-    <mergeCell ref="A32:M32"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="N32:AD32"/>
-    <mergeCell ref="N33:AD33"/>
-    <mergeCell ref="A42:M42"/>
-    <mergeCell ref="A43:M43"/>
-    <mergeCell ref="N42:AD42"/>
-    <mergeCell ref="N43:AD43"/>
-    <mergeCell ref="A40:M40"/>
-    <mergeCell ref="A41:M41"/>
-    <mergeCell ref="N40:AD40"/>
-    <mergeCell ref="N41:AD41"/>
-    <mergeCell ref="A38:M38"/>
-    <mergeCell ref="A39:M39"/>
-    <mergeCell ref="N38:AD38"/>
-    <mergeCell ref="N39:AD39"/>
-    <mergeCell ref="AE32:AJ32"/>
-    <mergeCell ref="AK32:AP32"/>
-    <mergeCell ref="AE43:AJ43"/>
-    <mergeCell ref="AK43:AP43"/>
-    <mergeCell ref="AE44:AJ44"/>
-    <mergeCell ref="AK44:AP44"/>
-    <mergeCell ref="AE45:AJ45"/>
-    <mergeCell ref="AK45:AP45"/>
-    <mergeCell ref="AE46:AJ46"/>
-    <mergeCell ref="AK46:AP46"/>
-    <mergeCell ref="AK49:AP49"/>
-    <mergeCell ref="A54:M54"/>
-    <mergeCell ref="A55:M55"/>
-    <mergeCell ref="N54:AD54"/>
-    <mergeCell ref="N55:AD55"/>
-    <mergeCell ref="A52:M52"/>
-    <mergeCell ref="A53:M53"/>
-    <mergeCell ref="N52:AD52"/>
-    <mergeCell ref="N53:AD53"/>
-    <mergeCell ref="A50:M50"/>
-    <mergeCell ref="A51:M51"/>
-    <mergeCell ref="N50:AD50"/>
-    <mergeCell ref="N51:AD51"/>
-    <mergeCell ref="A48:M48"/>
-    <mergeCell ref="A49:M49"/>
-    <mergeCell ref="N48:AD48"/>
-    <mergeCell ref="N49:AD49"/>
-    <mergeCell ref="A46:M46"/>
-    <mergeCell ref="A47:M47"/>
-    <mergeCell ref="N46:AD46"/>
-    <mergeCell ref="N47:AD47"/>
-    <mergeCell ref="A44:M44"/>
-    <mergeCell ref="A45:M45"/>
-    <mergeCell ref="N44:AD44"/>
-    <mergeCell ref="A60:M60"/>
-    <mergeCell ref="A61:M61"/>
-    <mergeCell ref="N60:AD60"/>
-    <mergeCell ref="N61:AD61"/>
-    <mergeCell ref="A58:M58"/>
-    <mergeCell ref="A59:M59"/>
-    <mergeCell ref="N58:AD58"/>
-    <mergeCell ref="N59:AD59"/>
-    <mergeCell ref="A56:M56"/>
-    <mergeCell ref="A57:M57"/>
-    <mergeCell ref="N56:AD56"/>
-    <mergeCell ref="N57:AD57"/>
-    <mergeCell ref="AE56:AJ56"/>
-    <mergeCell ref="AK56:AP56"/>
-    <mergeCell ref="AE57:AJ57"/>
-    <mergeCell ref="AK57:AP57"/>
-    <mergeCell ref="AE58:AJ58"/>
-    <mergeCell ref="AE61:AJ61"/>
-    <mergeCell ref="AK61:AP61"/>
-    <mergeCell ref="A66:M66"/>
-    <mergeCell ref="A67:M67"/>
-    <mergeCell ref="N66:AD66"/>
-    <mergeCell ref="N67:AD67"/>
-    <mergeCell ref="A64:M64"/>
-    <mergeCell ref="A65:M65"/>
-    <mergeCell ref="N64:AD64"/>
-    <mergeCell ref="N65:AD65"/>
-    <mergeCell ref="A62:M62"/>
-    <mergeCell ref="A63:M63"/>
-    <mergeCell ref="N62:AD62"/>
-    <mergeCell ref="N63:AD63"/>
-    <mergeCell ref="AE65:AJ65"/>
-    <mergeCell ref="AK65:AP65"/>
-    <mergeCell ref="AE66:AJ66"/>
-    <mergeCell ref="AK66:AP66"/>
-    <mergeCell ref="AE67:AJ67"/>
-    <mergeCell ref="AE62:AJ62"/>
-    <mergeCell ref="AK62:AP62"/>
-    <mergeCell ref="AE63:AJ63"/>
-    <mergeCell ref="AK63:AP63"/>
-    <mergeCell ref="AE64:AJ64"/>
-    <mergeCell ref="AK64:AP64"/>
-    <mergeCell ref="AK67:AP67"/>
-    <mergeCell ref="N81:AD81"/>
-    <mergeCell ref="AE83:AJ83"/>
-    <mergeCell ref="AK83:AP83"/>
-    <mergeCell ref="AE84:AJ84"/>
-    <mergeCell ref="AK84:AP84"/>
-    <mergeCell ref="AE85:AJ85"/>
-    <mergeCell ref="A72:M72"/>
-    <mergeCell ref="A73:M73"/>
-    <mergeCell ref="N72:AD72"/>
-    <mergeCell ref="N73:AD73"/>
-    <mergeCell ref="A70:M70"/>
-    <mergeCell ref="A71:M71"/>
-    <mergeCell ref="N70:AD70"/>
-    <mergeCell ref="N71:AD71"/>
-    <mergeCell ref="A68:M68"/>
-    <mergeCell ref="A69:M69"/>
-    <mergeCell ref="N68:AD68"/>
-    <mergeCell ref="N69:AD69"/>
-    <mergeCell ref="A78:M78"/>
-    <mergeCell ref="A79:M79"/>
-    <mergeCell ref="N78:AD78"/>
-    <mergeCell ref="N79:AD79"/>
-    <mergeCell ref="A76:M76"/>
-    <mergeCell ref="A77:M77"/>
-    <mergeCell ref="N76:AD76"/>
-    <mergeCell ref="N77:AD77"/>
-    <mergeCell ref="A74:M74"/>
-    <mergeCell ref="A75:M75"/>
-    <mergeCell ref="N74:AD74"/>
-    <mergeCell ref="N75:AD75"/>
-    <mergeCell ref="AE68:AJ68"/>
-    <mergeCell ref="AK68:AP68"/>
-    <mergeCell ref="AE79:AJ79"/>
-    <mergeCell ref="AK79:AP79"/>
-    <mergeCell ref="AE80:AJ80"/>
-    <mergeCell ref="AK80:AP80"/>
-    <mergeCell ref="AE81:AJ81"/>
-    <mergeCell ref="AK81:AP81"/>
-    <mergeCell ref="AE82:AJ82"/>
-    <mergeCell ref="AK82:AP82"/>
-    <mergeCell ref="AK85:AP85"/>
-    <mergeCell ref="A90:M90"/>
-    <mergeCell ref="A91:M91"/>
-    <mergeCell ref="N90:AD90"/>
-    <mergeCell ref="N91:AD91"/>
-    <mergeCell ref="A88:M88"/>
-    <mergeCell ref="A89:M89"/>
-    <mergeCell ref="N88:AD88"/>
-    <mergeCell ref="N89:AD89"/>
-    <mergeCell ref="A86:M86"/>
-    <mergeCell ref="A87:M87"/>
-    <mergeCell ref="N86:AD86"/>
-    <mergeCell ref="N87:AD87"/>
-    <mergeCell ref="A84:M84"/>
-    <mergeCell ref="A85:M85"/>
-    <mergeCell ref="N84:AD84"/>
-    <mergeCell ref="N85:AD85"/>
-    <mergeCell ref="A82:M82"/>
-    <mergeCell ref="A83:M83"/>
-    <mergeCell ref="N82:AD82"/>
-    <mergeCell ref="N83:AD83"/>
-    <mergeCell ref="A80:M80"/>
-    <mergeCell ref="A81:M81"/>
-    <mergeCell ref="N80:AD80"/>
-    <mergeCell ref="A96:M96"/>
-    <mergeCell ref="A97:M97"/>
-    <mergeCell ref="N96:AD96"/>
-    <mergeCell ref="N97:AD97"/>
-    <mergeCell ref="A94:M94"/>
-    <mergeCell ref="A95:M95"/>
-    <mergeCell ref="N94:AD94"/>
-    <mergeCell ref="N95:AD95"/>
-    <mergeCell ref="A92:M92"/>
-    <mergeCell ref="A93:M93"/>
-    <mergeCell ref="N92:AD92"/>
-    <mergeCell ref="N93:AD93"/>
-    <mergeCell ref="AE92:AJ92"/>
-    <mergeCell ref="AK92:AP92"/>
-    <mergeCell ref="AE93:AJ93"/>
-    <mergeCell ref="AK93:AP93"/>
-    <mergeCell ref="AE94:AJ94"/>
-    <mergeCell ref="AE97:AJ97"/>
-    <mergeCell ref="AK97:AP97"/>
-    <mergeCell ref="A102:M102"/>
-    <mergeCell ref="A103:M103"/>
-    <mergeCell ref="N102:AD102"/>
-    <mergeCell ref="N103:AD103"/>
-    <mergeCell ref="A100:M100"/>
-    <mergeCell ref="A101:M101"/>
-    <mergeCell ref="N100:AD100"/>
-    <mergeCell ref="N101:AD101"/>
-    <mergeCell ref="A98:M98"/>
-    <mergeCell ref="A99:M99"/>
-    <mergeCell ref="N98:AD98"/>
-    <mergeCell ref="N99:AD99"/>
-    <mergeCell ref="AE101:AJ101"/>
-    <mergeCell ref="AK101:AP101"/>
-    <mergeCell ref="AE102:AJ102"/>
-    <mergeCell ref="AK102:AP102"/>
-    <mergeCell ref="AE103:AJ103"/>
-    <mergeCell ref="AE98:AJ98"/>
-    <mergeCell ref="AK98:AP98"/>
-    <mergeCell ref="AE99:AJ99"/>
-    <mergeCell ref="AK99:AP99"/>
-    <mergeCell ref="AE100:AJ100"/>
-    <mergeCell ref="AK100:AP100"/>
-    <mergeCell ref="AK103:AP103"/>
-    <mergeCell ref="N117:AD117"/>
-    <mergeCell ref="AE119:AJ119"/>
-    <mergeCell ref="AK119:AP119"/>
-    <mergeCell ref="AE120:AJ120"/>
-    <mergeCell ref="AK120:AP120"/>
-    <mergeCell ref="AE121:AJ121"/>
-    <mergeCell ref="A108:M108"/>
-    <mergeCell ref="A109:M109"/>
-    <mergeCell ref="N108:AD108"/>
-    <mergeCell ref="N109:AD109"/>
-    <mergeCell ref="A106:M106"/>
-    <mergeCell ref="A107:M107"/>
-    <mergeCell ref="N106:AD106"/>
-    <mergeCell ref="N107:AD107"/>
-    <mergeCell ref="A104:M104"/>
-    <mergeCell ref="A105:M105"/>
-    <mergeCell ref="N104:AD104"/>
-    <mergeCell ref="N105:AD105"/>
-    <mergeCell ref="A114:M114"/>
-    <mergeCell ref="A115:M115"/>
-    <mergeCell ref="N114:AD114"/>
-    <mergeCell ref="N115:AD115"/>
-    <mergeCell ref="A112:M112"/>
-    <mergeCell ref="A113:M113"/>
-    <mergeCell ref="N112:AD112"/>
-    <mergeCell ref="N113:AD113"/>
-    <mergeCell ref="A110:M110"/>
-    <mergeCell ref="A111:M111"/>
-    <mergeCell ref="N110:AD110"/>
-    <mergeCell ref="N111:AD111"/>
-    <mergeCell ref="AE104:AJ104"/>
-    <mergeCell ref="AK104:AP104"/>
-    <mergeCell ref="AE115:AJ115"/>
-    <mergeCell ref="AK115:AP115"/>
-    <mergeCell ref="AE116:AJ116"/>
-    <mergeCell ref="AK116:AP116"/>
-    <mergeCell ref="AE117:AJ117"/>
-    <mergeCell ref="AK117:AP117"/>
-    <mergeCell ref="AE118:AJ118"/>
-    <mergeCell ref="AK118:AP118"/>
-    <mergeCell ref="AK121:AP121"/>
-    <mergeCell ref="A126:M126"/>
-    <mergeCell ref="A127:M127"/>
-    <mergeCell ref="N126:AD126"/>
-    <mergeCell ref="N127:AD127"/>
-    <mergeCell ref="A124:M124"/>
-    <mergeCell ref="A125:M125"/>
-    <mergeCell ref="N124:AD124"/>
-    <mergeCell ref="N125:AD125"/>
-    <mergeCell ref="A122:M122"/>
-    <mergeCell ref="A123:M123"/>
-    <mergeCell ref="N122:AD122"/>
-    <mergeCell ref="N123:AD123"/>
-    <mergeCell ref="A120:M120"/>
-    <mergeCell ref="A121:M121"/>
-    <mergeCell ref="N120:AD120"/>
-    <mergeCell ref="N121:AD121"/>
-    <mergeCell ref="A118:M118"/>
-    <mergeCell ref="A119:M119"/>
-    <mergeCell ref="N118:AD118"/>
-    <mergeCell ref="N119:AD119"/>
-    <mergeCell ref="A116:M116"/>
-    <mergeCell ref="A117:M117"/>
-    <mergeCell ref="N116:AD116"/>
-    <mergeCell ref="A132:M132"/>
-    <mergeCell ref="A133:M133"/>
-    <mergeCell ref="N132:AD132"/>
-    <mergeCell ref="N133:AD133"/>
-    <mergeCell ref="A130:M130"/>
-    <mergeCell ref="A131:M131"/>
-    <mergeCell ref="N130:AD130"/>
-    <mergeCell ref="N131:AD131"/>
-    <mergeCell ref="A128:M128"/>
-    <mergeCell ref="A129:M129"/>
-    <mergeCell ref="N128:AD128"/>
-    <mergeCell ref="N129:AD129"/>
-    <mergeCell ref="AE128:AJ128"/>
-    <mergeCell ref="AK128:AP128"/>
-    <mergeCell ref="AE129:AJ129"/>
-    <mergeCell ref="AK129:AP129"/>
-    <mergeCell ref="AE130:AJ130"/>
-    <mergeCell ref="AE133:AJ133"/>
-    <mergeCell ref="AK133:AP133"/>
-    <mergeCell ref="A138:M138"/>
-    <mergeCell ref="A139:M139"/>
-    <mergeCell ref="N138:AD138"/>
-    <mergeCell ref="N139:AD139"/>
-    <mergeCell ref="A136:M136"/>
-    <mergeCell ref="A137:M137"/>
-    <mergeCell ref="N136:AD136"/>
-    <mergeCell ref="N137:AD137"/>
-    <mergeCell ref="A134:M134"/>
-    <mergeCell ref="A135:M135"/>
-    <mergeCell ref="N134:AD134"/>
-    <mergeCell ref="N135:AD135"/>
-    <mergeCell ref="AE137:AJ137"/>
-    <mergeCell ref="AK137:AP137"/>
-    <mergeCell ref="AE138:AJ138"/>
-    <mergeCell ref="AK138:AP138"/>
-    <mergeCell ref="AE139:AJ139"/>
-    <mergeCell ref="AE134:AJ134"/>
-    <mergeCell ref="AK134:AP134"/>
-    <mergeCell ref="AE135:AJ135"/>
-    <mergeCell ref="AK135:AP135"/>
-    <mergeCell ref="AE136:AJ136"/>
-    <mergeCell ref="AK136:AP136"/>
-    <mergeCell ref="AK139:AP139"/>
-    <mergeCell ref="N153:AD153"/>
-    <mergeCell ref="AE155:AJ155"/>
-    <mergeCell ref="AK155:AP155"/>
-    <mergeCell ref="AE156:AJ156"/>
-    <mergeCell ref="AK156:AP156"/>
-    <mergeCell ref="AE157:AJ157"/>
-    <mergeCell ref="A144:M144"/>
-    <mergeCell ref="A145:M145"/>
-    <mergeCell ref="N144:AD144"/>
-    <mergeCell ref="N145:AD145"/>
-    <mergeCell ref="A142:M142"/>
-    <mergeCell ref="A143:M143"/>
-    <mergeCell ref="N142:AD142"/>
-    <mergeCell ref="N143:AD143"/>
-    <mergeCell ref="A140:M140"/>
-    <mergeCell ref="A141:M141"/>
-    <mergeCell ref="N140:AD140"/>
-    <mergeCell ref="N141:AD141"/>
-    <mergeCell ref="A150:M150"/>
-    <mergeCell ref="A151:M151"/>
-    <mergeCell ref="N150:AD150"/>
-    <mergeCell ref="N151:AD151"/>
-    <mergeCell ref="A148:M148"/>
-    <mergeCell ref="A149:M149"/>
-    <mergeCell ref="N148:AD148"/>
-    <mergeCell ref="N149:AD149"/>
-    <mergeCell ref="A146:M146"/>
-    <mergeCell ref="A147:M147"/>
-    <mergeCell ref="N146:AD146"/>
-    <mergeCell ref="N147:AD147"/>
-    <mergeCell ref="AE140:AJ140"/>
-    <mergeCell ref="AK140:AP140"/>
-    <mergeCell ref="AE151:AJ151"/>
-    <mergeCell ref="AK151:AP151"/>
-    <mergeCell ref="AE152:AJ152"/>
-    <mergeCell ref="AK152:AP152"/>
-    <mergeCell ref="AE153:AJ153"/>
-    <mergeCell ref="AK153:AP153"/>
-    <mergeCell ref="AE154:AJ154"/>
-    <mergeCell ref="AK154:AP154"/>
-    <mergeCell ref="AK157:AP157"/>
-    <mergeCell ref="A162:M162"/>
-    <mergeCell ref="A163:M163"/>
-    <mergeCell ref="N162:AD162"/>
-    <mergeCell ref="N163:AD163"/>
-    <mergeCell ref="A160:M160"/>
-    <mergeCell ref="A161:M161"/>
-    <mergeCell ref="N160:AD160"/>
-    <mergeCell ref="N161:AD161"/>
-    <mergeCell ref="A158:M158"/>
-    <mergeCell ref="A159:M159"/>
-    <mergeCell ref="N158:AD158"/>
-    <mergeCell ref="N159:AD159"/>
-    <mergeCell ref="A156:M156"/>
-    <mergeCell ref="A157:M157"/>
-    <mergeCell ref="N156:AD156"/>
-    <mergeCell ref="N157:AD157"/>
-    <mergeCell ref="A154:M154"/>
-    <mergeCell ref="A155:M155"/>
-    <mergeCell ref="N154:AD154"/>
-    <mergeCell ref="N155:AD155"/>
-    <mergeCell ref="A152:M152"/>
-    <mergeCell ref="A153:M153"/>
-    <mergeCell ref="N152:AD152"/>
-    <mergeCell ref="A168:M168"/>
-    <mergeCell ref="A169:M169"/>
-    <mergeCell ref="N168:AD168"/>
-    <mergeCell ref="N169:AD169"/>
-    <mergeCell ref="A166:M166"/>
-    <mergeCell ref="A167:M167"/>
-    <mergeCell ref="N166:AD166"/>
-    <mergeCell ref="N167:AD167"/>
-    <mergeCell ref="A164:M164"/>
-    <mergeCell ref="A165:M165"/>
-    <mergeCell ref="N164:AD164"/>
-    <mergeCell ref="N165:AD165"/>
-    <mergeCell ref="AE164:AJ164"/>
-    <mergeCell ref="AK164:AP164"/>
-    <mergeCell ref="AE165:AJ165"/>
-    <mergeCell ref="AK165:AP165"/>
-    <mergeCell ref="AE166:AJ166"/>
-    <mergeCell ref="AE169:AJ169"/>
-    <mergeCell ref="AK169:AP169"/>
-    <mergeCell ref="A174:M174"/>
-    <mergeCell ref="A175:M175"/>
-    <mergeCell ref="N174:AD174"/>
-    <mergeCell ref="N175:AD175"/>
-    <mergeCell ref="A172:M172"/>
-    <mergeCell ref="A173:M173"/>
-    <mergeCell ref="N172:AD172"/>
-    <mergeCell ref="N173:AD173"/>
-    <mergeCell ref="A170:M170"/>
-    <mergeCell ref="A171:M171"/>
-    <mergeCell ref="N170:AD170"/>
-    <mergeCell ref="N171:AD171"/>
-    <mergeCell ref="AE173:AJ173"/>
-    <mergeCell ref="AK173:AP173"/>
-    <mergeCell ref="AE174:AJ174"/>
-    <mergeCell ref="AK174:AP174"/>
-    <mergeCell ref="AE175:AJ175"/>
-    <mergeCell ref="AE170:AJ170"/>
-    <mergeCell ref="AK170:AP170"/>
-    <mergeCell ref="AE171:AJ171"/>
-    <mergeCell ref="AK171:AP171"/>
-    <mergeCell ref="AE172:AJ172"/>
-    <mergeCell ref="AK172:AP172"/>
-    <mergeCell ref="AK175:AP175"/>
-    <mergeCell ref="N189:AD189"/>
-    <mergeCell ref="AE191:AJ191"/>
-    <mergeCell ref="AK191:AP191"/>
-    <mergeCell ref="AE192:AJ192"/>
-    <mergeCell ref="AK192:AP192"/>
-    <mergeCell ref="AE193:AJ193"/>
-    <mergeCell ref="A180:M180"/>
-    <mergeCell ref="A181:M181"/>
-    <mergeCell ref="N180:AD180"/>
-    <mergeCell ref="N181:AD181"/>
-    <mergeCell ref="A178:M178"/>
-    <mergeCell ref="A179:M179"/>
-    <mergeCell ref="N178:AD178"/>
-    <mergeCell ref="N179:AD179"/>
-    <mergeCell ref="A176:M176"/>
-    <mergeCell ref="A177:M177"/>
-    <mergeCell ref="N176:AD176"/>
-    <mergeCell ref="N177:AD177"/>
-    <mergeCell ref="A186:M186"/>
-    <mergeCell ref="A187:M187"/>
-    <mergeCell ref="N186:AD186"/>
-    <mergeCell ref="N187:AD187"/>
-    <mergeCell ref="A184:M184"/>
-    <mergeCell ref="A185:M185"/>
-    <mergeCell ref="N184:AD184"/>
-    <mergeCell ref="N185:AD185"/>
-    <mergeCell ref="A182:M182"/>
-    <mergeCell ref="A183:M183"/>
-    <mergeCell ref="N182:AD182"/>
-    <mergeCell ref="N183:AD183"/>
-    <mergeCell ref="AE176:AJ176"/>
-    <mergeCell ref="AK176:AP176"/>
-    <mergeCell ref="AE187:AJ187"/>
-    <mergeCell ref="AK187:AP187"/>
-    <mergeCell ref="AE188:AJ188"/>
-    <mergeCell ref="AK188:AP188"/>
-    <mergeCell ref="AE189:AJ189"/>
-    <mergeCell ref="AK189:AP189"/>
-    <mergeCell ref="AE190:AJ190"/>
-    <mergeCell ref="AK190:AP190"/>
-    <mergeCell ref="AK193:AP193"/>
-    <mergeCell ref="A198:M198"/>
-    <mergeCell ref="A199:M199"/>
-    <mergeCell ref="N198:AD198"/>
-    <mergeCell ref="N199:AD199"/>
-    <mergeCell ref="A196:M196"/>
-    <mergeCell ref="A197:M197"/>
-    <mergeCell ref="N196:AD196"/>
-    <mergeCell ref="N197:AD197"/>
-    <mergeCell ref="A194:M194"/>
-    <mergeCell ref="A195:M195"/>
-    <mergeCell ref="N194:AD194"/>
-    <mergeCell ref="N195:AD195"/>
-    <mergeCell ref="A192:M192"/>
-    <mergeCell ref="A193:M193"/>
-    <mergeCell ref="N192:AD192"/>
-    <mergeCell ref="N193:AD193"/>
-    <mergeCell ref="A190:M190"/>
-    <mergeCell ref="A191:M191"/>
-    <mergeCell ref="N190:AD190"/>
-    <mergeCell ref="N191:AD191"/>
-    <mergeCell ref="A188:M188"/>
-    <mergeCell ref="A189:M189"/>
-    <mergeCell ref="N188:AD188"/>
-    <mergeCell ref="A204:M204"/>
-    <mergeCell ref="A205:M205"/>
-    <mergeCell ref="N204:AD204"/>
-    <mergeCell ref="N205:AD205"/>
-    <mergeCell ref="A202:M202"/>
-    <mergeCell ref="A203:M203"/>
-    <mergeCell ref="N202:AD202"/>
-    <mergeCell ref="N203:AD203"/>
-    <mergeCell ref="A200:M200"/>
-    <mergeCell ref="A201:M201"/>
-    <mergeCell ref="N200:AD200"/>
-    <mergeCell ref="N201:AD201"/>
-    <mergeCell ref="AE200:AJ200"/>
-    <mergeCell ref="AK200:AP200"/>
-    <mergeCell ref="AE201:AJ201"/>
-    <mergeCell ref="AK201:AP201"/>
-    <mergeCell ref="AE202:AJ202"/>
-    <mergeCell ref="AE205:AJ205"/>
-    <mergeCell ref="AK205:AP205"/>
-    <mergeCell ref="A210:M210"/>
-    <mergeCell ref="A211:M211"/>
-    <mergeCell ref="N210:AD210"/>
-    <mergeCell ref="N211:AD211"/>
-    <mergeCell ref="A208:M208"/>
-    <mergeCell ref="A209:M209"/>
-    <mergeCell ref="N208:AD208"/>
-    <mergeCell ref="N209:AD209"/>
-    <mergeCell ref="A206:M206"/>
-    <mergeCell ref="A207:M207"/>
-    <mergeCell ref="N206:AD206"/>
-    <mergeCell ref="N207:AD207"/>
-    <mergeCell ref="AE209:AJ209"/>
-    <mergeCell ref="AK209:AP209"/>
-    <mergeCell ref="AE210:AJ210"/>
-    <mergeCell ref="AK210:AP210"/>
-    <mergeCell ref="AE211:AJ211"/>
-    <mergeCell ref="AE206:AJ206"/>
-    <mergeCell ref="AK206:AP206"/>
-    <mergeCell ref="AE207:AJ207"/>
-    <mergeCell ref="AK207:AP207"/>
-    <mergeCell ref="AE208:AJ208"/>
-    <mergeCell ref="AK208:AP208"/>
-    <mergeCell ref="AK211:AP211"/>
-    <mergeCell ref="N225:AD225"/>
-    <mergeCell ref="AE227:AJ227"/>
-    <mergeCell ref="AK227:AP227"/>
-    <mergeCell ref="AE228:AJ228"/>
-    <mergeCell ref="AK228:AP228"/>
-    <mergeCell ref="AE229:AJ229"/>
-    <mergeCell ref="A216:M216"/>
-    <mergeCell ref="A217:M217"/>
-    <mergeCell ref="N216:AD216"/>
-    <mergeCell ref="N217:AD217"/>
-    <mergeCell ref="A214:M214"/>
-    <mergeCell ref="A215:M215"/>
-    <mergeCell ref="N214:AD214"/>
-    <mergeCell ref="N215:AD215"/>
-    <mergeCell ref="A212:M212"/>
-    <mergeCell ref="A213:M213"/>
-    <mergeCell ref="N212:AD212"/>
-    <mergeCell ref="N213:AD213"/>
-    <mergeCell ref="A222:M222"/>
-    <mergeCell ref="A223:M223"/>
-    <mergeCell ref="N222:AD222"/>
-    <mergeCell ref="N223:AD223"/>
-    <mergeCell ref="A220:M220"/>
-    <mergeCell ref="A221:M221"/>
-    <mergeCell ref="N220:AD220"/>
-    <mergeCell ref="N221:AD221"/>
-    <mergeCell ref="A218:M218"/>
-    <mergeCell ref="A219:M219"/>
-    <mergeCell ref="N218:AD218"/>
-    <mergeCell ref="N219:AD219"/>
-    <mergeCell ref="AE212:AJ212"/>
-    <mergeCell ref="AK212:AP212"/>
-    <mergeCell ref="AE223:AJ223"/>
-    <mergeCell ref="AK223:AP223"/>
-    <mergeCell ref="AE224:AJ224"/>
-    <mergeCell ref="AK224:AP224"/>
-    <mergeCell ref="AE225:AJ225"/>
-    <mergeCell ref="AK225:AP225"/>
-    <mergeCell ref="AE226:AJ226"/>
-    <mergeCell ref="AK226:AP226"/>
-    <mergeCell ref="AK229:AP229"/>
-    <mergeCell ref="A234:M234"/>
-    <mergeCell ref="A235:M235"/>
-    <mergeCell ref="N234:AD234"/>
-    <mergeCell ref="N235:AD235"/>
-    <mergeCell ref="A232:M232"/>
-    <mergeCell ref="A233:M233"/>
-    <mergeCell ref="N232:AD232"/>
-    <mergeCell ref="N233:AD233"/>
-    <mergeCell ref="A230:M230"/>
-    <mergeCell ref="A231:M231"/>
-    <mergeCell ref="N230:AD230"/>
-    <mergeCell ref="N231:AD231"/>
-    <mergeCell ref="A228:M228"/>
-    <mergeCell ref="A229:M229"/>
-    <mergeCell ref="N228:AD228"/>
-    <mergeCell ref="N229:AD229"/>
-    <mergeCell ref="A226:M226"/>
-    <mergeCell ref="A227:M227"/>
-    <mergeCell ref="N226:AD226"/>
-    <mergeCell ref="N227:AD227"/>
-    <mergeCell ref="A224:M224"/>
-    <mergeCell ref="A225:M225"/>
-    <mergeCell ref="N224:AD224"/>
-    <mergeCell ref="A240:M240"/>
-    <mergeCell ref="A241:M241"/>
-    <mergeCell ref="N240:AD240"/>
-    <mergeCell ref="N241:AD241"/>
-    <mergeCell ref="A238:M238"/>
-    <mergeCell ref="A239:M239"/>
-    <mergeCell ref="N238:AD238"/>
-    <mergeCell ref="N239:AD239"/>
-    <mergeCell ref="A236:M236"/>
-    <mergeCell ref="A237:M237"/>
-    <mergeCell ref="N236:AD236"/>
-    <mergeCell ref="N237:AD237"/>
-    <mergeCell ref="AE236:AJ236"/>
-    <mergeCell ref="AK236:AP236"/>
-    <mergeCell ref="AE237:AJ237"/>
-    <mergeCell ref="AK237:AP237"/>
-    <mergeCell ref="AE238:AJ238"/>
-    <mergeCell ref="AE241:AJ241"/>
-    <mergeCell ref="AK241:AP241"/>
-    <mergeCell ref="A246:M246"/>
-    <mergeCell ref="A247:M247"/>
-    <mergeCell ref="N246:AD246"/>
-    <mergeCell ref="N247:AD247"/>
-    <mergeCell ref="A244:M244"/>
-    <mergeCell ref="A245:M245"/>
-    <mergeCell ref="N244:AD244"/>
-    <mergeCell ref="N245:AD245"/>
-    <mergeCell ref="A242:M242"/>
-    <mergeCell ref="A243:M243"/>
-    <mergeCell ref="N242:AD242"/>
-    <mergeCell ref="N243:AD243"/>
-    <mergeCell ref="AE245:AJ245"/>
-    <mergeCell ref="AK245:AP245"/>
-    <mergeCell ref="AE246:AJ246"/>
-    <mergeCell ref="AK246:AP246"/>
-    <mergeCell ref="AE247:AJ247"/>
-    <mergeCell ref="AE242:AJ242"/>
-    <mergeCell ref="AK242:AP242"/>
-    <mergeCell ref="AE243:AJ243"/>
-    <mergeCell ref="AK243:AP243"/>
-    <mergeCell ref="AE244:AJ244"/>
-    <mergeCell ref="AK244:AP244"/>
-    <mergeCell ref="AK247:AP247"/>
-    <mergeCell ref="N261:AD261"/>
-    <mergeCell ref="AE263:AJ263"/>
-    <mergeCell ref="AK263:AP263"/>
-    <mergeCell ref="AE264:AJ264"/>
-    <mergeCell ref="AK264:AP264"/>
-    <mergeCell ref="AE265:AJ265"/>
-    <mergeCell ref="A252:M252"/>
-    <mergeCell ref="A253:M253"/>
-    <mergeCell ref="N252:AD252"/>
-    <mergeCell ref="N253:AD253"/>
-    <mergeCell ref="A250:M250"/>
-    <mergeCell ref="A251:M251"/>
-    <mergeCell ref="N250:AD250"/>
-    <mergeCell ref="N251:AD251"/>
-    <mergeCell ref="A248:M248"/>
-    <mergeCell ref="A249:M249"/>
-    <mergeCell ref="N248:AD248"/>
-    <mergeCell ref="N249:AD249"/>
-    <mergeCell ref="A258:M258"/>
-    <mergeCell ref="A259:M259"/>
-    <mergeCell ref="N258:AD258"/>
-    <mergeCell ref="N259:AD259"/>
-    <mergeCell ref="A256:M256"/>
-    <mergeCell ref="A257:M257"/>
-    <mergeCell ref="N256:AD256"/>
-    <mergeCell ref="N257:AD257"/>
-    <mergeCell ref="A254:M254"/>
-    <mergeCell ref="A255:M255"/>
-    <mergeCell ref="N254:AD254"/>
-    <mergeCell ref="N255:AD255"/>
-    <mergeCell ref="AE248:AJ248"/>
-    <mergeCell ref="AK248:AP248"/>
-    <mergeCell ref="AE259:AJ259"/>
-    <mergeCell ref="AK259:AP259"/>
-    <mergeCell ref="AE260:AJ260"/>
-    <mergeCell ref="AK260:AP260"/>
-    <mergeCell ref="AE261:AJ261"/>
-    <mergeCell ref="AK261:AP261"/>
-    <mergeCell ref="AE262:AJ262"/>
-    <mergeCell ref="AK262:AP262"/>
-    <mergeCell ref="AK265:AP265"/>
-    <mergeCell ref="A270:M270"/>
-    <mergeCell ref="A271:M271"/>
-    <mergeCell ref="N270:AD270"/>
-    <mergeCell ref="N271:AD271"/>
-    <mergeCell ref="A268:M268"/>
-    <mergeCell ref="A269:M269"/>
-    <mergeCell ref="N268:AD268"/>
-    <mergeCell ref="N269:AD269"/>
-    <mergeCell ref="A266:M266"/>
-    <mergeCell ref="A267:M267"/>
-    <mergeCell ref="N266:AD266"/>
-    <mergeCell ref="N267:AD267"/>
-    <mergeCell ref="A264:M264"/>
-    <mergeCell ref="A265:M265"/>
-    <mergeCell ref="N264:AD264"/>
-    <mergeCell ref="N265:AD265"/>
-    <mergeCell ref="A262:M262"/>
-    <mergeCell ref="A263:M263"/>
-    <mergeCell ref="N262:AD262"/>
-    <mergeCell ref="N263:AD263"/>
-    <mergeCell ref="A260:M260"/>
-    <mergeCell ref="A261:M261"/>
-    <mergeCell ref="N260:AD260"/>
-    <mergeCell ref="A276:M276"/>
-    <mergeCell ref="A277:M277"/>
-    <mergeCell ref="N276:AD276"/>
-    <mergeCell ref="N277:AD277"/>
-    <mergeCell ref="A274:M274"/>
-    <mergeCell ref="A275:M275"/>
-    <mergeCell ref="N274:AD274"/>
-    <mergeCell ref="N275:AD275"/>
-    <mergeCell ref="A272:M272"/>
-    <mergeCell ref="A273:M273"/>
-    <mergeCell ref="N272:AD272"/>
-    <mergeCell ref="N273:AD273"/>
-    <mergeCell ref="AE272:AJ272"/>
-    <mergeCell ref="AK272:AP272"/>
-    <mergeCell ref="AE273:AJ273"/>
-    <mergeCell ref="AK273:AP273"/>
-    <mergeCell ref="AE274:AJ274"/>
-    <mergeCell ref="AE277:AJ277"/>
-    <mergeCell ref="AK277:AP277"/>
-    <mergeCell ref="A282:M282"/>
-    <mergeCell ref="A283:M283"/>
-    <mergeCell ref="N282:AD282"/>
-    <mergeCell ref="N283:AD283"/>
-    <mergeCell ref="A280:M280"/>
-    <mergeCell ref="A281:M281"/>
-    <mergeCell ref="N280:AD280"/>
-    <mergeCell ref="N281:AD281"/>
-    <mergeCell ref="A278:M278"/>
-    <mergeCell ref="A279:M279"/>
-    <mergeCell ref="N278:AD278"/>
-    <mergeCell ref="N279:AD279"/>
-    <mergeCell ref="AE281:AJ281"/>
-    <mergeCell ref="AK281:AP281"/>
-    <mergeCell ref="AE282:AJ282"/>
-    <mergeCell ref="AK282:AP282"/>
-    <mergeCell ref="AE283:AJ283"/>
-    <mergeCell ref="AE278:AJ278"/>
-    <mergeCell ref="AK278:AP278"/>
-    <mergeCell ref="AE279:AJ279"/>
-    <mergeCell ref="AK279:AP279"/>
-    <mergeCell ref="AE280:AJ280"/>
-    <mergeCell ref="AK280:AP280"/>
-    <mergeCell ref="AK283:AP283"/>
-    <mergeCell ref="N297:AD297"/>
-    <mergeCell ref="AE299:AJ299"/>
-    <mergeCell ref="AK299:AP299"/>
-    <mergeCell ref="AE300:AJ300"/>
-    <mergeCell ref="AK300:AP300"/>
-    <mergeCell ref="AE301:AJ301"/>
-    <mergeCell ref="A288:M288"/>
-    <mergeCell ref="A289:M289"/>
-    <mergeCell ref="N288:AD288"/>
-    <mergeCell ref="N289:AD289"/>
-    <mergeCell ref="A286:M286"/>
-    <mergeCell ref="A287:M287"/>
-    <mergeCell ref="N286:AD286"/>
-    <mergeCell ref="N287:AD287"/>
-    <mergeCell ref="A284:M284"/>
-    <mergeCell ref="A285:M285"/>
-    <mergeCell ref="N284:AD284"/>
-    <mergeCell ref="N285:AD285"/>
-    <mergeCell ref="A294:M294"/>
-    <mergeCell ref="A295:M295"/>
-    <mergeCell ref="N294:AD294"/>
-    <mergeCell ref="N295:AD295"/>
-    <mergeCell ref="A292:M292"/>
-    <mergeCell ref="A293:M293"/>
-    <mergeCell ref="N292:AD292"/>
-    <mergeCell ref="N293:AD293"/>
-    <mergeCell ref="A290:M290"/>
-    <mergeCell ref="A291:M291"/>
-    <mergeCell ref="N290:AD290"/>
-    <mergeCell ref="N291:AD291"/>
-    <mergeCell ref="AE284:AJ284"/>
-    <mergeCell ref="AK284:AP284"/>
-    <mergeCell ref="AE295:AJ295"/>
-    <mergeCell ref="AK295:AP295"/>
-    <mergeCell ref="AE296:AJ296"/>
-    <mergeCell ref="AK296:AP296"/>
-    <mergeCell ref="AE297:AJ297"/>
-    <mergeCell ref="AK297:AP297"/>
-    <mergeCell ref="AE298:AJ298"/>
-    <mergeCell ref="AK298:AP298"/>
-    <mergeCell ref="AK301:AP301"/>
-    <mergeCell ref="A306:M306"/>
-    <mergeCell ref="A307:M307"/>
-    <mergeCell ref="N306:AD306"/>
-    <mergeCell ref="N307:AD307"/>
-    <mergeCell ref="A304:M304"/>
-    <mergeCell ref="A305:M305"/>
-    <mergeCell ref="N304:AD304"/>
-    <mergeCell ref="N305:AD305"/>
-    <mergeCell ref="A302:M302"/>
-    <mergeCell ref="A303:M303"/>
-    <mergeCell ref="N302:AD302"/>
-    <mergeCell ref="N303:AD303"/>
-    <mergeCell ref="A300:M300"/>
-    <mergeCell ref="A301:M301"/>
-    <mergeCell ref="N300:AD300"/>
-    <mergeCell ref="N301:AD301"/>
-    <mergeCell ref="A298:M298"/>
-    <mergeCell ref="A299:M299"/>
-    <mergeCell ref="N298:AD298"/>
-    <mergeCell ref="N299:AD299"/>
-    <mergeCell ref="A296:M296"/>
-    <mergeCell ref="A297:M297"/>
-    <mergeCell ref="N296:AD296"/>
-    <mergeCell ref="A312:M312"/>
-    <mergeCell ref="A313:M313"/>
-    <mergeCell ref="N312:AD312"/>
-    <mergeCell ref="N313:AD313"/>
-    <mergeCell ref="A310:M310"/>
-    <mergeCell ref="A311:M311"/>
-    <mergeCell ref="N310:AD310"/>
-    <mergeCell ref="N311:AD311"/>
-    <mergeCell ref="A308:M308"/>
-    <mergeCell ref="A309:M309"/>
-    <mergeCell ref="N308:AD308"/>
-    <mergeCell ref="N309:AD309"/>
-    <mergeCell ref="AE308:AJ308"/>
-    <mergeCell ref="AK308:AP308"/>
-    <mergeCell ref="AE309:AJ309"/>
-    <mergeCell ref="AK309:AP309"/>
-    <mergeCell ref="AE310:AJ310"/>
-    <mergeCell ref="AE313:AJ313"/>
-    <mergeCell ref="AK313:AP313"/>
-    <mergeCell ref="A318:M318"/>
-    <mergeCell ref="A319:M319"/>
-    <mergeCell ref="N318:AD318"/>
-    <mergeCell ref="N319:AD319"/>
-    <mergeCell ref="A316:M316"/>
-    <mergeCell ref="A317:M317"/>
-    <mergeCell ref="N316:AD316"/>
-    <mergeCell ref="N317:AD317"/>
-    <mergeCell ref="A314:M314"/>
-    <mergeCell ref="A315:M315"/>
-    <mergeCell ref="N314:AD314"/>
-    <mergeCell ref="N315:AD315"/>
-    <mergeCell ref="AE317:AJ317"/>
-    <mergeCell ref="AK317:AP317"/>
-    <mergeCell ref="AE318:AJ318"/>
-    <mergeCell ref="AK318:AP318"/>
-    <mergeCell ref="AE319:AJ319"/>
-    <mergeCell ref="AE314:AJ314"/>
-    <mergeCell ref="AK314:AP314"/>
-    <mergeCell ref="AE315:AJ315"/>
-    <mergeCell ref="AK315:AP315"/>
-    <mergeCell ref="AE316:AJ316"/>
-    <mergeCell ref="AK316:AP316"/>
-    <mergeCell ref="AK319:AP319"/>
-    <mergeCell ref="N333:AD333"/>
-    <mergeCell ref="AE335:AJ335"/>
-    <mergeCell ref="AK335:AP335"/>
-    <mergeCell ref="AE336:AJ336"/>
-    <mergeCell ref="AK336:AP336"/>
-    <mergeCell ref="AE337:AJ337"/>
-    <mergeCell ref="A324:M324"/>
-    <mergeCell ref="A325:M325"/>
-    <mergeCell ref="N324:AD324"/>
-    <mergeCell ref="N325:AD325"/>
-    <mergeCell ref="A322:M322"/>
-    <mergeCell ref="A323:M323"/>
-    <mergeCell ref="N322:AD322"/>
-    <mergeCell ref="N323:AD323"/>
-    <mergeCell ref="A320:M320"/>
-    <mergeCell ref="A321:M321"/>
-    <mergeCell ref="N320:AD320"/>
-    <mergeCell ref="N321:AD321"/>
-    <mergeCell ref="A330:M330"/>
-    <mergeCell ref="A331:M331"/>
-    <mergeCell ref="N330:AD330"/>
-    <mergeCell ref="N331:AD331"/>
-    <mergeCell ref="A328:M328"/>
-    <mergeCell ref="A329:M329"/>
-    <mergeCell ref="N328:AD328"/>
-    <mergeCell ref="N329:AD329"/>
-    <mergeCell ref="A326:M326"/>
-    <mergeCell ref="A327:M327"/>
-    <mergeCell ref="N326:AD326"/>
-    <mergeCell ref="N327:AD327"/>
-    <mergeCell ref="AE320:AJ320"/>
-    <mergeCell ref="AK320:AP320"/>
-    <mergeCell ref="AE331:AJ331"/>
-    <mergeCell ref="AK331:AP331"/>
-    <mergeCell ref="AE332:AJ332"/>
-    <mergeCell ref="AK332:AP332"/>
-    <mergeCell ref="AE333:AJ333"/>
-    <mergeCell ref="AK333:AP333"/>
-    <mergeCell ref="AE334:AJ334"/>
-    <mergeCell ref="AK334:AP334"/>
-    <mergeCell ref="AK337:AP337"/>
-    <mergeCell ref="A342:M342"/>
-    <mergeCell ref="A343:M343"/>
-    <mergeCell ref="N342:AD342"/>
-    <mergeCell ref="N343:AD343"/>
-    <mergeCell ref="A340:M340"/>
-    <mergeCell ref="A341:M341"/>
-    <mergeCell ref="N340:AD340"/>
-    <mergeCell ref="N341:AD341"/>
-    <mergeCell ref="A338:M338"/>
-    <mergeCell ref="A339:M339"/>
-    <mergeCell ref="N338:AD338"/>
-    <mergeCell ref="N339:AD339"/>
-    <mergeCell ref="A336:M336"/>
-    <mergeCell ref="A337:M337"/>
-    <mergeCell ref="N336:AD336"/>
-    <mergeCell ref="N337:AD337"/>
-    <mergeCell ref="A334:M334"/>
-    <mergeCell ref="A335:M335"/>
-    <mergeCell ref="N334:AD334"/>
-    <mergeCell ref="N335:AD335"/>
-    <mergeCell ref="A332:M332"/>
-    <mergeCell ref="A333:M333"/>
-    <mergeCell ref="N332:AD332"/>
-    <mergeCell ref="A348:M348"/>
-    <mergeCell ref="A349:M349"/>
-    <mergeCell ref="N348:AD348"/>
-    <mergeCell ref="N349:AD349"/>
-    <mergeCell ref="A346:M346"/>
-    <mergeCell ref="A347:M347"/>
-    <mergeCell ref="N346:AD346"/>
-    <mergeCell ref="N347:AD347"/>
-    <mergeCell ref="A344:M344"/>
-    <mergeCell ref="A345:M345"/>
-    <mergeCell ref="N344:AD344"/>
-    <mergeCell ref="N345:AD345"/>
-    <mergeCell ref="AE344:AJ344"/>
-    <mergeCell ref="AK344:AP344"/>
-    <mergeCell ref="AE345:AJ345"/>
-    <mergeCell ref="AK345:AP345"/>
-    <mergeCell ref="AE346:AJ346"/>
-    <mergeCell ref="AE349:AJ349"/>
-    <mergeCell ref="AK349:AP349"/>
-    <mergeCell ref="A354:M354"/>
-    <mergeCell ref="A355:M355"/>
-    <mergeCell ref="N354:AD354"/>
-    <mergeCell ref="N355:AD355"/>
-    <mergeCell ref="A352:M352"/>
-    <mergeCell ref="A353:M353"/>
-    <mergeCell ref="N352:AD352"/>
-    <mergeCell ref="N353:AD353"/>
-    <mergeCell ref="A350:M350"/>
-    <mergeCell ref="A351:M351"/>
-    <mergeCell ref="N350:AD350"/>
-    <mergeCell ref="N351:AD351"/>
-    <mergeCell ref="AE353:AJ353"/>
-    <mergeCell ref="AK353:AP353"/>
-    <mergeCell ref="AE354:AJ354"/>
-    <mergeCell ref="AK354:AP354"/>
-    <mergeCell ref="AE355:AJ355"/>
-    <mergeCell ref="AE350:AJ350"/>
-    <mergeCell ref="AK350:AP350"/>
-    <mergeCell ref="AE351:AJ351"/>
-    <mergeCell ref="AK351:AP351"/>
-    <mergeCell ref="AE352:AJ352"/>
-    <mergeCell ref="AK352:AP352"/>
-    <mergeCell ref="AK355:AP355"/>
-    <mergeCell ref="N369:AD369"/>
-    <mergeCell ref="AE371:AJ371"/>
-    <mergeCell ref="AK371:AP371"/>
-    <mergeCell ref="AE372:AJ372"/>
-    <mergeCell ref="AK372:AP372"/>
-    <mergeCell ref="AE373:AJ373"/>
-    <mergeCell ref="A360:M360"/>
-    <mergeCell ref="A361:M361"/>
-    <mergeCell ref="N360:AD360"/>
-    <mergeCell ref="N361:AD361"/>
-    <mergeCell ref="A358:M358"/>
-    <mergeCell ref="A359:M359"/>
-    <mergeCell ref="N358:AD358"/>
-    <mergeCell ref="N359:AD359"/>
-    <mergeCell ref="A356:M356"/>
-    <mergeCell ref="A357:M357"/>
-    <mergeCell ref="N356:AD356"/>
-    <mergeCell ref="N357:AD357"/>
-    <mergeCell ref="A366:M366"/>
-    <mergeCell ref="A367:M367"/>
-    <mergeCell ref="N366:AD366"/>
-    <mergeCell ref="N367:AD367"/>
-    <mergeCell ref="A364:M364"/>
-    <mergeCell ref="A365:M365"/>
-    <mergeCell ref="N364:AD364"/>
-    <mergeCell ref="N365:AD365"/>
-    <mergeCell ref="A362:M362"/>
-    <mergeCell ref="A363:M363"/>
-    <mergeCell ref="N362:AD362"/>
-    <mergeCell ref="N363:AD363"/>
-    <mergeCell ref="AE356:AJ356"/>
-    <mergeCell ref="AK356:AP356"/>
-    <mergeCell ref="AE367:AJ367"/>
-    <mergeCell ref="AK367:AP367"/>
-    <mergeCell ref="AE368:AJ368"/>
-    <mergeCell ref="AK368:AP368"/>
-    <mergeCell ref="AE369:AJ369"/>
-    <mergeCell ref="AK369:AP369"/>
-    <mergeCell ref="AE370:AJ370"/>
-    <mergeCell ref="AK370:AP370"/>
-    <mergeCell ref="AK373:AP373"/>
-    <mergeCell ref="A378:M378"/>
-    <mergeCell ref="A379:M379"/>
-    <mergeCell ref="N378:AD378"/>
-    <mergeCell ref="N379:AD379"/>
-    <mergeCell ref="A376:M376"/>
-    <mergeCell ref="A377:M377"/>
-    <mergeCell ref="N376:AD376"/>
-    <mergeCell ref="N377:AD377"/>
-    <mergeCell ref="A374:M374"/>
-    <mergeCell ref="A375:M375"/>
-    <mergeCell ref="N374:AD374"/>
-    <mergeCell ref="N375:AD375"/>
-    <mergeCell ref="A372:M372"/>
-    <mergeCell ref="A373:M373"/>
-    <mergeCell ref="N372:AD372"/>
-    <mergeCell ref="N373:AD373"/>
-    <mergeCell ref="A370:M370"/>
-    <mergeCell ref="A371:M371"/>
-    <mergeCell ref="N370:AD370"/>
-    <mergeCell ref="N371:AD371"/>
-    <mergeCell ref="A368:M368"/>
-    <mergeCell ref="A369:M369"/>
-    <mergeCell ref="N368:AD368"/>
-    <mergeCell ref="A384:M384"/>
-    <mergeCell ref="A385:M385"/>
-    <mergeCell ref="N384:AD384"/>
-    <mergeCell ref="N385:AD385"/>
-    <mergeCell ref="A382:M382"/>
-    <mergeCell ref="A383:M383"/>
-    <mergeCell ref="N382:AD382"/>
-    <mergeCell ref="N383:AD383"/>
-    <mergeCell ref="A380:M380"/>
-    <mergeCell ref="A381:M381"/>
-    <mergeCell ref="N380:AD380"/>
-    <mergeCell ref="N381:AD381"/>
-    <mergeCell ref="AE380:AJ380"/>
-    <mergeCell ref="AK380:AP380"/>
-    <mergeCell ref="AE381:AJ381"/>
-    <mergeCell ref="AK381:AP381"/>
-    <mergeCell ref="AE382:AJ382"/>
-    <mergeCell ref="AE385:AJ385"/>
-    <mergeCell ref="AK385:AP385"/>
-    <mergeCell ref="A390:M390"/>
-    <mergeCell ref="A391:M391"/>
-    <mergeCell ref="N390:AD390"/>
-    <mergeCell ref="N391:AD391"/>
-    <mergeCell ref="A388:M388"/>
-    <mergeCell ref="A389:M389"/>
-    <mergeCell ref="N388:AD388"/>
-    <mergeCell ref="N389:AD389"/>
-    <mergeCell ref="A386:M386"/>
-    <mergeCell ref="A387:M387"/>
-    <mergeCell ref="N386:AD386"/>
-    <mergeCell ref="N387:AD387"/>
-    <mergeCell ref="AE389:AJ389"/>
-    <mergeCell ref="AK389:AP389"/>
-    <mergeCell ref="AE390:AJ390"/>
-    <mergeCell ref="AK390:AP390"/>
-    <mergeCell ref="AE391:AJ391"/>
-    <mergeCell ref="AE386:AJ386"/>
-    <mergeCell ref="AK386:AP386"/>
-    <mergeCell ref="AE387:AJ387"/>
-    <mergeCell ref="AK387:AP387"/>
-    <mergeCell ref="AE388:AJ388"/>
-    <mergeCell ref="AK388:AP388"/>
-    <mergeCell ref="AK391:AP391"/>
-    <mergeCell ref="N405:AD405"/>
-    <mergeCell ref="AE407:AJ407"/>
-    <mergeCell ref="AK407:AP407"/>
-    <mergeCell ref="AE408:AJ408"/>
-    <mergeCell ref="AK408:AP408"/>
-    <mergeCell ref="AE409:AJ409"/>
-    <mergeCell ref="A396:M396"/>
-    <mergeCell ref="A397:M397"/>
-    <mergeCell ref="N396:AD396"/>
-    <mergeCell ref="N397:AD397"/>
-    <mergeCell ref="A394:M394"/>
-    <mergeCell ref="A395:M395"/>
-    <mergeCell ref="N394:AD394"/>
-    <mergeCell ref="N395:AD395"/>
-    <mergeCell ref="A392:M392"/>
-    <mergeCell ref="A393:M393"/>
-    <mergeCell ref="N392:AD392"/>
-    <mergeCell ref="N393:AD393"/>
-    <mergeCell ref="A402:M402"/>
-    <mergeCell ref="A403:M403"/>
-    <mergeCell ref="N402:AD402"/>
-    <mergeCell ref="N403:AD403"/>
-    <mergeCell ref="A400:M400"/>
-    <mergeCell ref="A401:M401"/>
-    <mergeCell ref="N400:AD400"/>
-    <mergeCell ref="N401:AD401"/>
-    <mergeCell ref="A398:M398"/>
-    <mergeCell ref="A399:M399"/>
-    <mergeCell ref="N398:AD398"/>
-    <mergeCell ref="N399:AD399"/>
-    <mergeCell ref="AE392:AJ392"/>
-    <mergeCell ref="AK392:AP392"/>
-    <mergeCell ref="AE403:AJ403"/>
-    <mergeCell ref="AK403:AP403"/>
-    <mergeCell ref="AE404:AJ404"/>
-    <mergeCell ref="AK404:AP404"/>
-    <mergeCell ref="AE405:AJ405"/>
-    <mergeCell ref="AK405:AP405"/>
-    <mergeCell ref="AE406:AJ406"/>
-    <mergeCell ref="AK406:AP406"/>
-    <mergeCell ref="AK409:AP409"/>
-    <mergeCell ref="A414:M414"/>
-    <mergeCell ref="A415:M415"/>
-    <mergeCell ref="N414:AD414"/>
-    <mergeCell ref="N415:AD415"/>
-    <mergeCell ref="A412:M412"/>
-    <mergeCell ref="A413:M413"/>
-    <mergeCell ref="N412:AD412"/>
-    <mergeCell ref="N413:AD413"/>
-    <mergeCell ref="A410:M410"/>
-    <mergeCell ref="A411:M411"/>
-    <mergeCell ref="N410:AD410"/>
-    <mergeCell ref="N411:AD411"/>
-    <mergeCell ref="A408:M408"/>
-    <mergeCell ref="A409:M409"/>
-    <mergeCell ref="N408:AD408"/>
-    <mergeCell ref="N409:AD409"/>
-    <mergeCell ref="A406:M406"/>
-    <mergeCell ref="A407:M407"/>
-    <mergeCell ref="N406:AD406"/>
-    <mergeCell ref="N407:AD407"/>
-    <mergeCell ref="A404:M404"/>
-    <mergeCell ref="A405:M405"/>
-    <mergeCell ref="N404:AD404"/>
-    <mergeCell ref="A420:M420"/>
-    <mergeCell ref="A421:M421"/>
-    <mergeCell ref="N420:AD420"/>
-    <mergeCell ref="N421:AD421"/>
-    <mergeCell ref="A418:M418"/>
-    <mergeCell ref="A419:M419"/>
-    <mergeCell ref="N418:AD418"/>
-    <mergeCell ref="N419:AD419"/>
-    <mergeCell ref="A416:M416"/>
-    <mergeCell ref="A417:M417"/>
-    <mergeCell ref="N416:AD416"/>
-    <mergeCell ref="N417:AD417"/>
-    <mergeCell ref="AE416:AJ416"/>
-    <mergeCell ref="AK416:AP416"/>
-    <mergeCell ref="AE417:AJ417"/>
-    <mergeCell ref="AK417:AP417"/>
-    <mergeCell ref="AE418:AJ418"/>
-    <mergeCell ref="AE421:AJ421"/>
-    <mergeCell ref="AK421:AP421"/>
-    <mergeCell ref="A426:M426"/>
-    <mergeCell ref="A427:M427"/>
-    <mergeCell ref="N426:AD426"/>
-    <mergeCell ref="N427:AD427"/>
-    <mergeCell ref="A424:M424"/>
-    <mergeCell ref="A425:M425"/>
-    <mergeCell ref="N424:AD424"/>
-    <mergeCell ref="N425:AD425"/>
-    <mergeCell ref="A422:M422"/>
-    <mergeCell ref="A423:M423"/>
-    <mergeCell ref="N422:AD422"/>
-    <mergeCell ref="N423:AD423"/>
-    <mergeCell ref="AE425:AJ425"/>
-    <mergeCell ref="AK425:AP425"/>
-    <mergeCell ref="AE426:AJ426"/>
-    <mergeCell ref="AK426:AP426"/>
-    <mergeCell ref="AE427:AJ427"/>
-    <mergeCell ref="AE422:AJ422"/>
-    <mergeCell ref="AK422:AP422"/>
-    <mergeCell ref="AE423:AJ423"/>
-    <mergeCell ref="AK423:AP423"/>
-    <mergeCell ref="AE424:AJ424"/>
-    <mergeCell ref="AK424:AP424"/>
-    <mergeCell ref="AK427:AP427"/>
-    <mergeCell ref="N441:AD441"/>
-    <mergeCell ref="AE443:AJ443"/>
-    <mergeCell ref="AK443:AP443"/>
-    <mergeCell ref="AE444:AJ444"/>
-    <mergeCell ref="AK444:AP444"/>
-    <mergeCell ref="AE445:AJ445"/>
-    <mergeCell ref="A432:M432"/>
-    <mergeCell ref="A433:M433"/>
-    <mergeCell ref="N432:AD432"/>
-    <mergeCell ref="N433:AD433"/>
-    <mergeCell ref="A430:M430"/>
-    <mergeCell ref="A431:M431"/>
-    <mergeCell ref="N430:AD430"/>
-    <mergeCell ref="N431:AD431"/>
-    <mergeCell ref="A428:M428"/>
-    <mergeCell ref="A429:M429"/>
-    <mergeCell ref="N428:AD428"/>
-    <mergeCell ref="N429:AD429"/>
-    <mergeCell ref="A438:M438"/>
-    <mergeCell ref="A439:M439"/>
-    <mergeCell ref="N438:AD438"/>
-    <mergeCell ref="N439:AD439"/>
-    <mergeCell ref="A436:M436"/>
-    <mergeCell ref="A437:M437"/>
-    <mergeCell ref="N436:AD436"/>
-    <mergeCell ref="N437:AD437"/>
-    <mergeCell ref="A434:M434"/>
-    <mergeCell ref="A435:M435"/>
-    <mergeCell ref="N434:AD434"/>
-    <mergeCell ref="N435:AD435"/>
-    <mergeCell ref="AE428:AJ428"/>
-    <mergeCell ref="AK428:AP428"/>
-    <mergeCell ref="AE439:AJ439"/>
-    <mergeCell ref="AK439:AP439"/>
-    <mergeCell ref="AE440:AJ440"/>
-    <mergeCell ref="AK440:AP440"/>
-    <mergeCell ref="AE441:AJ441"/>
-    <mergeCell ref="AK441:AP441"/>
-    <mergeCell ref="AE442:AJ442"/>
-    <mergeCell ref="AK442:AP442"/>
-    <mergeCell ref="AK445:AP445"/>
-    <mergeCell ref="A450:M450"/>
-    <mergeCell ref="A451:M451"/>
-    <mergeCell ref="N450:AD450"/>
-    <mergeCell ref="N451:AD451"/>
-    <mergeCell ref="A448:M448"/>
-    <mergeCell ref="A449:M449"/>
-    <mergeCell ref="N448:AD448"/>
-    <mergeCell ref="N449:AD449"/>
-    <mergeCell ref="A446:M446"/>
-    <mergeCell ref="A447:M447"/>
-    <mergeCell ref="N446:AD446"/>
-    <mergeCell ref="N447:AD447"/>
-    <mergeCell ref="A444:M444"/>
-    <mergeCell ref="A445:M445"/>
-    <mergeCell ref="N444:AD444"/>
-    <mergeCell ref="N445:AD445"/>
-    <mergeCell ref="A442:M442"/>
-    <mergeCell ref="A443:M443"/>
-    <mergeCell ref="N442:AD442"/>
-    <mergeCell ref="N443:AD443"/>
-    <mergeCell ref="A440:M440"/>
-    <mergeCell ref="A441:M441"/>
-    <mergeCell ref="N440:AD440"/>
-    <mergeCell ref="A456:M456"/>
-    <mergeCell ref="A457:M457"/>
-    <mergeCell ref="N456:AD456"/>
-    <mergeCell ref="N457:AD457"/>
-    <mergeCell ref="A454:M454"/>
-    <mergeCell ref="A455:M455"/>
-    <mergeCell ref="N454:AD454"/>
-    <mergeCell ref="N455:AD455"/>
-    <mergeCell ref="A452:M452"/>
-    <mergeCell ref="A453:M453"/>
-    <mergeCell ref="N452:AD452"/>
-    <mergeCell ref="N453:AD453"/>
-    <mergeCell ref="AE452:AJ452"/>
-    <mergeCell ref="AK452:AP452"/>
-    <mergeCell ref="AE453:AJ453"/>
-    <mergeCell ref="AK453:AP453"/>
-    <mergeCell ref="AE454:AJ454"/>
-    <mergeCell ref="AE457:AJ457"/>
-    <mergeCell ref="AK457:AP457"/>
-    <mergeCell ref="A462:M462"/>
-    <mergeCell ref="A463:M463"/>
-    <mergeCell ref="N462:AD462"/>
-    <mergeCell ref="N463:AD463"/>
-    <mergeCell ref="A460:M460"/>
-    <mergeCell ref="A461:M461"/>
-    <mergeCell ref="N460:AD460"/>
-    <mergeCell ref="N461:AD461"/>
-    <mergeCell ref="A458:M458"/>
-    <mergeCell ref="A459:M459"/>
-    <mergeCell ref="N458:AD458"/>
-    <mergeCell ref="N459:AD459"/>
-    <mergeCell ref="AE461:AJ461"/>
-    <mergeCell ref="AK461:AP461"/>
-    <mergeCell ref="AE462:AJ462"/>
-    <mergeCell ref="AK462:AP462"/>
-    <mergeCell ref="AE463:AJ463"/>
-    <mergeCell ref="AE458:AJ458"/>
-    <mergeCell ref="AK458:AP458"/>
-    <mergeCell ref="AE459:AJ459"/>
-    <mergeCell ref="AK459:AP459"/>
-    <mergeCell ref="AE460:AJ460"/>
-    <mergeCell ref="AK460:AP460"/>
-    <mergeCell ref="AK463:AP463"/>
-    <mergeCell ref="N477:AD477"/>
-    <mergeCell ref="AE479:AJ479"/>
-    <mergeCell ref="AK479:AP479"/>
-    <mergeCell ref="AE480:AJ480"/>
-    <mergeCell ref="AK480:AP480"/>
-    <mergeCell ref="AE481:AJ481"/>
-    <mergeCell ref="A468:M468"/>
-    <mergeCell ref="A469:M469"/>
-    <mergeCell ref="N468:AD468"/>
-    <mergeCell ref="N469:AD469"/>
-    <mergeCell ref="A466:M466"/>
-    <mergeCell ref="A467:M467"/>
-    <mergeCell ref="N466:AD466"/>
-    <mergeCell ref="N467:AD467"/>
-    <mergeCell ref="A464:M464"/>
-    <mergeCell ref="A465:M465"/>
-    <mergeCell ref="N464:AD464"/>
-    <mergeCell ref="N465:AD465"/>
-    <mergeCell ref="A474:M474"/>
-    <mergeCell ref="A475:M475"/>
-    <mergeCell ref="N474:AD474"/>
-    <mergeCell ref="N475:AD475"/>
-    <mergeCell ref="A472:M472"/>
-    <mergeCell ref="A473:M473"/>
-    <mergeCell ref="N472:AD472"/>
-    <mergeCell ref="N473:AD473"/>
-    <mergeCell ref="A470:M470"/>
-    <mergeCell ref="A471:M471"/>
-    <mergeCell ref="N470:AD470"/>
-    <mergeCell ref="N471:AD471"/>
-    <mergeCell ref="AE464:AJ464"/>
-    <mergeCell ref="AK464:AP464"/>
-    <mergeCell ref="AE475:AJ475"/>
-    <mergeCell ref="AK475:AP475"/>
-    <mergeCell ref="AE476:AJ476"/>
-    <mergeCell ref="AK476:AP476"/>
-    <mergeCell ref="AE477:AJ477"/>
-    <mergeCell ref="AK477:AP477"/>
-    <mergeCell ref="AE478:AJ478"/>
-    <mergeCell ref="AK478:AP478"/>
-    <mergeCell ref="AK481:AP481"/>
-    <mergeCell ref="A486:M486"/>
-    <mergeCell ref="A487:M487"/>
-    <mergeCell ref="N486:AD486"/>
-    <mergeCell ref="N487:AD487"/>
-    <mergeCell ref="A484:M484"/>
-    <mergeCell ref="A485:M485"/>
-    <mergeCell ref="N484:AD484"/>
-    <mergeCell ref="N485:AD485"/>
-    <mergeCell ref="A482:M482"/>
-    <mergeCell ref="A483:M483"/>
-    <mergeCell ref="N482:AD482"/>
-    <mergeCell ref="N483:AD483"/>
-    <mergeCell ref="A480:M480"/>
-    <mergeCell ref="A481:M481"/>
-    <mergeCell ref="N480:AD480"/>
-    <mergeCell ref="N481:AD481"/>
-    <mergeCell ref="A478:M478"/>
-    <mergeCell ref="A479:M479"/>
-    <mergeCell ref="N478:AD478"/>
-    <mergeCell ref="N479:AD479"/>
-    <mergeCell ref="A476:M476"/>
-    <mergeCell ref="A477:M477"/>
-    <mergeCell ref="N476:AD476"/>
-    <mergeCell ref="A492:M492"/>
-    <mergeCell ref="A493:M493"/>
-    <mergeCell ref="N492:AD492"/>
-    <mergeCell ref="N493:AD493"/>
-    <mergeCell ref="A490:M490"/>
-    <mergeCell ref="A491:M491"/>
-    <mergeCell ref="N490:AD490"/>
-    <mergeCell ref="N491:AD491"/>
-    <mergeCell ref="A488:M488"/>
-    <mergeCell ref="A489:M489"/>
-    <mergeCell ref="N488:AD488"/>
-    <mergeCell ref="N489:AD489"/>
-    <mergeCell ref="AE488:AJ488"/>
-    <mergeCell ref="AK488:AP488"/>
-    <mergeCell ref="AE489:AJ489"/>
-    <mergeCell ref="AK489:AP489"/>
-    <mergeCell ref="AE490:AJ490"/>
-    <mergeCell ref="AE493:AJ493"/>
-    <mergeCell ref="AK493:AP493"/>
-    <mergeCell ref="A498:M498"/>
-    <mergeCell ref="A499:M499"/>
-    <mergeCell ref="N498:AD498"/>
-    <mergeCell ref="N499:AD499"/>
-    <mergeCell ref="A496:M496"/>
-    <mergeCell ref="A497:M497"/>
-    <mergeCell ref="N496:AD496"/>
-    <mergeCell ref="N497:AD497"/>
-    <mergeCell ref="A494:M494"/>
-    <mergeCell ref="A495:M495"/>
-    <mergeCell ref="N494:AD494"/>
-    <mergeCell ref="N495:AD495"/>
-    <mergeCell ref="AE497:AJ497"/>
-    <mergeCell ref="AK497:AP497"/>
-    <mergeCell ref="AE498:AJ498"/>
-    <mergeCell ref="AK498:AP498"/>
-    <mergeCell ref="AE499:AJ499"/>
-    <mergeCell ref="AE494:AJ494"/>
-    <mergeCell ref="AK494:AP494"/>
-    <mergeCell ref="AE495:AJ495"/>
-    <mergeCell ref="AK495:AP495"/>
-    <mergeCell ref="AE496:AJ496"/>
-    <mergeCell ref="AK496:AP496"/>
-    <mergeCell ref="AK499:AP499"/>
-    <mergeCell ref="N513:AD513"/>
-    <mergeCell ref="AE515:AJ515"/>
-    <mergeCell ref="AK515:AP515"/>
-    <mergeCell ref="AE516:AJ516"/>
-    <mergeCell ref="AK516:AP516"/>
-    <mergeCell ref="AE517:AJ517"/>
-    <mergeCell ref="A504:M504"/>
-    <mergeCell ref="A505:M505"/>
-    <mergeCell ref="N504:AD504"/>
-    <mergeCell ref="N505:AD505"/>
-    <mergeCell ref="A502:M502"/>
-    <mergeCell ref="A503:M503"/>
-    <mergeCell ref="N502:AD502"/>
-    <mergeCell ref="N503:AD503"/>
-    <mergeCell ref="A500:M500"/>
-    <mergeCell ref="A501:M501"/>
-    <mergeCell ref="N500:AD500"/>
-    <mergeCell ref="N501:AD501"/>
-    <mergeCell ref="A510:M510"/>
-    <mergeCell ref="A511:M511"/>
-    <mergeCell ref="N510:AD510"/>
-    <mergeCell ref="N511:AD511"/>
-    <mergeCell ref="A508:M508"/>
-    <mergeCell ref="A509:M509"/>
-    <mergeCell ref="N508:AD508"/>
-    <mergeCell ref="N509:AD509"/>
-    <mergeCell ref="A506:M506"/>
-    <mergeCell ref="A507:M507"/>
-    <mergeCell ref="N506:AD506"/>
-    <mergeCell ref="N507:AD507"/>
-    <mergeCell ref="AE500:AJ500"/>
-    <mergeCell ref="AK500:AP500"/>
-    <mergeCell ref="AE511:AJ511"/>
-    <mergeCell ref="AK511:AP511"/>
-    <mergeCell ref="AE512:AJ512"/>
-    <mergeCell ref="AK512:AP512"/>
-    <mergeCell ref="AE513:AJ513"/>
-    <mergeCell ref="AK513:AP513"/>
-    <mergeCell ref="AE514:AJ514"/>
-    <mergeCell ref="AK514:AP514"/>
-    <mergeCell ref="AK517:AP517"/>
-    <mergeCell ref="A522:M522"/>
-    <mergeCell ref="A523:M523"/>
-    <mergeCell ref="N522:AD522"/>
-    <mergeCell ref="N523:AD523"/>
-    <mergeCell ref="A520:M520"/>
-    <mergeCell ref="A521:M521"/>
-    <mergeCell ref="N520:AD520"/>
-    <mergeCell ref="N521:AD521"/>
-    <mergeCell ref="A518:M518"/>
-    <mergeCell ref="A519:M519"/>
-    <mergeCell ref="N518:AD518"/>
-    <mergeCell ref="N519:AD519"/>
-    <mergeCell ref="A516:M516"/>
-    <mergeCell ref="A517:M517"/>
-    <mergeCell ref="N516:AD516"/>
-    <mergeCell ref="N517:AD517"/>
-    <mergeCell ref="A514:M514"/>
-    <mergeCell ref="A515:M515"/>
-    <mergeCell ref="N514:AD514"/>
-    <mergeCell ref="N515:AD515"/>
-    <mergeCell ref="A512:M512"/>
-    <mergeCell ref="A513:M513"/>
-    <mergeCell ref="N512:AD512"/>
-    <mergeCell ref="A528:M528"/>
-    <mergeCell ref="A529:M529"/>
-    <mergeCell ref="N528:AD528"/>
-    <mergeCell ref="N529:AD529"/>
-    <mergeCell ref="A526:M526"/>
-    <mergeCell ref="A527:M527"/>
-    <mergeCell ref="N526:AD526"/>
-    <mergeCell ref="N527:AD527"/>
-    <mergeCell ref="A524:M524"/>
-    <mergeCell ref="A525:M525"/>
-    <mergeCell ref="N524:AD524"/>
-    <mergeCell ref="N525:AD525"/>
-    <mergeCell ref="AE524:AJ524"/>
-    <mergeCell ref="AK524:AP524"/>
-    <mergeCell ref="AE525:AJ525"/>
-    <mergeCell ref="AK525:AP525"/>
-    <mergeCell ref="AE526:AJ526"/>
-    <mergeCell ref="AE529:AJ529"/>
-    <mergeCell ref="AK529:AP529"/>
-    <mergeCell ref="A534:M534"/>
-    <mergeCell ref="A535:M535"/>
-    <mergeCell ref="N534:AD534"/>
-    <mergeCell ref="N535:AD535"/>
-    <mergeCell ref="A532:M532"/>
-    <mergeCell ref="A533:M533"/>
-    <mergeCell ref="N532:AD532"/>
-    <mergeCell ref="N533:AD533"/>
-    <mergeCell ref="A530:M530"/>
-    <mergeCell ref="A531:M531"/>
-    <mergeCell ref="N530:AD530"/>
-    <mergeCell ref="N531:AD531"/>
-    <mergeCell ref="AE533:AJ533"/>
-    <mergeCell ref="AK533:AP533"/>
-    <mergeCell ref="AE534:AJ534"/>
-    <mergeCell ref="AK534:AP534"/>
-    <mergeCell ref="AE535:AJ535"/>
-    <mergeCell ref="AE530:AJ530"/>
-    <mergeCell ref="AK530:AP530"/>
-    <mergeCell ref="AE531:AJ531"/>
-    <mergeCell ref="AK531:AP531"/>
-    <mergeCell ref="AE532:AJ532"/>
-    <mergeCell ref="AK532:AP532"/>
-    <mergeCell ref="AK535:AP535"/>
-    <mergeCell ref="N549:AD549"/>
-    <mergeCell ref="AE551:AJ551"/>
-    <mergeCell ref="AK551:AP551"/>
-    <mergeCell ref="AE552:AJ552"/>
-    <mergeCell ref="AK552:AP552"/>
-    <mergeCell ref="AE553:AJ553"/>
-    <mergeCell ref="A540:M540"/>
-    <mergeCell ref="A541:M541"/>
-    <mergeCell ref="N540:AD540"/>
-    <mergeCell ref="N541:AD541"/>
-    <mergeCell ref="A538:M538"/>
-    <mergeCell ref="A539:M539"/>
-    <mergeCell ref="N538:AD538"/>
-    <mergeCell ref="N539:AD539"/>
-    <mergeCell ref="A536:M536"/>
-    <mergeCell ref="A537:M537"/>
-    <mergeCell ref="N536:AD536"/>
-    <mergeCell ref="N537:AD537"/>
-    <mergeCell ref="A546:M546"/>
-    <mergeCell ref="A547:M547"/>
-    <mergeCell ref="N546:AD546"/>
-    <mergeCell ref="N547:AD547"/>
-    <mergeCell ref="A544:M544"/>
-    <mergeCell ref="A545:M545"/>
-    <mergeCell ref="N544:AD544"/>
-    <mergeCell ref="N545:AD545"/>
-    <mergeCell ref="A542:M542"/>
-    <mergeCell ref="A543:M543"/>
-    <mergeCell ref="N542:AD542"/>
-    <mergeCell ref="N543:AD543"/>
-    <mergeCell ref="AE536:AJ536"/>
-    <mergeCell ref="AK536:AP536"/>
-    <mergeCell ref="AE547:AJ547"/>
-    <mergeCell ref="AK547:AP547"/>
-    <mergeCell ref="AE548:AJ548"/>
-    <mergeCell ref="AK548:AP548"/>
-    <mergeCell ref="AE549:AJ549"/>
-    <mergeCell ref="AK549:AP549"/>
-    <mergeCell ref="AE550:AJ550"/>
-    <mergeCell ref="AK550:AP550"/>
-    <mergeCell ref="AK553:AP553"/>
-    <mergeCell ref="A558:M558"/>
-    <mergeCell ref="A559:M559"/>
-    <mergeCell ref="N558:AD558"/>
-    <mergeCell ref="N559:AD559"/>
-    <mergeCell ref="A556:M556"/>
-    <mergeCell ref="A557:M557"/>
-    <mergeCell ref="N556:AD556"/>
-    <mergeCell ref="N557:AD557"/>
-    <mergeCell ref="A554:M554"/>
-    <mergeCell ref="A555:M555"/>
-    <mergeCell ref="N554:AD554"/>
-    <mergeCell ref="N555:AD555"/>
-    <mergeCell ref="A552:M552"/>
-    <mergeCell ref="A553:M553"/>
-    <mergeCell ref="N552:AD552"/>
-    <mergeCell ref="N553:AD553"/>
-    <mergeCell ref="A550:M550"/>
-    <mergeCell ref="A551:M551"/>
-    <mergeCell ref="N550:AD550"/>
-    <mergeCell ref="N551:AD551"/>
-    <mergeCell ref="A548:M548"/>
-    <mergeCell ref="A549:M549"/>
-    <mergeCell ref="N548:AD548"/>
-    <mergeCell ref="A564:M564"/>
-    <mergeCell ref="A565:M565"/>
-    <mergeCell ref="N564:AD564"/>
-    <mergeCell ref="N565:AD565"/>
-    <mergeCell ref="A562:M562"/>
-    <mergeCell ref="A563:M563"/>
-    <mergeCell ref="N562:AD562"/>
-    <mergeCell ref="N563:AD563"/>
-    <mergeCell ref="A560:M560"/>
-    <mergeCell ref="A561:M561"/>
-    <mergeCell ref="N560:AD560"/>
-    <mergeCell ref="N561:AD561"/>
-    <mergeCell ref="AE560:AJ560"/>
-    <mergeCell ref="AK560:AP560"/>
-    <mergeCell ref="AE561:AJ561"/>
-    <mergeCell ref="AK561:AP561"/>
-    <mergeCell ref="AE562:AJ562"/>
-    <mergeCell ref="AE565:AJ565"/>
-    <mergeCell ref="AK565:AP565"/>
-    <mergeCell ref="A570:M570"/>
-    <mergeCell ref="A571:M571"/>
-    <mergeCell ref="N570:AD570"/>
-    <mergeCell ref="N571:AD571"/>
-    <mergeCell ref="A568:M568"/>
-    <mergeCell ref="A569:M569"/>
-    <mergeCell ref="N568:AD568"/>
-    <mergeCell ref="N569:AD569"/>
-    <mergeCell ref="A566:M566"/>
-    <mergeCell ref="A567:M567"/>
-    <mergeCell ref="N566:AD566"/>
-    <mergeCell ref="N567:AD567"/>
-    <mergeCell ref="AE569:AJ569"/>
-    <mergeCell ref="AK569:AP569"/>
-    <mergeCell ref="AE570:AJ570"/>
-    <mergeCell ref="AK570:AP570"/>
-    <mergeCell ref="AE571:AJ571"/>
-    <mergeCell ref="AE566:AJ566"/>
-    <mergeCell ref="AK566:AP566"/>
-    <mergeCell ref="AE567:AJ567"/>
-    <mergeCell ref="AK567:AP567"/>
-    <mergeCell ref="AE568:AJ568"/>
-    <mergeCell ref="AK568:AP568"/>
-    <mergeCell ref="AK571:AP571"/>
-    <mergeCell ref="A574:M574"/>
-    <mergeCell ref="A575:M575"/>
-    <mergeCell ref="N574:AD574"/>
-    <mergeCell ref="N575:AD575"/>
-    <mergeCell ref="A572:M572"/>
-    <mergeCell ref="A573:M573"/>
-    <mergeCell ref="N572:AD572"/>
-    <mergeCell ref="N573:AD573"/>
-    <mergeCell ref="A582:M582"/>
-    <mergeCell ref="A583:M583"/>
-    <mergeCell ref="N582:AD582"/>
-    <mergeCell ref="N583:AD583"/>
-    <mergeCell ref="A580:M580"/>
-    <mergeCell ref="A581:M581"/>
-    <mergeCell ref="N580:AD580"/>
-    <mergeCell ref="N581:AD581"/>
-    <mergeCell ref="A578:M578"/>
-    <mergeCell ref="A579:M579"/>
-    <mergeCell ref="N578:AD578"/>
-    <mergeCell ref="N579:AD579"/>
-    <mergeCell ref="A588:M588"/>
-    <mergeCell ref="A589:M589"/>
-    <mergeCell ref="N588:AD588"/>
-    <mergeCell ref="N589:AD589"/>
-    <mergeCell ref="A586:M586"/>
-    <mergeCell ref="A587:M587"/>
-    <mergeCell ref="N586:AD586"/>
-    <mergeCell ref="N587:AD587"/>
-    <mergeCell ref="A584:M584"/>
-    <mergeCell ref="A585:M585"/>
-    <mergeCell ref="N584:AD584"/>
-    <mergeCell ref="N585:AD585"/>
-    <mergeCell ref="AE587:AJ587"/>
-    <mergeCell ref="AK587:AP587"/>
-    <mergeCell ref="AE588:AJ588"/>
-    <mergeCell ref="AK588:AP588"/>
-    <mergeCell ref="AE589:AJ589"/>
-    <mergeCell ref="N594:AD594"/>
-    <mergeCell ref="N595:AD595"/>
-    <mergeCell ref="A592:M592"/>
-    <mergeCell ref="A593:M593"/>
-    <mergeCell ref="N592:AD592"/>
-    <mergeCell ref="N593:AD593"/>
-    <mergeCell ref="A590:M590"/>
-    <mergeCell ref="A591:M591"/>
-    <mergeCell ref="N590:AD590"/>
-    <mergeCell ref="N591:AD591"/>
-    <mergeCell ref="N600:AD600"/>
-    <mergeCell ref="A600:M600"/>
-    <mergeCell ref="N14:AD14"/>
-    <mergeCell ref="N15:AD15"/>
-    <mergeCell ref="N16:AD16"/>
-    <mergeCell ref="N17:AD17"/>
-    <mergeCell ref="N18:AD18"/>
-    <mergeCell ref="N19:AD19"/>
-    <mergeCell ref="A598:M598"/>
-    <mergeCell ref="A599:M599"/>
-    <mergeCell ref="N598:AD598"/>
-    <mergeCell ref="N599:AD599"/>
-    <mergeCell ref="A596:M596"/>
-    <mergeCell ref="A597:M597"/>
-    <mergeCell ref="N596:AD596"/>
-    <mergeCell ref="N597:AD597"/>
-    <mergeCell ref="A594:M594"/>
-    <mergeCell ref="A595:M595"/>
-    <mergeCell ref="A576:M576"/>
-    <mergeCell ref="A577:M577"/>
-    <mergeCell ref="N576:AD576"/>
-    <mergeCell ref="N577:AD577"/>
+    <mergeCell ref="AE596:AJ596"/>
+    <mergeCell ref="AK596:AP596"/>
+    <mergeCell ref="AE597:AJ597"/>
+    <mergeCell ref="AK597:AP597"/>
+    <mergeCell ref="AE598:AJ598"/>
+    <mergeCell ref="AK598:AP598"/>
+    <mergeCell ref="AE599:AJ599"/>
+    <mergeCell ref="AK599:AP599"/>
+    <mergeCell ref="AE600:AJ600"/>
+    <mergeCell ref="AK600:AP600"/>
+    <mergeCell ref="AK589:AP589"/>
+    <mergeCell ref="AE590:AJ590"/>
+    <mergeCell ref="AK590:AP590"/>
+    <mergeCell ref="AE591:AJ591"/>
+    <mergeCell ref="AK591:AP591"/>
+    <mergeCell ref="AE592:AJ592"/>
+    <mergeCell ref="AK592:AP592"/>
+    <mergeCell ref="AE593:AJ593"/>
+    <mergeCell ref="AK593:AP593"/>
+    <mergeCell ref="AE594:AJ594"/>
+    <mergeCell ref="AK594:AP594"/>
   </mergeCells>
   <conditionalFormatting sqref="A14:AP600">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>